<commit_message>
Code organization - help added
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="13530" windowHeight="6225" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="13530" windowHeight="6015" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="5" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Preferences" sheetId="6" r:id="rId3"/>
     <sheet name="SummarizedInformation" sheetId="1" r:id="rId4"/>
     <sheet name="Relations" sheetId="9" r:id="rId5"/>
+    <sheet name="Help" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="240">
   <si>
     <t>Type</t>
   </si>
@@ -650,9 +651,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t>A04MQ|\source.label|\part.label|\prod.label|\animage.label</t>
-  </si>
-  <si>
     <t>Settings</t>
   </si>
   <si>
@@ -720,6 +718,27 @@
   </si>
   <si>
     <t>RELATION{Report, country.code}</t>
+  </si>
+  <si>
+    <t>htmlFilename</t>
+  </si>
+  <si>
+    <t>tableName</t>
+  </si>
+  <si>
+    <t>startupHelp.html</t>
+  </si>
+  <si>
+    <t>aggregated_level.html</t>
+  </si>
+  <si>
+    <t>main.html</t>
+  </si>
+  <si>
+    <t>naturalKey</t>
+  </si>
+  <si>
+    <t>A04MQ|\source.code|\part.code|\prod.code|\animage.code</t>
   </si>
 </sst>
 </file>
@@ -861,158 +880,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="68">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
+          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -1566,6 +1439,175 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1650,103 +1692,107 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:P6" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
-  <autoFilter ref="A1:P6"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="id" dataDxfId="62"/>
-    <tableColumn id="2" name="code" dataDxfId="61"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="60"/>
-    <tableColumn id="4" name="label" dataDxfId="59"/>
-    <tableColumn id="5" name="tip" dataDxfId="58"/>
-    <tableColumn id="6" name="type" dataDxfId="57"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="56"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="55"/>
-    <tableColumn id="9" name="editable" dataDxfId="54"/>
-    <tableColumn id="10" name="visible" dataDxfId="53"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="52"/>
-    <tableColumn id="12" name="picklistFilter" dataDxfId="51"/>
-    <tableColumn id="13" name="defaultCode" dataDxfId="50"/>
-    <tableColumn id="14" name="defaultValue" dataDxfId="49"/>
-    <tableColumn id="15" name="putInOutput" dataDxfId="48"/>
-    <tableColumn id="16" name="order" dataDxfId="47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q6" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+  <autoFilter ref="A1:Q6"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="id" dataDxfId="65"/>
+    <tableColumn id="2" name="code" dataDxfId="64"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="63"/>
+    <tableColumn id="4" name="label" dataDxfId="62"/>
+    <tableColumn id="5" name="tip" dataDxfId="61"/>
+    <tableColumn id="6" name="type" dataDxfId="60"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="59"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="58"/>
+    <tableColumn id="9" name="editable" dataDxfId="57"/>
+    <tableColumn id="10" name="visible" dataDxfId="56"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="55"/>
+    <tableColumn id="12" name="picklistFilter" dataDxfId="54"/>
+    <tableColumn id="13" name="defaultCode" dataDxfId="53"/>
+    <tableColumn id="14" name="defaultValue" dataDxfId="52"/>
+    <tableColumn id="15" name="putInOutput" dataDxfId="51"/>
+    <tableColumn id="16" name="order" dataDxfId="50"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:P4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:P4"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="id" dataDxfId="17"/>
-    <tableColumn id="2" name="code" dataDxfId="16"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="15"/>
-    <tableColumn id="4" name="label" dataDxfId="14"/>
-    <tableColumn id="5" name="tip" dataDxfId="13"/>
-    <tableColumn id="6" name="type" dataDxfId="12"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="11"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="10"/>
-    <tableColumn id="9" name="editable" dataDxfId="9"/>
-    <tableColumn id="10" name="visible" dataDxfId="8"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="7"/>
-    <tableColumn id="12" name="picklistFilter" dataDxfId="6"/>
-    <tableColumn id="13" name="defaultCode" dataDxfId="5"/>
-    <tableColumn id="14" name="defaultValue" dataDxfId="4"/>
-    <tableColumn id="15" name="putInOutput" dataDxfId="3"/>
-    <tableColumn id="16" name="order" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:Q4" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:Q4"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="id" dataDxfId="46"/>
+    <tableColumn id="2" name="code" dataDxfId="45"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="44"/>
+    <tableColumn id="4" name="label" dataDxfId="43"/>
+    <tableColumn id="5" name="tip" dataDxfId="42"/>
+    <tableColumn id="6" name="type" dataDxfId="41"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="40"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="39"/>
+    <tableColumn id="9" name="editable" dataDxfId="38"/>
+    <tableColumn id="10" name="visible" dataDxfId="37"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="36"/>
+    <tableColumn id="12" name="picklistFilter" dataDxfId="35"/>
+    <tableColumn id="13" name="defaultCode" dataDxfId="34"/>
+    <tableColumn id="14" name="defaultValue" dataDxfId="33"/>
+    <tableColumn id="15" name="putInOutput" dataDxfId="32"/>
+    <tableColumn id="16" name="order" dataDxfId="31"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:P8" totalsRowShown="0" headerRowDxfId="46">
-  <autoFilter ref="A1:P8"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="id" dataDxfId="45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:Q8" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="A1:Q8"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="id" dataDxfId="28"/>
     <tableColumn id="2" name="code"/>
     <tableColumn id="3" name="xmlTag"/>
-    <tableColumn id="4" name="label" dataDxfId="44"/>
-    <tableColumn id="5" name="tip" dataDxfId="43"/>
-    <tableColumn id="6" name="type" dataDxfId="42"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="41"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="40"/>
-    <tableColumn id="9" name="editable" dataDxfId="39"/>
-    <tableColumn id="10" name="visible" dataDxfId="38"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="37"/>
-    <tableColumn id="17" name="picklistFilter" dataDxfId="36"/>
+    <tableColumn id="4" name="label" dataDxfId="27"/>
+    <tableColumn id="5" name="tip" dataDxfId="26"/>
+    <tableColumn id="6" name="type" dataDxfId="25"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="24"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="23"/>
+    <tableColumn id="9" name="editable" dataDxfId="22"/>
+    <tableColumn id="10" name="visible" dataDxfId="21"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="20"/>
+    <tableColumn id="17" name="picklistFilter" dataDxfId="19"/>
     <tableColumn id="12" name="defaultCode"/>
     <tableColumn id="13" name="defaultValue"/>
     <tableColumn id="14" name="putInOutput"/>
     <tableColumn id="15" name="order"/>
+    <tableColumn id="16" name="naturalKey"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P36" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:P36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q36" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:Q36"/>
   <sortState ref="A2:P33">
     <sortCondition ref="P1:P33"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="1" name="id" dataDxfId="33"/>
-    <tableColumn id="2" name="code" dataDxfId="32"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="31"/>
-    <tableColumn id="4" name="label" dataDxfId="30"/>
-    <tableColumn id="5" name="tip" dataDxfId="29"/>
-    <tableColumn id="6" name="type" dataDxfId="28"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="27"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="26"/>
-    <tableColumn id="9" name="editable" dataDxfId="25"/>
-    <tableColumn id="10" name="visible" dataDxfId="24"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="23"/>
-    <tableColumn id="16" name="picklistFilter" dataDxfId="22"/>
-    <tableColumn id="12" name="defaultCode" dataDxfId="21"/>
-    <tableColumn id="13" name="defaultValue" dataDxfId="20"/>
-    <tableColumn id="14" name="putInOutput" dataDxfId="19"/>
-    <tableColumn id="15" name="order" dataDxfId="18"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="id" dataDxfId="16"/>
+    <tableColumn id="2" name="code" dataDxfId="15"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="14"/>
+    <tableColumn id="4" name="label" dataDxfId="13"/>
+    <tableColumn id="5" name="tip" dataDxfId="12"/>
+    <tableColumn id="6" name="type" dataDxfId="11"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="10"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="9"/>
+    <tableColumn id="9" name="editable" dataDxfId="8"/>
+    <tableColumn id="10" name="visible" dataDxfId="7"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="6"/>
+    <tableColumn id="16" name="picklistFilter" dataDxfId="5"/>
+    <tableColumn id="12" name="defaultCode" dataDxfId="4"/>
+    <tableColumn id="13" name="defaultValue" dataDxfId="3"/>
+    <tableColumn id="14" name="putInOutput" dataDxfId="2"/>
+    <tableColumn id="15" name="order" dataDxfId="1"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1758,6 +1804,17 @@
   <tableColumns count="2">
     <tableColumn id="1" name="parentTable"/>
     <tableColumn id="2" name="childTable"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="tableName"/>
+    <tableColumn id="2" name="htmlFilename"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2050,13 +2107,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,7 +2135,7 @@
     <col min="15" max="15" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -2127,8 +2184,11 @@
       <c r="P1" s="12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>200</v>
       </c>
@@ -2171,8 +2231,11 @@
       <c r="P2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>201</v>
       </c>
@@ -2215,13 +2278,16 @@
       <c r="P3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2241,17 +2307,18 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>132</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
@@ -2280,19 +2347,22 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O5" s="16"/>
       <c r="P5" s="16">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>207</v>
@@ -2315,13 +2385,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2412,7 @@
     <col min="15" max="15" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -2391,8 +2461,11 @@
       <c r="P1" s="12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>154</v>
       </c>
@@ -2429,8 +2502,9 @@
       <c r="P2" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="12"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>155</v>
       </c>
@@ -2467,20 +2541,21 @@
       <c r="P3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>208</v>
@@ -2505,6 +2580,7 @@
       <c r="P4" s="16">
         <v>3</v>
       </c>
+      <c r="Q4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2517,13 +2593,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,7 +2619,7 @@
     <col min="15" max="15" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
@@ -2592,8 +2668,11 @@
       <c r="P1" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>132</v>
       </c>
@@ -2629,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>135</v>
       </c>
@@ -2668,7 +2747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>138</v>
       </c>
@@ -2707,7 +2786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>141</v>
       </c>
@@ -2746,7 +2825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>144</v>
       </c>
@@ -2785,7 +2864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>147</v>
       </c>
@@ -2824,7 +2903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>150</v>
       </c>
@@ -2873,13 +2952,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2899,10 +2978,11 @@
     <col min="13" max="13" width="50.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="80.7109375" style="12" customWidth="1"/>
     <col min="15" max="15" width="20" style="12" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="12"/>
+    <col min="16" max="16" width="9.7109375" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -2951,8 +3031,11 @@
       <c r="P1" s="12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>67</v>
       </c>
@@ -2992,8 +3075,11 @@
       <c r="P2" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>71</v>
       </c>
@@ -3039,8 +3125,11 @@
       <c r="P3" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>75</v>
       </c>
@@ -3086,8 +3175,11 @@
       <c r="P4" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>79</v>
       </c>
@@ -3127,8 +3219,11 @@
       <c r="P5" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
@@ -3168,8 +3263,11 @@
       <c r="P6" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
@@ -3212,8 +3310,11 @@
       <c r="P7" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>102</v>
       </c>
@@ -3251,10 +3352,10 @@
         <v>180</v>
       </c>
       <c r="M8" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="N8" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>218</v>
       </c>
       <c r="O8" s="12" t="s">
         <v>11</v>
@@ -3262,8 +3363,11 @@
       <c r="P8" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
@@ -3301,7 +3405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>29</v>
       </c>
@@ -3339,7 +3443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>32</v>
       </c>
@@ -3377,7 +3481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
@@ -3415,7 +3519,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
@@ -3453,7 +3557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
@@ -3485,7 +3589,7 @@
         <v>3</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O14" s="12" t="s">
         <v>11</v>
@@ -3494,7 +3598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>107</v>
       </c>
@@ -3532,7 +3636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>13</v>
       </c>
@@ -3689,10 +3793,10 @@
         <v>4</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O20" s="12" t="s">
         <v>11</v>
@@ -3724,10 +3828,10 @@
         <v>4</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>11</v>
@@ -3759,10 +3863,10 @@
         <v>4</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O22" s="12" t="s">
         <v>11</v>
@@ -3794,7 +3898,7 @@
         <v>4</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O23" s="12" t="s">
         <v>11</v>
@@ -3826,10 +3930,10 @@
         <v>4</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O24" s="12" t="s">
         <v>11</v>
@@ -3896,7 +4000,7 @@
         <v>4</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="O26" s="12" t="s">
         <v>11</v>
@@ -3960,7 +4064,7 @@
         <v>4</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O28" s="12" t="s">
         <v>11</v>
@@ -4154,7 +4258,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>207</v>
@@ -4171,7 +4275,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>207</v>
@@ -4199,7 +4303,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4226,7 +4330,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
         <v>205</v>
@@ -4234,7 +4338,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
         <v>205</v>
@@ -4242,10 +4346,71 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
         <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unifomed packages to custom uses added. Added columns codeFormula and labelFormula in the xlsx schema.
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="242">
   <si>
     <t>Type</t>
   </si>
@@ -739,6 +739,12 @@
   </si>
   <si>
     <t>A04MQ|\source.code|\part.code|\prod.code|\animage.code</t>
+  </si>
+  <si>
+    <t>codeFormula</t>
+  </si>
+  <si>
+    <t>labelFormula</t>
   </si>
 </sst>
 </file>
@@ -880,7 +886,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="72">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1692,75 +1732,81 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q6" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
-  <autoFilter ref="A1:Q6"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="id" dataDxfId="65"/>
-    <tableColumn id="2" name="code" dataDxfId="64"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="63"/>
-    <tableColumn id="4" name="label" dataDxfId="62"/>
-    <tableColumn id="5" name="tip" dataDxfId="61"/>
-    <tableColumn id="6" name="type" dataDxfId="60"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="59"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="58"/>
-    <tableColumn id="9" name="editable" dataDxfId="57"/>
-    <tableColumn id="10" name="visible" dataDxfId="56"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="55"/>
-    <tableColumn id="12" name="picklistFilter" dataDxfId="54"/>
-    <tableColumn id="13" name="defaultCode" dataDxfId="53"/>
-    <tableColumn id="14" name="defaultValue" dataDxfId="52"/>
-    <tableColumn id="15" name="putInOutput" dataDxfId="51"/>
-    <tableColumn id="16" name="order" dataDxfId="50"/>
-    <tableColumn id="17" name="naturalKey" dataDxfId="49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S6" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="A1:S6"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="id" dataDxfId="69"/>
+    <tableColumn id="2" name="code" dataDxfId="68"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="67"/>
+    <tableColumn id="4" name="label" dataDxfId="66"/>
+    <tableColumn id="5" name="tip" dataDxfId="65"/>
+    <tableColumn id="6" name="type" dataDxfId="64"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="63"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="62"/>
+    <tableColumn id="9" name="editable" dataDxfId="61"/>
+    <tableColumn id="10" name="visible" dataDxfId="60"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="59"/>
+    <tableColumn id="12" name="picklistFilter" dataDxfId="58"/>
+    <tableColumn id="13" name="defaultCode" dataDxfId="57"/>
+    <tableColumn id="18" name="codeFormula"/>
+    <tableColumn id="14" name="defaultValue" dataDxfId="56"/>
+    <tableColumn id="19" name="labelFormula"/>
+    <tableColumn id="15" name="putInOutput" dataDxfId="55"/>
+    <tableColumn id="16" name="order" dataDxfId="54"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:Q4" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A1:Q4"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="id" dataDxfId="46"/>
-    <tableColumn id="2" name="code" dataDxfId="45"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="44"/>
-    <tableColumn id="4" name="label" dataDxfId="43"/>
-    <tableColumn id="5" name="tip" dataDxfId="42"/>
-    <tableColumn id="6" name="type" dataDxfId="41"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="40"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="39"/>
-    <tableColumn id="9" name="editable" dataDxfId="38"/>
-    <tableColumn id="10" name="visible" dataDxfId="37"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="36"/>
-    <tableColumn id="12" name="picklistFilter" dataDxfId="35"/>
-    <tableColumn id="13" name="defaultCode" dataDxfId="34"/>
-    <tableColumn id="14" name="defaultValue" dataDxfId="33"/>
-    <tableColumn id="15" name="putInOutput" dataDxfId="32"/>
-    <tableColumn id="16" name="order" dataDxfId="31"/>
-    <tableColumn id="17" name="naturalKey" dataDxfId="30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:S4" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+  <autoFilter ref="A1:S4"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="id" dataDxfId="50"/>
+    <tableColumn id="2" name="code" dataDxfId="49"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="48"/>
+    <tableColumn id="4" name="label" dataDxfId="47"/>
+    <tableColumn id="5" name="tip" dataDxfId="46"/>
+    <tableColumn id="6" name="type" dataDxfId="45"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="44"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="43"/>
+    <tableColumn id="9" name="editable" dataDxfId="42"/>
+    <tableColumn id="10" name="visible" dataDxfId="41"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="40"/>
+    <tableColumn id="12" name="picklistFilter" dataDxfId="39"/>
+    <tableColumn id="13" name="defaultCode" dataDxfId="38"/>
+    <tableColumn id="18" name="codeFormula" dataDxfId="1"/>
+    <tableColumn id="14" name="defaultValue" dataDxfId="37"/>
+    <tableColumn id="19" name="labelFormula" dataDxfId="0"/>
+    <tableColumn id="15" name="putInOutput" dataDxfId="36"/>
+    <tableColumn id="16" name="order" dataDxfId="35"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:Q8" totalsRowShown="0" headerRowDxfId="29">
-  <autoFilter ref="A1:Q8"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="id" dataDxfId="28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:S8" totalsRowShown="0" headerRowDxfId="33">
+  <autoFilter ref="A1:S8"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="id" dataDxfId="32"/>
     <tableColumn id="2" name="code"/>
     <tableColumn id="3" name="xmlTag"/>
-    <tableColumn id="4" name="label" dataDxfId="27"/>
-    <tableColumn id="5" name="tip" dataDxfId="26"/>
-    <tableColumn id="6" name="type" dataDxfId="25"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="24"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="23"/>
-    <tableColumn id="9" name="editable" dataDxfId="22"/>
-    <tableColumn id="10" name="visible" dataDxfId="21"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="20"/>
-    <tableColumn id="17" name="picklistFilter" dataDxfId="19"/>
+    <tableColumn id="4" name="label" dataDxfId="31"/>
+    <tableColumn id="5" name="tip" dataDxfId="30"/>
+    <tableColumn id="6" name="type" dataDxfId="29"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="28"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="27"/>
+    <tableColumn id="9" name="editable" dataDxfId="26"/>
+    <tableColumn id="10" name="visible" dataDxfId="25"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="24"/>
+    <tableColumn id="17" name="picklistFilter" dataDxfId="23"/>
     <tableColumn id="12" name="defaultCode"/>
+    <tableColumn id="18" name="codeFormula"/>
     <tableColumn id="13" name="defaultValue"/>
+    <tableColumn id="19" name="labelFormula"/>
     <tableColumn id="14" name="putInOutput"/>
     <tableColumn id="15" name="order"/>
     <tableColumn id="16" name="naturalKey"/>
@@ -1770,29 +1816,31 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q36" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:Q36"/>
-  <sortState ref="A2:P33">
-    <sortCondition ref="P1:P33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S36" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:S36"/>
+  <sortState ref="A2:R33">
+    <sortCondition ref="R1:R33"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="1" name="id" dataDxfId="16"/>
-    <tableColumn id="2" name="code" dataDxfId="15"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="14"/>
-    <tableColumn id="4" name="label" dataDxfId="13"/>
-    <tableColumn id="5" name="tip" dataDxfId="12"/>
-    <tableColumn id="6" name="type" dataDxfId="11"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="10"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="9"/>
-    <tableColumn id="9" name="editable" dataDxfId="8"/>
-    <tableColumn id="10" name="visible" dataDxfId="7"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="6"/>
-    <tableColumn id="16" name="picklistFilter" dataDxfId="5"/>
-    <tableColumn id="12" name="defaultCode" dataDxfId="4"/>
-    <tableColumn id="13" name="defaultValue" dataDxfId="3"/>
-    <tableColumn id="14" name="putInOutput" dataDxfId="2"/>
-    <tableColumn id="15" name="order" dataDxfId="1"/>
-    <tableColumn id="17" name="naturalKey" dataDxfId="0"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="id" dataDxfId="20"/>
+    <tableColumn id="2" name="code" dataDxfId="19"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="18"/>
+    <tableColumn id="4" name="label" dataDxfId="17"/>
+    <tableColumn id="5" name="tip" dataDxfId="16"/>
+    <tableColumn id="6" name="type" dataDxfId="15"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="14"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="13"/>
+    <tableColumn id="9" name="editable" dataDxfId="12"/>
+    <tableColumn id="10" name="visible" dataDxfId="11"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="10"/>
+    <tableColumn id="16" name="picklistFilter" dataDxfId="9"/>
+    <tableColumn id="12" name="defaultCode" dataDxfId="8"/>
+    <tableColumn id="18" name="codeFormula" dataDxfId="3"/>
+    <tableColumn id="13" name="defaultValue" dataDxfId="7"/>
+    <tableColumn id="19" name="labelFormula" dataDxfId="2"/>
+    <tableColumn id="14" name="putInOutput" dataDxfId="6"/>
+    <tableColumn id="15" name="order" dataDxfId="5"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2107,13 +2155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,12 +2178,14 @@
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" customWidth="1"/>
-    <col min="14" max="14" width="22" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" customWidth="1"/>
+    <col min="14" max="14" width="38.85546875" customWidth="1"/>
+    <col min="15" max="15" width="35.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -2176,19 +2226,25 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>200</v>
       </c>
@@ -2224,18 +2280,20 @@
       <c r="M2" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2">
+      <c r="P2" s="11"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2">
         <v>1</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>201</v>
       </c>
@@ -2271,18 +2329,20 @@
       <c r="M3" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2">
+      <c r="P3" s="11"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2">
         <v>2</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>228</v>
       </c>
@@ -2306,14 +2366,16 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>132</v>
       </c>
@@ -2346,21 +2408,23 @@
         <v>175</v>
       </c>
       <c r="L5" s="11"/>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="16"/>
+      <c r="N5" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="O5" s="16"/>
+      <c r="P5" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16">
+        <v>3</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>212</v>
       </c>
@@ -2385,13 +2449,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2407,12 +2471,12 @@
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="12" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -2453,19 +2517,25 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>154</v>
       </c>
@@ -2499,12 +2569,14 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="12">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="12">
         <v>1</v>
       </c>
-      <c r="Q2" s="12"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S2" s="12"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>155</v>
       </c>
@@ -2538,12 +2610,14 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2">
         <v>2</v>
       </c>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>224</v>
       </c>
@@ -2577,10 +2651,12 @@
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="16">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="2"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16">
+        <v>3</v>
+      </c>
+      <c r="S4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2593,13 +2669,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,12 +2690,12 @@
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="13" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
@@ -2660,19 +2736,25 @@
         <v>128</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>132</v>
       </c>
@@ -2704,11 +2786,11 @@
         <v>175</v>
       </c>
       <c r="L2" s="9"/>
-      <c r="P2">
+      <c r="R2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>135</v>
       </c>
@@ -2743,11 +2825,11 @@
       <c r="L3" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>138</v>
       </c>
@@ -2782,11 +2864,11 @@
       <c r="L4" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="P4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>141</v>
       </c>
@@ -2821,11 +2903,11 @@
       <c r="L5" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="P5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>144</v>
       </c>
@@ -2860,11 +2942,11 @@
       <c r="L6" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>147</v>
       </c>
@@ -2899,11 +2981,11 @@
       <c r="L7" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>150</v>
       </c>
@@ -2938,7 +3020,7 @@
       <c r="L8" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>7</v>
       </c>
     </row>
@@ -2952,13 +3034,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,14 +3057,14 @@
     <col min="10" max="10" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="50.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="80.7109375" style="12" customWidth="1"/>
-    <col min="15" max="15" width="20" style="12" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="50.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" style="12" customWidth="1"/>
+    <col min="16" max="16" width="76.28515625" style="12" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -3023,19 +3105,25 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>67</v>
       </c>
@@ -3069,17 +3157,17 @@
       <c r="L2" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="12">
+      <c r="R2" s="12">
         <v>1</v>
       </c>
-      <c r="Q2" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S2" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>71</v>
       </c>
@@ -3116,20 +3204,20 @@
       <c r="M3" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="12">
+      <c r="R3" s="12">
         <v>2</v>
       </c>
-      <c r="Q3" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>75</v>
       </c>
@@ -3166,20 +3254,20 @@
       <c r="M4" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="Q4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="12">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="12">
+        <v>3</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>79</v>
       </c>
@@ -3213,17 +3301,17 @@
       <c r="L5" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="12">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="12">
+        <v>4</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
@@ -3257,17 +3345,17 @@
       <c r="L6" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="Q6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="12">
+      <c r="R6" s="12">
         <v>5</v>
       </c>
-      <c r="Q6" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S6" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
@@ -3304,17 +3392,17 @@
       <c r="L7" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="P7" s="12">
+      <c r="R7" s="12">
         <v>6</v>
       </c>
-      <c r="Q7" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S7" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>102</v>
       </c>
@@ -3340,7 +3428,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
@@ -3354,20 +3442,17 @@
       <c r="M8" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="O8" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="O8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="P8" s="12">
+      <c r="Q8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R8" s="12">
         <v>7</v>
       </c>
-      <c r="Q8" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
@@ -3395,17 +3480,17 @@
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N9" s="12">
+      <c r="O9" s="12">
         <v>0</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="Q9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P9" s="12">
+      <c r="R9" s="12">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>29</v>
       </c>
@@ -3433,17 +3518,17 @@
       <c r="J10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="12">
+      <c r="O10" s="12">
         <v>0</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="Q10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="12">
+      <c r="R10" s="12">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>32</v>
       </c>
@@ -3471,17 +3556,17 @@
       <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="12">
+      <c r="O11" s="12">
         <v>0</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="Q11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P11" s="12">
+      <c r="R11" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
@@ -3509,17 +3594,17 @@
       <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="P12" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P12" s="12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
@@ -3547,17 +3632,17 @@
       <c r="J13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N13" s="12">
+      <c r="O13" s="12">
         <v>0</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="Q13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P13" s="12">
+      <c r="R13" s="12">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
@@ -3588,17 +3673,17 @@
       <c r="J14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="P14" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="O14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="P14" s="12">
+      <c r="Q14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R14" s="12">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>107</v>
       </c>
@@ -3626,17 +3711,20 @@
       <c r="K15" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="N15" s="12" t="s">
+      <c r="M15" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="O15" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="O15" s="12" t="s">
+      <c r="Q15" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P15" s="12">
+      <c r="R15" s="12">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>13</v>
       </c>
@@ -3664,14 +3752,14 @@
       <c r="M16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="O16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="O16" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
@@ -3696,14 +3784,14 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N17" s="12" t="s">
+      <c r="P17" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="O17" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>39</v>
       </c>
@@ -3728,14 +3816,14 @@
       <c r="J18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N18" s="12" t="s">
+      <c r="P18" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="O18" s="12" t="s">
+      <c r="Q18" s="12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>46</v>
       </c>
@@ -3760,14 +3848,14 @@
       <c r="J19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N19" s="12" t="s">
+      <c r="P19" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="O19" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
@@ -3792,17 +3880,17 @@
       <c r="J20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="N20" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="N20" s="12" t="s">
+      <c r="P20" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="O20" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>51</v>
       </c>
@@ -3827,17 +3915,17 @@
       <c r="J21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="N21" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="N21" s="12" t="s">
+      <c r="P21" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="O21" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>53</v>
       </c>
@@ -3862,17 +3950,17 @@
       <c r="J22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="N22" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="N22" s="12" t="s">
+      <c r="P22" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="O22" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>55</v>
       </c>
@@ -3897,14 +3985,14 @@
       <c r="J23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N23" s="12" t="s">
+      <c r="P23" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="O23" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>58</v>
       </c>
@@ -3929,17 +4017,17 @@
       <c r="J24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="12" t="s">
+      <c r="N24" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="N24" s="12" t="s">
+      <c r="P24" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="O24" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>61</v>
       </c>
@@ -3967,14 +4055,14 @@
       <c r="M25" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="N25" s="12" t="s">
+      <c r="O25" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="O25" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>65</v>
       </c>
@@ -3999,14 +4087,14 @@
       <c r="J26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N26" s="12" t="s">
+      <c r="P26" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="O26" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>84</v>
       </c>
@@ -4031,14 +4119,14 @@
       <c r="J27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="12" t="s">
+      <c r="P27" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="O27" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>86</v>
       </c>
@@ -4063,14 +4151,14 @@
       <c r="J28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N28" s="12" t="s">
+      <c r="P28" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="O28" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -4098,14 +4186,14 @@
       <c r="M29" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="N29" s="12" t="s">
+      <c r="O29" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>92</v>
       </c>
@@ -4133,14 +4221,14 @@
       <c r="M30" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="N30" s="12" t="s">
+      <c r="O30" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="O30" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>96</v>
       </c>
@@ -4165,14 +4253,14 @@
       <c r="J31" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N31" s="12" t="s">
+      <c r="P31" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="O31" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>98</v>
       </c>
@@ -4200,14 +4288,14 @@
       <c r="M32" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N32" s="12" t="s">
+      <c r="O32" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="O32" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>106</v>
       </c>
@@ -4232,14 +4320,14 @@
       <c r="J33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N33" s="12" t="s">
+      <c r="P33" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="O33" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>206</v>
       </c>
@@ -4252,11 +4340,11 @@
       <c r="J34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O34" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>212</v>
       </c>
@@ -4269,11 +4357,11 @@
       <c r="J35" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O35" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>213</v>
       </c>
@@ -4286,7 +4374,7 @@
       <c r="J36" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O36" s="12" t="s">
+      <c r="Q36" s="12" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
analytical results added, dataset xml creator added
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -12,15 +12,16 @@
     <sheet name="Preferences" sheetId="6" r:id="rId3"/>
     <sheet name="SummarizedInformation" sheetId="1" r:id="rId4"/>
     <sheet name="CasesInformation" sheetId="11" r:id="rId5"/>
-    <sheet name="Relations" sheetId="9" r:id="rId6"/>
-    <sheet name="Help" sheetId="10" r:id="rId7"/>
+    <sheet name="AnalyticalResults" sheetId="12" r:id="rId6"/>
+    <sheet name="Relations" sheetId="9" r:id="rId7"/>
+    <sheet name="Help" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="304">
   <si>
     <t>Type</t>
   </si>
@@ -664,193 +665,274 @@
     <t>SettingsId</t>
   </si>
   <si>
+    <t>RELATION{Preferences, country.code}</t>
+  </si>
+  <si>
+    <t>RELATION{Preferences, defScreening\type.code.code}</t>
+  </si>
+  <si>
+    <t>RELATION{Preferences, defScreening\type.code.label}</t>
+  </si>
+  <si>
+    <t>RELATION{Report, reportYear.label}</t>
+  </si>
+  <si>
+    <t>RELATION{Report, reportMonth.label}</t>
+  </si>
+  <si>
+    <t>\repYear.label</t>
+  </si>
+  <si>
+    <t>END_TRIM(\repYear.code, 2)|END_TRIM(ZERO_PADDING(\sampM.code,2), 2)|_ZERO_PADDING({rowId},4)</t>
+  </si>
+  <si>
+    <t>RELATION{Report, reportMonth.code}</t>
+  </si>
+  <si>
+    <t>RELATION{Report, reportYear.code}</t>
+  </si>
+  <si>
+    <t>orgCode</t>
+  </si>
+  <si>
+    <t>Organisation code</t>
+  </si>
+  <si>
+    <t>organisationCode</t>
+  </si>
+  <si>
+    <t>The organisation code used for sending reports</t>
+  </si>
+  <si>
+    <t>reportSenderId</t>
+  </si>
+  <si>
+    <t>RELATION{Preferences, country.code}|END_TRIM(\reportYear.code, 2)|END_TRIM(ZERO_PADDING(\reportMonth.code,2), 2)</t>
+  </si>
+  <si>
+    <t>reportCountry</t>
+  </si>
+  <si>
+    <t>RELATION{Report, country.label}</t>
+  </si>
+  <si>
+    <t>RELATION{Report, country.code}</t>
+  </si>
+  <si>
+    <t>htmlFilename</t>
+  </si>
+  <si>
+    <t>tableName</t>
+  </si>
+  <si>
+    <t>startupHelp.html</t>
+  </si>
+  <si>
+    <t>aggregated_level.html</t>
+  </si>
+  <si>
+    <t>main.html</t>
+  </si>
+  <si>
+    <t>naturalKey</t>
+  </si>
+  <si>
+    <t>A04MQ|\source.code|\part.code|\prod.code|\animage.code</t>
+  </si>
+  <si>
+    <t>codeFormula</t>
+  </si>
+  <si>
+    <t>labelFormula</t>
+  </si>
+  <si>
+    <t>tseNationalCaseId</t>
+  </si>
+  <si>
+    <t>N.06</t>
+  </si>
+  <si>
+    <t>National case ID</t>
+  </si>
+  <si>
+    <t>Id univocally assigned to the case at country level</t>
+  </si>
+  <si>
+    <t>tseIndexCase</t>
+  </si>
+  <si>
+    <t>Index case</t>
+  </si>
+  <si>
+    <t>Is it an index case?</t>
+  </si>
+  <si>
+    <t>YESNO</t>
+  </si>
+  <si>
+    <t>indexCaseLists</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>Id univocally assigned to the sample at country level</t>
+  </si>
+  <si>
+    <t>animalId</t>
+  </si>
+  <si>
+    <t>C.05</t>
+  </si>
+  <si>
+    <t>Animal ID</t>
+  </si>
+  <si>
+    <t>Id univocally assigned to the animal at country level</t>
+  </si>
+  <si>
+    <t>herdId</t>
+  </si>
+  <si>
+    <t>Herd ID</t>
+  </si>
+  <si>
+    <t>Id univocally assigned to the flock/herd at country level</t>
+  </si>
+  <si>
+    <t>birthCountry</t>
+  </si>
+  <si>
+    <t>Country of birth</t>
+  </si>
+  <si>
+    <t>Country of birth of the animal</t>
+  </si>
+  <si>
+    <t>sampAnAsses</t>
+  </si>
+  <si>
+    <t>Case assessment</t>
+  </si>
+  <si>
+    <t>Final evaluation of the case after discriminatory testing</t>
+  </si>
+  <si>
+    <t>assessmentLists</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,type.label}</t>
+  </si>
+  <si>
+    <t>sampArea</t>
+  </si>
+  <si>
+    <t>D.04</t>
+  </si>
+  <si>
+    <t>Sampling area</t>
+  </si>
+  <si>
+    <t>Area of sampling</t>
+  </si>
+  <si>
+    <t>NUTS</t>
+  </si>
+  <si>
+    <t>sampAreaLists</t>
+  </si>
+  <si>
+    <t>RELATION{Report,country.code}</t>
+  </si>
+  <si>
+    <t>SummarizedInformationId</t>
+  </si>
+  <si>
+    <t>CasesInformation</t>
+  </si>
+  <si>
     <t>RELATION{Preferences, country.label}</t>
   </si>
   <si>
-    <t>RELATION{Preferences, country.code}</t>
-  </si>
-  <si>
-    <t>RELATION{Preferences, defScreening\type.code.code}</t>
-  </si>
-  <si>
-    <t>RELATION{Preferences, defScreening\type.code.label}</t>
-  </si>
-  <si>
-    <t>RELATION{Report, reportYear.label}</t>
-  </si>
-  <si>
-    <t>RELATION{Report, reportMonth.label}</t>
-  </si>
-  <si>
-    <t>\repYear.label</t>
-  </si>
-  <si>
-    <t>END_TRIM(\repYear.code, 2)|END_TRIM(ZERO_PADDING(\sampM.code,2), 2)|_ZERO_PADDING({rowId},4)</t>
-  </si>
-  <si>
-    <t>RELATION{Report, reportMonth.code}</t>
-  </si>
-  <si>
-    <t>RELATION{Report, reportYear.code}</t>
-  </si>
-  <si>
-    <t>orgCode</t>
-  </si>
-  <si>
-    <t>Organisation code</t>
-  </si>
-  <si>
-    <t>organisationCode</t>
-  </si>
-  <si>
-    <t>The organisation code used for sending reports</t>
-  </si>
-  <si>
-    <t>reportSenderId</t>
-  </si>
-  <si>
-    <t>RELATION{Preferences, country.code}|END_TRIM(\reportYear.code, 2)|END_TRIM(ZERO_PADDING(\reportMonth.code,2), 2)</t>
-  </si>
-  <si>
-    <t>reportCountry</t>
-  </si>
-  <si>
-    <t>RELATION{Report, country.label}</t>
-  </si>
-  <si>
-    <t>RELATION{Report, country.code}</t>
-  </si>
-  <si>
-    <t>htmlFilename</t>
-  </si>
-  <si>
-    <t>tableName</t>
-  </si>
-  <si>
-    <t>startupHelp.html</t>
-  </si>
-  <si>
-    <t>aggregated_level.html</t>
-  </si>
-  <si>
-    <t>main.html</t>
-  </si>
-  <si>
-    <t>naturalKey</t>
-  </si>
-  <si>
-    <t>A04MQ|\source.code|\part.code|\prod.code|\animage.code</t>
-  </si>
-  <si>
-    <t>codeFormula</t>
-  </si>
-  <si>
-    <t>labelFormula</t>
-  </si>
-  <si>
-    <t>tseNationalCaseId</t>
-  </si>
-  <si>
-    <t>N.06</t>
-  </si>
-  <si>
-    <t>National case ID</t>
-  </si>
-  <si>
-    <t>Id univocally assigned to the case at country level</t>
-  </si>
-  <si>
-    <t>tseIndexCase</t>
-  </si>
-  <si>
-    <t>Index case</t>
-  </si>
-  <si>
-    <t>Is it an index case?</t>
-  </si>
-  <si>
-    <t>YESNO</t>
-  </si>
-  <si>
-    <t>indexCaseLists</t>
-  </si>
-  <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
-    <t>Id univocally assigned to the sample at country level</t>
-  </si>
-  <si>
-    <t>animalId</t>
-  </si>
-  <si>
-    <t>C.05</t>
-  </si>
-  <si>
-    <t>Animal ID</t>
-  </si>
-  <si>
-    <t>Id univocally assigned to the animal at country level</t>
-  </si>
-  <si>
-    <t>herdId</t>
-  </si>
-  <si>
-    <t>Herd ID</t>
-  </si>
-  <si>
-    <t>Id univocally assigned to the flock/herd at country level</t>
-  </si>
-  <si>
-    <t>birthCountry</t>
-  </si>
-  <si>
-    <t>Country of birth</t>
-  </si>
-  <si>
-    <t>Country of birth of the animal</t>
-  </si>
-  <si>
-    <t>sampAnAsses</t>
-  </si>
-  <si>
-    <t>Case assessment</t>
-  </si>
-  <si>
-    <t>Final evaluation of the case after discriminatory testing</t>
-  </si>
-  <si>
-    <t>assessmentLists</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,type.label}</t>
-  </si>
-  <si>
-    <t>sampArea</t>
-  </si>
-  <si>
-    <t>D.04</t>
-  </si>
-  <si>
-    <t>Sampling area</t>
-  </si>
-  <si>
-    <t>Area of sampling</t>
-  </si>
-  <si>
-    <t>NUTS</t>
-  </si>
-  <si>
-    <t>sampAreaLists</t>
-  </si>
-  <si>
-    <t>RELATION{Report,country.code}</t>
-  </si>
-  <si>
-    <t>SummarizedInformationId</t>
-  </si>
-  <si>
-    <t>CasesInformation</t>
+    <t>RELATION{SummarizedInformation,progId.label}</t>
+  </si>
+  <si>
+    <t>tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.\animalId.label</t>
+  </si>
+  <si>
+    <t>sampUnitIds</t>
+  </si>
+  <si>
+    <t>animalId=\animalId|IF_NOT_NULL(herdId,$herdId=\herdId.label,)</t>
+  </si>
+  <si>
+    <t>birthCountry=\birthCountry|IF_NOT_NULL(statusHerd,$statusHerd=\statusHerd.label,)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,sampMatCode.label}</t>
+  </si>
+  <si>
+    <t>\sampId.label</t>
+  </si>
+  <si>
+    <t>Year of analysis</t>
+  </si>
+  <si>
+    <t>Year in whcih the samples has been analysed</t>
+  </si>
+  <si>
+    <t>analysisM</t>
+  </si>
+  <si>
+    <t>F.04</t>
+  </si>
+  <si>
+    <t>Month of analysis</t>
+  </si>
+  <si>
+    <t>Month in whcih the samples has been analysed</t>
+  </si>
+  <si>
+    <t>P001A</t>
+  </si>
+  <si>
+    <t>evalInfo</t>
+  </si>
+  <si>
+    <t>tseNationalCaseId=\tseNationalCaseId$tseIndexCase=\tseIndexCase$sampAnAsses=\sampAnAsses</t>
+  </si>
+  <si>
+    <t>CasesInformationId</t>
+  </si>
+  <si>
+    <t>AnalyticalResults</t>
+  </si>
+  <si>
+    <t>directRelation</t>
+  </si>
+  <si>
+    <t>tes</t>
+  </si>
+  <si>
+    <t>RELATION{CasesInformation,tseNationalCaseId.label}</t>
+  </si>
+  <si>
+    <t>RELATION{CasesInformation,tseNationalCaseId.code}</t>
+  </si>
+  <si>
+    <t>RELATION{CasesInformation,sampAnAsses.label}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation, anMethCode.code}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation, anMethCode.label}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation, type.code}</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1074,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="114">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1005,7 +1087,16 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -1024,15 +1115,6 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -1052,6 +1134,185 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2034,77 +2295,77 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S6" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S6" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="A1:S6"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="id" dataDxfId="91"/>
-    <tableColumn id="2" name="code" dataDxfId="90"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="89"/>
-    <tableColumn id="4" name="label" dataDxfId="88"/>
-    <tableColumn id="5" name="tip" dataDxfId="87"/>
-    <tableColumn id="6" name="type" dataDxfId="86"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="85"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="84"/>
-    <tableColumn id="9" name="editable" dataDxfId="83"/>
-    <tableColumn id="10" name="visible" dataDxfId="82"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="81"/>
-    <tableColumn id="12" name="picklistFilter" dataDxfId="80"/>
-    <tableColumn id="13" name="defaultCode" dataDxfId="79"/>
+    <tableColumn id="1" name="id" dataDxfId="111"/>
+    <tableColumn id="2" name="code" dataDxfId="110"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="109"/>
+    <tableColumn id="4" name="label" dataDxfId="108"/>
+    <tableColumn id="5" name="tip" dataDxfId="107"/>
+    <tableColumn id="6" name="type" dataDxfId="106"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="105"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="104"/>
+    <tableColumn id="9" name="editable" dataDxfId="103"/>
+    <tableColumn id="10" name="visible" dataDxfId="102"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="101"/>
+    <tableColumn id="12" name="picklistFilter" dataDxfId="100"/>
+    <tableColumn id="13" name="defaultCode" dataDxfId="99"/>
     <tableColumn id="18" name="codeFormula"/>
-    <tableColumn id="14" name="defaultValue" dataDxfId="78"/>
+    <tableColumn id="14" name="defaultValue" dataDxfId="98"/>
     <tableColumn id="19" name="labelFormula"/>
-    <tableColumn id="15" name="putInOutput" dataDxfId="77"/>
-    <tableColumn id="16" name="order" dataDxfId="76"/>
-    <tableColumn id="17" name="naturalKey" dataDxfId="75"/>
+    <tableColumn id="15" name="putInOutput" dataDxfId="97"/>
+    <tableColumn id="16" name="order" dataDxfId="96"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:S4" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:S4" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="A1:S4"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="id" dataDxfId="72"/>
-    <tableColumn id="2" name="code" dataDxfId="71"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="70"/>
-    <tableColumn id="4" name="label" dataDxfId="69"/>
-    <tableColumn id="5" name="tip" dataDxfId="68"/>
-    <tableColumn id="6" name="type" dataDxfId="67"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="66"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="65"/>
-    <tableColumn id="9" name="editable" dataDxfId="64"/>
-    <tableColumn id="10" name="visible" dataDxfId="63"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="62"/>
-    <tableColumn id="12" name="picklistFilter" dataDxfId="61"/>
-    <tableColumn id="13" name="defaultCode" dataDxfId="60"/>
-    <tableColumn id="18" name="codeFormula" dataDxfId="59"/>
-    <tableColumn id="14" name="defaultValue" dataDxfId="58"/>
-    <tableColumn id="19" name="labelFormula" dataDxfId="57"/>
-    <tableColumn id="15" name="putInOutput" dataDxfId="56"/>
-    <tableColumn id="16" name="order" dataDxfId="55"/>
-    <tableColumn id="17" name="naturalKey" dataDxfId="54"/>
+    <tableColumn id="1" name="id" dataDxfId="92"/>
+    <tableColumn id="2" name="code" dataDxfId="91"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="90"/>
+    <tableColumn id="4" name="label" dataDxfId="89"/>
+    <tableColumn id="5" name="tip" dataDxfId="88"/>
+    <tableColumn id="6" name="type" dataDxfId="87"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="86"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="85"/>
+    <tableColumn id="9" name="editable" dataDxfId="84"/>
+    <tableColumn id="10" name="visible" dataDxfId="83"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="82"/>
+    <tableColumn id="12" name="picklistFilter" dataDxfId="81"/>
+    <tableColumn id="13" name="defaultCode" dataDxfId="80"/>
+    <tableColumn id="18" name="codeFormula" dataDxfId="79"/>
+    <tableColumn id="14" name="defaultValue" dataDxfId="78"/>
+    <tableColumn id="19" name="labelFormula" dataDxfId="77"/>
+    <tableColumn id="15" name="putInOutput" dataDxfId="76"/>
+    <tableColumn id="16" name="order" dataDxfId="75"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:S8" totalsRowShown="0" headerRowDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:S8" totalsRowShown="0" headerRowDxfId="73">
   <autoFilter ref="A1:S8"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="id" dataDxfId="52"/>
+    <tableColumn id="1" name="id" dataDxfId="72"/>
     <tableColumn id="2" name="code"/>
     <tableColumn id="3" name="xmlTag"/>
-    <tableColumn id="4" name="label" dataDxfId="51"/>
-    <tableColumn id="5" name="tip" dataDxfId="50"/>
-    <tableColumn id="6" name="type" dataDxfId="49"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="48"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="47"/>
-    <tableColumn id="9" name="editable" dataDxfId="46"/>
-    <tableColumn id="10" name="visible" dataDxfId="45"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="44"/>
-    <tableColumn id="17" name="picklistFilter" dataDxfId="43"/>
+    <tableColumn id="4" name="label" dataDxfId="71"/>
+    <tableColumn id="5" name="tip" dataDxfId="70"/>
+    <tableColumn id="6" name="type" dataDxfId="69"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="68"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="67"/>
+    <tableColumn id="9" name="editable" dataDxfId="66"/>
+    <tableColumn id="10" name="visible" dataDxfId="65"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="64"/>
+    <tableColumn id="17" name="picklistFilter" dataDxfId="63"/>
     <tableColumn id="12" name="defaultCode"/>
     <tableColumn id="18" name="codeFormula"/>
     <tableColumn id="13" name="defaultValue"/>
@@ -2118,79 +2379,110 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S36" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S36" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:S36"/>
   <sortState ref="A2:R33">
     <sortCondition ref="R1:R33"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="id" dataDxfId="40"/>
-    <tableColumn id="2" name="code" dataDxfId="39"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="38"/>
-    <tableColumn id="4" name="label" dataDxfId="37"/>
-    <tableColumn id="5" name="tip" dataDxfId="36"/>
-    <tableColumn id="6" name="type" dataDxfId="35"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="34"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="33"/>
-    <tableColumn id="9" name="editable" dataDxfId="32"/>
-    <tableColumn id="10" name="visible" dataDxfId="31"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="30"/>
-    <tableColumn id="16" name="picklistFilter" dataDxfId="29"/>
-    <tableColumn id="12" name="defaultCode" dataDxfId="28"/>
-    <tableColumn id="18" name="codeFormula" dataDxfId="27"/>
-    <tableColumn id="13" name="defaultValue" dataDxfId="26"/>
-    <tableColumn id="19" name="labelFormula" dataDxfId="25"/>
-    <tableColumn id="14" name="putInOutput" dataDxfId="24"/>
-    <tableColumn id="15" name="order" dataDxfId="23"/>
-    <tableColumn id="17" name="naturalKey" dataDxfId="22"/>
+    <tableColumn id="1" name="id" dataDxfId="60"/>
+    <tableColumn id="2" name="code" dataDxfId="59"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="58"/>
+    <tableColumn id="4" name="label" dataDxfId="57"/>
+    <tableColumn id="5" name="tip" dataDxfId="56"/>
+    <tableColumn id="6" name="type" dataDxfId="55"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="54"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="53"/>
+    <tableColumn id="9" name="editable" dataDxfId="52"/>
+    <tableColumn id="10" name="visible" dataDxfId="51"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="50"/>
+    <tableColumn id="16" name="picklistFilter" dataDxfId="49"/>
+    <tableColumn id="12" name="defaultCode" dataDxfId="48"/>
+    <tableColumn id="18" name="codeFormula" dataDxfId="47"/>
+    <tableColumn id="13" name="defaultValue" dataDxfId="46"/>
+    <tableColumn id="19" name="labelFormula" dataDxfId="45"/>
+    <tableColumn id="14" name="putInOutput" dataDxfId="44"/>
+    <tableColumn id="15" name="order" dataDxfId="43"/>
+    <tableColumn id="17" name="naturalKey" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table25" displayName="Table25" ref="A1:S11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table25" displayName="Table25" ref="A1:S11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:S11"/>
   <sortState ref="A2:R33">
     <sortCondition ref="R1:R33"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="id" dataDxfId="19"/>
-    <tableColumn id="2" name="code" dataDxfId="18"/>
-    <tableColumn id="3" name="xmlTag" dataDxfId="17"/>
-    <tableColumn id="4" name="label" dataDxfId="16"/>
-    <tableColumn id="5" name="tip" dataDxfId="15"/>
-    <tableColumn id="6" name="type" dataDxfId="14"/>
-    <tableColumn id="7" name="Controlled terminology" dataDxfId="13"/>
-    <tableColumn id="8" name="mandatory" dataDxfId="12"/>
-    <tableColumn id="9" name="editable" dataDxfId="11"/>
-    <tableColumn id="10" name="visible" dataDxfId="10"/>
-    <tableColumn id="11" name="picklistKey" dataDxfId="9"/>
-    <tableColumn id="16" name="picklistFilter" dataDxfId="8"/>
-    <tableColumn id="12" name="defaultCode" dataDxfId="7"/>
-    <tableColumn id="17" name="codeFormula" dataDxfId="3"/>
-    <tableColumn id="13" name="defaultValue" dataDxfId="6"/>
-    <tableColumn id="18" name="labelFormula" dataDxfId="2"/>
-    <tableColumn id="14" name="putInOutput" dataDxfId="5"/>
-    <tableColumn id="15" name="order" dataDxfId="4"/>
-    <tableColumn id="19" name="naturalKey" dataDxfId="1"/>
+    <tableColumn id="1" name="id" dataDxfId="39"/>
+    <tableColumn id="2" name="code" dataDxfId="38"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="37"/>
+    <tableColumn id="4" name="label" dataDxfId="36"/>
+    <tableColumn id="5" name="tip" dataDxfId="35"/>
+    <tableColumn id="6" name="type" dataDxfId="34"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="33"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="32"/>
+    <tableColumn id="9" name="editable" dataDxfId="31"/>
+    <tableColumn id="10" name="visible" dataDxfId="30"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="29"/>
+    <tableColumn id="16" name="picklistFilter" dataDxfId="28"/>
+    <tableColumn id="12" name="defaultCode" dataDxfId="27"/>
+    <tableColumn id="17" name="codeFormula" dataDxfId="26"/>
+    <tableColumn id="13" name="defaultValue" dataDxfId="25"/>
+    <tableColumn id="18" name="labelFormula" dataDxfId="24"/>
+    <tableColumn id="14" name="putInOutput" dataDxfId="23"/>
+    <tableColumn id="15" name="order" dataDxfId="22"/>
+    <tableColumn id="19" name="naturalKey" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="parentTable"/>
-    <tableColumn id="2" name="childTable" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table257" displayName="Table257" ref="A1:R36" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:R36"/>
+  <sortState ref="A2:P44">
+    <sortCondition ref="B1:B44"/>
+  </sortState>
+  <tableColumns count="18">
+    <tableColumn id="1" name="id" dataDxfId="18"/>
+    <tableColumn id="2" name="code" dataDxfId="17"/>
+    <tableColumn id="3" name="xmlTag" dataDxfId="16"/>
+    <tableColumn id="4" name="label" dataDxfId="15"/>
+    <tableColumn id="5" name="tip" dataDxfId="14"/>
+    <tableColumn id="6" name="type" dataDxfId="13"/>
+    <tableColumn id="7" name="Controlled terminology" dataDxfId="12"/>
+    <tableColumn id="8" name="mandatory" dataDxfId="11"/>
+    <tableColumn id="9" name="editable" dataDxfId="10"/>
+    <tableColumn id="10" name="visible" dataDxfId="9"/>
+    <tableColumn id="11" name="picklistKey" dataDxfId="8"/>
+    <tableColumn id="16" name="picklistFilter" dataDxfId="7"/>
+    <tableColumn id="12" name="defaultCode" dataDxfId="6"/>
+    <tableColumn id="17" name="codeFormula" dataDxfId="5"/>
+    <tableColumn id="13" name="defaultValue" dataDxfId="4"/>
+    <tableColumn id="18" name="labelFormula" dataDxfId="3"/>
+    <tableColumn id="14" name="putInOutput" dataDxfId="2"/>
+    <tableColumn id="15" name="order" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="parentTable"/>
+    <tableColumn id="2" name="childTable" dataDxfId="0"/>
+    <tableColumn id="3" name="directRelation"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:B5" totalsRowShown="0">
   <autoFilter ref="A1:B5"/>
   <tableColumns count="2">
@@ -2491,10 +2783,10 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2559,13 +2851,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -2574,7 +2866,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2677,10 +2969,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2698,11 +2990,10 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12" t="s">
-        <v>229</v>
+      <c r="O4" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -2713,7 +3004,7 @@
         <v>132</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
@@ -2741,14 +3032,13 @@
         <v>175</v>
       </c>
       <c r="L5" s="11"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>214</v>
       </c>
+      <c r="O5" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16">
         <v>3</v>
@@ -2850,13 +3140,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -2865,7 +3155,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2952,17 +3242,17 @@
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>208</v>
@@ -3069,13 +3359,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>115</v>
@@ -3084,7 +3374,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3370,10 +3660,10 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3438,13 +3728,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -3453,7 +3743,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3773,10 +4063,10 @@
         <v>180</v>
       </c>
       <c r="M8" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="O8" s="12" t="s">
         <v>216</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>217</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>11</v>
@@ -4007,7 +4297,7 @@
         <v>3</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>11</v>
@@ -4214,10 +4504,10 @@
         <v>4</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>11</v>
@@ -4249,10 +4539,10 @@
         <v>4</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P21" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>11</v>
@@ -4284,10 +4574,10 @@
         <v>4</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>11</v>
@@ -4319,7 +4609,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>11</v>
@@ -4351,10 +4641,10 @@
         <v>4</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>11</v>
@@ -4421,7 +4711,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>11</v>
@@ -4485,7 +4775,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>11</v>
@@ -4792,13 +5082,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -4807,21 +5097,21 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
         <v>242</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>244</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>245</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>208</v>
@@ -4841,34 +5131,34 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="B3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>248</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>250</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4885,10 +5175,10 @@
         <v>45</v>
       </c>
       <c r="D4" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>251</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>252</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>208</v>
@@ -4908,16 +5198,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>256</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>208</v>
@@ -4937,16 +5227,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>258</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>259</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>208</v>
@@ -4966,16 +5256,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>261</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>262</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>14</v>
@@ -5006,16 +5296,16 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="B8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>264</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>265</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>14</v>
@@ -5033,10 +5323,10 @@
         <v>3</v>
       </c>
       <c r="K8" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>266</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>267</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -5047,37 +5337,37 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="E9" s="12" t="s">
         <v>270</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>271</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="12" t="s">
+      <c r="L9" s="12" t="s">
         <v>273</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>274</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -5088,7 +5378,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>207</v>
@@ -5131,72 +5421,1192 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="3" max="3" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="12" customWidth="1"/>
+    <col min="12" max="12" width="46.85546875" style="12" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="50.7109375" style="12" customWidth="1"/>
+    <col min="15" max="15" width="20" style="12" customWidth="1"/>
+    <col min="16" max="16" width="88.28515625" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" t="s">
-        <v>205</v>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R23" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q24" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q25" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q27" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="P28" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q28" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R28" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q30" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P31" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q31" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q32" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P33" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q33" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q34" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q35" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q36" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -5208,6 +6618,138 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -5222,10 +6764,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5233,7 +6775,7 @@
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5241,7 +6783,7 @@
         <v>204</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5249,7 +6791,7 @@
         <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5257,7 +6799,7 @@
         <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added configuration for headers and fixed export report
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="13530" windowHeight="6015" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="13530" windowHeight="6015" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="5" r:id="rId1"/>
@@ -14,14 +14,15 @@
     <sheet name="CasesInformation" sheetId="11" r:id="rId5"/>
     <sheet name="AnalyticalResults" sheetId="12" r:id="rId6"/>
     <sheet name="Relations" sheetId="9" r:id="rId7"/>
-    <sheet name="Help" sheetId="10" r:id="rId8"/>
+    <sheet name="Tables" sheetId="10" r:id="rId8"/>
+    <sheet name="MessageConfig" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="317">
   <si>
     <t>Type</t>
   </si>
@@ -725,15 +726,9 @@
     <t>tableName</t>
   </si>
   <si>
-    <t>startupHelp.html</t>
-  </si>
-  <si>
     <t>aggregated_level.html</t>
   </si>
   <si>
-    <t>main.html</t>
-  </si>
-  <si>
     <t>naturalKey</t>
   </si>
   <si>
@@ -854,27 +849,9 @@
     <t>RELATION{Preferences, country.label}</t>
   </si>
   <si>
-    <t>RELATION{SummarizedInformation,progId.label}</t>
-  </si>
-  <si>
-    <t>tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code}</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|.\animalId.label</t>
-  </si>
-  <si>
     <t>sampUnitIds</t>
   </si>
   <si>
-    <t>animalId=\animalId|IF_NOT_NULL(herdId,$herdId=\herdId.label,)</t>
-  </si>
-  <si>
-    <t>birthCountry=\birthCountry|IF_NOT_NULL(statusHerd,$statusHerd=\statusHerd.label,)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,sampMatCode.label}</t>
-  </si>
-  <si>
     <t>\sampId.label</t>
   </si>
   <si>
@@ -902,9 +879,6 @@
     <t>evalInfo</t>
   </si>
   <si>
-    <t>tseNationalCaseId=\tseNationalCaseId$tseIndexCase=\tseIndexCase$sampAnAsses=\sampAnAsses</t>
-  </si>
-  <si>
     <t>CasesInformationId</t>
   </si>
   <si>
@@ -914,18 +888,6 @@
     <t>directRelation</t>
   </si>
   <si>
-    <t>tes</t>
-  </si>
-  <si>
-    <t>RELATION{CasesInformation,tseNationalCaseId.label}</t>
-  </si>
-  <si>
-    <t>RELATION{CasesInformation,tseNationalCaseId.code}</t>
-  </si>
-  <si>
-    <t>RELATION{CasesInformation,sampAnAsses.label}</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation, anMethCode.code}</t>
   </si>
   <si>
@@ -933,6 +895,84 @@
   </si>
   <si>
     <t>RELATION{SummarizedInformation, type.code}</t>
+  </si>
+  <si>
+    <t>tseNationalCaseId=\tseNationalCaseId.label$tseIndexCase=\tseIndexCase.label$sampAnAsses=\sampAnAsses.label</t>
+  </si>
+  <si>
+    <t>generateRecord</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation, progId.label}|.\animalId.label</t>
+  </si>
+  <si>
+    <t>tseTargetGroup=RELATION{SummarizedInformation, tseTargetGroup.code}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation, progId.label}</t>
+  </si>
+  <si>
+    <t>animalId=\animalId.code|IF_NOT_NULL(herdId, $herdId=\herdId.label, )</t>
+  </si>
+  <si>
+    <t>birthCountry=\birthCountry.code|IF_NOT_NULL(statusHerd, $statusHerd=\statusHerd.label, )</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation, sampMatCode.label}</t>
+  </si>
+  <si>
+    <t>RELATION{CasesInformation, tseNationalCaseId.label}</t>
+  </si>
+  <si>
+    <t>RELATION{CasesInformation, tseNationalCaseId.code}</t>
+  </si>
+  <si>
+    <t>RELATION{CasesInformation, sampAnAsses.label}</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>dcfmsg</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>senderMessageId</t>
+  </si>
+  <si>
+    <t>senderOrgCode</t>
+  </si>
+  <si>
+    <t>receiverOrgCode</t>
+  </si>
+  <si>
+    <t>EFSA</t>
+  </si>
+  <si>
+    <t>senderDatasetId</t>
+  </si>
+  <si>
+    <t>RELATION{Report, reportSenderId.code}</t>
+  </si>
+  <si>
+    <t>RELATION{Settings, orgCode.code}</t>
+  </si>
+  <si>
+    <t>RELATION{Report, reportSenderId.code}|today.timestamp</t>
+  </si>
+  <si>
+    <t>putInHeader</t>
+  </si>
+  <si>
+    <t>putInOperation</t>
+  </si>
+  <si>
+    <t>isDatasetRoot</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1070,6 +1110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2483,11 +2524,26 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="tableName"/>
     <tableColumn id="2" name="htmlFilename"/>
+    <tableColumn id="3" name="generateRecord"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="xmlTag"/>
+    <tableColumn id="2" name="value"/>
+    <tableColumn id="3" name="putInHeader"/>
+    <tableColumn id="4" name="putInOperation"/>
+    <tableColumn id="5" name="isDatasetRoot"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2786,7 +2842,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,13 +2907,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -2866,7 +2922,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3036,7 +3092,7 @@
         <v>214</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
@@ -3140,13 +3196,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -3155,7 +3211,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3359,13 +3415,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>115</v>
@@ -3374,7 +3430,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3660,10 +3716,10 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3728,13 +3784,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -3743,7 +3799,7 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4711,7 +4767,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>11</v>
@@ -5017,7 +5073,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,13 +5138,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -5097,21 +5153,21 @@
         <v>174</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>244</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>208</v>
@@ -5131,22 +5187,22 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="B3" t="s">
-        <v>242</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>247</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>3</v>
@@ -5158,7 +5214,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -5175,10 +5231,10 @@
         <v>45</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>208</v>
@@ -5198,16 +5254,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>253</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>255</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>208</v>
@@ -5227,16 +5283,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>258</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>208</v>
@@ -5256,16 +5312,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>14</v>
@@ -5296,16 +5352,16 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>262</v>
-      </c>
-      <c r="B8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>264</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>14</v>
@@ -5323,10 +5379,10 @@
         <v>3</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -5337,37 +5393,37 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="E9" s="12" t="s">
         <v>268</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>270</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>271</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>273</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -5378,7 +5434,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>207</v>
@@ -5423,11 +5479,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5492,13 +5548,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -5536,7 +5592,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>11</v>
@@ -5603,7 +5659,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>11</v>
@@ -5635,7 +5691,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>11</v>
@@ -5643,13 +5699,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>208</v>
@@ -5667,7 +5723,7 @@
         <v>4</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>11</v>
@@ -5675,13 +5731,13 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>253</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>255</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>208</v>
@@ -5704,13 +5760,13 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>258</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>208</v>
@@ -5751,7 +5807,7 @@
         <v>4</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>11</v>
@@ -5791,13 +5847,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>14</v>
@@ -5829,10 +5885,10 @@
         <v>45</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>208</v>
@@ -5925,22 +5981,22 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="E15" s="12" t="s">
         <v>268</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>270</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>3</v>
@@ -5952,10 +6008,10 @@
         <v>4</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>11</v>
@@ -6127,7 +6183,7 @@
         <v>4</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>11</v>
@@ -6159,7 +6215,7 @@
         <v>4</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>11</v>
@@ -6176,10 +6232,10 @@
         <v>86</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>209</v>
@@ -6214,19 +6270,19 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>209</v>
@@ -6285,10 +6341,10 @@
         <v>4</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="O24" s="12" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>11</v>
@@ -6431,13 +6487,13 @@
         <v>123</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>11</v>
@@ -6477,13 +6533,13 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>4</v>
@@ -6492,7 +6548,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>11</v>
@@ -6500,10 +6556,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>4</v>
@@ -6512,7 +6568,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>5</v>
@@ -6520,10 +6576,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I32" s="12" t="s">
         <v>4</v>
@@ -6532,7 +6588,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>5</v>
@@ -6540,10 +6596,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>4</v>
@@ -6552,7 +6608,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>5</v>
@@ -6560,7 +6616,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>207</v>
@@ -6577,7 +6633,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>207</v>
@@ -6622,7 +6678,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6639,7 +6695,7 @@
         <v>203</v>
       </c>
       <c r="C1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6647,7 +6703,7 @@
         <v>204</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -6658,7 +6714,7 @@
         <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -6710,13 +6766,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
-        <v>297</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6724,7 +6780,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -6735,7 +6791,7 @@
         <v>205</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -6751,55 +6807,208 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>233</v>
       </c>
       <c r="B1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>204</v>
       </c>
-      <c r="B3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>210</v>
       </c>
-      <c r="B4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>211</v>
       </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>307</v>
+      </c>
       <c r="B5" t="s">
-        <v>234</v>
+        <v>312</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added refresh button to summ info dialog
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="328">
   <si>
     <t>Type</t>
   </si>
@@ -985,6 +985,27 @@
   </si>
   <si>
     <t>repVersion</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>repMexId</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH, used with GetAck</t>
+  </si>
+  <si>
+    <t>General formula: TableName + Version to save the table version</t>
+  </si>
+  <si>
+    <t>reportMessageId</t>
+  </si>
+  <si>
+    <t>reportStatus</t>
+  </si>
+  <si>
+    <t>repStatus</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1123,6 +1144,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2485,8 +2510,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S7" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131">
-  <autoFilter ref="A1:S7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S8" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131">
+  <autoFilter ref="A1:S8"/>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="130"/>
     <tableColumn id="2" name="code" dataDxfId="129"/>
@@ -3000,13 +3025,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3015,7 +3040,7 @@
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="62.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
@@ -3130,7 +3155,9 @@
         <v>198</v>
       </c>
       <c r="P2" s="11"/>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="R2" s="2">
         <v>1</v>
       </c>
@@ -3179,7 +3206,9 @@
         <v>196</v>
       </c>
       <c r="P3" s="11"/>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="R3" s="2">
         <v>2</v>
       </c>
@@ -3217,9 +3246,13 @@
       <c r="O4" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -3261,7 +3294,9 @@
         <v>272</v>
       </c>
       <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
+      <c r="Q5" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="R5" s="16">
         <v>3</v>
       </c>
@@ -3285,6 +3320,12 @@
       <c r="J6" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="Q6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -3293,6 +3334,9 @@
       <c r="B7" s="12" t="s">
         <v>320</v>
       </c>
+      <c r="E7" s="12" t="s">
+        <v>324</v>
+      </c>
       <c r="F7" s="12" t="s">
         <v>208</v>
       </c>
@@ -3305,8 +3349,92 @@
       <c r="J7" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="M7" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="S7" s="12" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -7146,10 +7274,10 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
improved opening time of a report
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="13530" windowHeight="6015" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="13530" windowHeight="5895" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="398">
   <si>
     <t>Type</t>
   </si>
@@ -1089,9 +1089,6 @@
     <t>ALL</t>
   </si>
   <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==SCRAPIE),Yes,No)</t>
-  </si>
-  <si>
     <t>First test</t>
   </si>
   <si>
@@ -1149,9 +1146,6 @@
     <t>(%anMethType.code==AT13A)</t>
   </si>
   <si>
-    <t>A04MQ#%source.code$%part.code$%prod.code$%animage.code</t>
-  </si>
-  <si>
     <t>birthCountry=RELATION{CasesInformation,birthCountry.code}|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
   </si>
   <si>
@@ -1167,9 +1161,6 @@
     <t>%type.label</t>
   </si>
   <si>
-    <t>(RELATION{SummarizedInformation,prod.code}!=F21.A07RY)</t>
-  </si>
-  <si>
     <t>opType</t>
   </si>
   <si>
@@ -1194,9 +1185,6 @@
     <t>%country.code|END_TRIM(%reportYear.code,2)|END_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
   </si>
   <si>
-    <t>RF-00004628-PAR|IF_NOT_NULL(%allele1.code,#allele=%allele1.code,)|IF_NOT_NULL(%allele2.code,$allele=%allele2.code,)</t>
-  </si>
-  <si>
     <t>RES|_ZERO_PADDING({rowId},6)</t>
   </si>
   <si>
@@ -1207,6 +1195,27 @@
   </si>
   <si>
     <t>RESEVAL</t>
+  </si>
+  <si>
+    <t>A04MQ#%source.code$%prod.code$%animage.code</t>
+  </si>
+  <si>
+    <t>(%sampAnAsses.code!=J051A)</t>
+  </si>
+  <si>
+    <t>((%sampAnAsses.code!=J051A)AND(RELATION{SummarizedInformation,prod.code}!=F21.A07RY))</t>
+  </si>
+  <si>
+    <t>paramCodeBaseTerm</t>
+  </si>
+  <si>
+    <t>%paramCodeBaseTerm.code|IF_NOT_NULL(%allele1.code,#allele=%allele1.code,)|IF_NOT_NULL(%allele2.code,$allele=%allele2.code,)</t>
+  </si>
+  <si>
+    <t>NOTE: AUTOMATICALLY FILLED BY CUSTOM LIBRARY</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,type.code}==SCRAPIE)</t>
   </si>
 </sst>
 </file>
@@ -2811,8 +2820,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S36" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S35" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:S35"/>
   <sortState ref="A2:S36">
     <sortCondition ref="R1:R36"/>
   </sortState>
@@ -2873,8 +2882,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R34" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A1:R34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R35" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A1:R35"/>
   <sortState ref="A2:R37">
     <sortCondition ref="B1:B37"/>
   </sortState>
@@ -4049,7 +4058,7 @@
         <v>332</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4137,13 +4146,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>262</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>194</v>
@@ -4293,13 +4302,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4414,7 +4423,7 @@
         <v>119</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4458,10 +4467,10 @@
         <v>121</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>129</v>
@@ -4478,22 +4487,22 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
@@ -4505,22 +4514,16 @@
         <v>3</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>378</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>127</v>
+        <v>367</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>11</v>
@@ -4528,22 +4531,22 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>3</v>
@@ -4555,16 +4558,16 @@
         <v>3</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>11</v>
@@ -4572,25 +4575,28 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>17</v>
+        <v>40</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>3</v>
+        <v>370</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>3</v>
@@ -4599,16 +4605,16 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q6" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="R6" s="12">
         <v>5</v>
-      </c>
-      <c r="R6" s="12">
-        <v>4</v>
       </c>
       <c r="S6" s="12" t="s">
         <v>11</v>
@@ -4616,28 +4622,28 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>42</v>
+        <v>352</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>43</v>
+        <v>351</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>371</v>
+        <v>3</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
@@ -4646,42 +4652,45 @@
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>118</v>
+        <v>353</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>368</v>
       </c>
+      <c r="M7" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>286</v>
+      </c>
       <c r="Q7" s="12" t="s">
-        <v>372</v>
+        <v>11</v>
       </c>
       <c r="R7" s="12">
-        <v>5</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>3</v>
@@ -4693,45 +4702,42 @@
         <v>3</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>353</v>
+        <v>123</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>100</v>
+        <v>363</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>286</v>
+        <v>362</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>356</v>
+        <v>27</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>357</v>
+        <v>28</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>14</v>
+        <v>261</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>3</v>
@@ -4742,37 +4748,28 @@
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>363</v>
+      <c r="O9" s="12">
+        <v>0</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="R9" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>261</v>
@@ -4796,21 +4793,21 @@
         <v>5</v>
       </c>
       <c r="R10" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>261</v>
@@ -4834,21 +4831,21 @@
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>261</v>
@@ -4860,33 +4857,33 @@
         <v>3</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="12">
-        <v>0</v>
+      <c r="P12" s="12" t="s">
+        <v>361</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>261</v>
@@ -4898,36 +4895,39 @@
         <v>3</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P13" s="12" t="s">
-        <v>362</v>
+      <c r="O13" s="12">
+        <v>0</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>261</v>
+        <v>194</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>10</v>
@@ -4936,45 +4936,39 @@
         <v>3</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="12">
-        <v>0</v>
+      <c r="O14" s="12" t="s">
+        <v>388</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="R14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>7</v>
+        <v>107</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -4982,72 +4976,72 @@
       <c r="J15" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="K15" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="O15" s="12" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="R15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>159</v>
+        <v>15</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>160</v>
+        <v>4</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>368</v>
+        <v>16</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>380</v>
+        <v>16</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R16" s="12">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>3</v>
@@ -5058,11 +5052,8 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>16</v>
+      <c r="P17" s="12" t="s">
+        <v>360</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>11</v>
@@ -5070,13 +5061,13 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>194</v>
@@ -5085,7 +5076,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>3</v>
+        <v>369</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -5094,21 +5085,21 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>11</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>194</v>
@@ -5117,7 +5108,7 @@
         <v>10</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>370</v>
+        <v>3</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -5129,24 +5120,24 @@
         <v>365</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>370</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>3</v>
@@ -5157,8 +5148,11 @@
       <c r="J20" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N20" s="12" t="s">
+        <v>242</v>
+      </c>
       <c r="P20" s="12" t="s">
-        <v>366</v>
+        <v>328</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>11</v>
@@ -5166,13 +5160,13 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>194</v>
@@ -5201,19 +5195,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>194</v>
+        <v>261</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>3</v>
@@ -5225,10 +5219,10 @@
         <v>4</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>242</v>
+        <v>326</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>11</v>
@@ -5236,13 +5230,13 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>261</v>
@@ -5259,11 +5253,8 @@
       <c r="J23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N23" s="12" t="s">
-        <v>326</v>
-      </c>
       <c r="P23" s="12" t="s">
-        <v>329</v>
+        <v>359</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>11</v>
@@ -5271,13 +5262,13 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>261</v>
@@ -5294,8 +5285,11 @@
       <c r="J24" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N24" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="P24" s="12" t="s">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>11</v>
@@ -5303,19 +5297,19 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>261</v>
+        <v>194</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>3</v>
@@ -5326,11 +5320,11 @@
       <c r="J25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N25" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="P25" s="12" t="s">
-        <v>330</v>
+      <c r="M25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>11</v>
@@ -5338,19 +5332,19 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>3</v>
@@ -5361,11 +5355,8 @@
       <c r="J26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="O26" s="12" t="s">
-        <v>63</v>
+      <c r="P26" s="12" t="s">
+        <v>391</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>11</v>
@@ -5373,19 +5364,19 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>3</v>
@@ -5397,7 +5388,7 @@
         <v>4</v>
       </c>
       <c r="P27" s="12" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>11</v>
@@ -5405,16 +5396,16 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>194</v>
+        <v>261</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>10</v>
@@ -5429,7 +5420,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>11</v>
@@ -5437,19 +5428,19 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>261</v>
+        <v>194</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>3</v>
@@ -5460,8 +5451,11 @@
       <c r="J29" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P29" s="12" t="s">
-        <v>360</v>
+      <c r="M29" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>11</v>
@@ -5469,19 +5463,19 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>3</v>
@@ -5493,10 +5487,10 @@
         <v>4</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>11</v>
@@ -5504,19 +5498,19 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>3</v>
@@ -5527,11 +5521,8 @@
       <c r="J31" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M31" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="O31" s="12" t="s">
-        <v>94</v>
+      <c r="P31" s="12" t="s">
+        <v>366</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>11</v>
@@ -5539,13 +5530,13 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>194</v>
@@ -5562,8 +5553,8 @@
       <c r="J32" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P32" s="12" t="s">
-        <v>367</v>
+      <c r="O32" s="12" t="s">
+        <v>372</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>11</v>
@@ -5571,22 +5562,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>106</v>
+        <v>192</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>4</v>
@@ -5594,16 +5573,13 @@
       <c r="J33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O33" s="12" t="s">
-        <v>373</v>
-      </c>
       <c r="Q33" s="12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>193</v>
@@ -5620,7 +5596,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>193</v>
@@ -5632,23 +5608,6 @@
         <v>4</v>
       </c>
       <c r="Q35" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5665,10 +5624,10 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5768,7 +5727,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>3</v>
@@ -5827,7 +5786,7 @@
         <v>337</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>127</v>
@@ -5862,7 +5821,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>3</v>
+        <v>392</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>3</v>
@@ -5935,7 +5894,7 @@
         <v>218</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>3</v>
+        <v>392</v>
       </c>
       <c r="I6" s="29" t="s">
         <v>3</v>
@@ -5976,7 +5935,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>3</v>
+        <v>392</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
@@ -6082,7 +6041,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>3</v>
+        <v>392</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>3</v>
@@ -6110,10 +6069,10 @@
         <v>40</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>358</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>359</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>14</v>
@@ -6160,7 +6119,7 @@
         <v>313</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>3</v>
@@ -6196,7 +6155,7 @@
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="29" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="I13" s="26" t="s">
         <v>3</v>
@@ -6234,7 +6193,7 @@
         <v>240</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>3</v>
+        <v>392</v>
       </c>
       <c r="I14" s="23" t="s">
         <v>3</v>
@@ -6405,13 +6364,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6517,7 +6476,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>11</v>
@@ -6677,7 +6636,7 @@
         <v>4</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>11</v>
@@ -7169,13 +7128,10 @@
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>92</v>
+        <v>394</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>396</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>194</v>
@@ -7192,147 +7148,135 @@
       <c r="J22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P22" s="12" t="s">
-        <v>390</v>
-      </c>
       <c r="Q22" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>296</v>
+        <v>92</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>294</v>
+      <c r="C23" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>14</v>
+        <v>194</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>374</v>
+        <v>3</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>355</v>
+        <v>4</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="L23" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>395</v>
+      </c>
       <c r="Q23" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R23" s="12">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>91</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>355</v>
+        <v>397</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>355</v>
+        <v>397</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="L24" s="13"/>
       <c r="Q24" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R24" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>96</v>
+        <v>293</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>3</v>
+        <v>373</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>3</v>
+        <v>397</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O25" s="12" t="s">
-        <v>341</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="L25" s="13"/>
       <c r="Q25" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="R25" s="12">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>194</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>3</v>
@@ -7343,46 +7287,37 @@
       <c r="J26" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="M26" s="12" t="s">
-        <v>100</v>
-      </c>
       <c r="O26" s="12" t="s">
-        <v>286</v>
+        <v>341</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R26" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>103</v>
+        <v>287</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>14</v>
+        <v>194</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>3</v>
@@ -7394,45 +7329,45 @@
         <v>3</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>123</v>
+        <v>353</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="N27" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="P27" s="12" t="s">
-        <v>336</v>
+        <v>354</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>286</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R27" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>285</v>
+        <v>158</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>284</v>
+        <v>103</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>194</v>
+        <v>14</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>3</v>
@@ -7443,37 +7378,46 @@
       <c r="J28" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="K28" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>338</v>
+      </c>
       <c r="O28" s="12" t="s">
-        <v>391</v>
+        <v>336</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R28" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>282</v>
+        <v>106</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>283</v>
+        <v>105</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>282</v>
+        <v>106</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>14</v>
+        <v>194</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>279</v>
+        <v>10</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>3</v>
@@ -7484,54 +7428,66 @@
       <c r="J29" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="12" t="s">
-        <v>278</v>
+      <c r="O29" s="12" t="s">
+        <v>387</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R29" s="12">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q30" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R30" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B31" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>276</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>248</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>194</v>
@@ -7545,33 +7501,45 @@
       <c r="J31" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P31" s="12" t="s">
+      <c r="M31" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q31" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P32" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="Q31" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>4</v>
-      </c>
       <c r="Q32" s="12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>193</v>
@@ -7588,7 +7556,7 @@
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>192</v>
+        <v>249</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>193</v>
@@ -7600,6 +7568,23 @@
         <v>4</v>
       </c>
       <c r="Q34" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q35" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7836,7 +7821,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8162,7 +8147,7 @@
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>194</v>
@@ -8184,7 +8169,7 @@
         <v>345</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -8243,18 +8228,18 @@
         <v>346</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>194</v>

</xml_diff>

<commit_message>
renamed data folder to picklists, added documentation
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="399">
   <si>
     <t>Type</t>
   </si>
@@ -1216,6 +1216,9 @@
   </si>
   <si>
     <t>(RELATION{SummarizedInformation,type.code}==SCRAPIE)</t>
+  </si>
+  <si>
+    <t>Zoonotic Agent</t>
   </si>
 </sst>
 </file>
@@ -4308,7 +4311,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6367,10 +6370,10 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7130,6 +7133,9 @@
       <c r="A22" s="12" t="s">
         <v>394</v>
       </c>
+      <c r="D22" s="12" t="s">
+        <v>398</v>
+      </c>
       <c r="E22" s="28" t="s">
         <v>396</v>
       </c>
@@ -7143,10 +7149,10 @@
         <v>3</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Fixed configuration bug and import/download bugs
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="13530" windowHeight="5835" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="13530" windowHeight="5835" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="420">
   <si>
     <t>Type</t>
   </si>
@@ -507,15 +507,6 @@
     <t>picklistFilter</t>
   </si>
   <si>
-    <t>BSE</t>
-  </si>
-  <si>
-    <t>SCRAPIE</t>
-  </si>
-  <si>
-    <t>CWD</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -849,9 +840,6 @@
     <t>POSNEG</t>
   </si>
   <si>
-    <t>Result of the applied test</t>
-  </si>
-  <si>
     <t>Test Result</t>
   </si>
   <si>
@@ -1011,33 +999,15 @@
     <t>RELATION{Preferences,country.label}</t>
   </si>
   <si>
-    <t>RELATION{SummarizedInformation,sampMatCode.label}</t>
-  </si>
-  <si>
     <t>IF_NOT_NULL(RELATION{CasesInformation,breed.label},com=RELATION{CasesInformation,breed.label},)</t>
   </si>
   <si>
-    <t>RELATION{SummarizedInformation,anMethCode.label}</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation,type.code}</t>
   </si>
   <si>
-    <t>RELATION{SummarizedInformation,anMethCode.code}</t>
-  </si>
-  <si>
     <t>daysList</t>
   </si>
   <si>
-    <t>RELATION{SummarizedInformation,progId.label}|.RELATION{CasesInformation,animalId.label}</t>
-  </si>
-  <si>
-    <t>AT06A|.|RELATION{SummarizedInformation,anMethCode.code}</t>
-  </si>
-  <si>
-    <t>animalId=RELATION{CasesInformation,animalId.code}|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)</t>
-  </si>
-  <si>
     <t>RELATION{Settings,orgCode.code}</t>
   </si>
   <si>
@@ -1053,9 +1023,6 @@
     <t>{app.dcTable}</t>
   </si>
   <si>
-    <t>tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}|$tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}|$sampAnAsses=RELATION{CasesInformation,sampAnAsses.code}|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
-  </si>
-  <si>
     <t>Type of the first executed test</t>
   </si>
   <si>
@@ -1065,9 +1032,6 @@
     <t>anMethTypesLists</t>
   </si>
   <si>
-    <t>ALL</t>
-  </si>
-  <si>
     <t>First test</t>
   </si>
   <si>
@@ -1113,9 +1077,6 @@
     <t>IF_NOT_NULL(%statusHerd.code,yes,no)</t>
   </si>
   <si>
-    <t>(%type.code == SCRAPIE)</t>
-  </si>
-  <si>
     <t>IF_NOT_NULL(%statusHerd.code,Yes,No)</t>
   </si>
   <si>
@@ -1125,9 +1086,6 @@
     <t>(%anMethType.code==AT13A)</t>
   </si>
   <si>
-    <t>birthCountry=RELATION{CasesInformation,birthCountry.code}|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation,progId.label}</t>
   </si>
   <si>
@@ -1242,9 +1200,6 @@
     <t>testAim</t>
   </si>
   <si>
-    <t>Test aim</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation,type.code}|%anMethType.code</t>
   </si>
   <si>
@@ -1282,6 +1237,51 @@
   </si>
   <si>
     <t>IF((%internalOpType.label!=Test),RELATION{Report,reportSenderId.code}|-|today.timestamp,TEST_CONNECTION_|RELATION{Settings,username.code}|_version_{app.version})</t>
+  </si>
+  <si>
+    <t>BSE$AT06A</t>
+  </si>
+  <si>
+    <t>SCRAPIE$AT06A</t>
+  </si>
+  <si>
+    <t>CWD$AT06A</t>
+  </si>
+  <si>
+    <t>BSE$AT08A</t>
+  </si>
+  <si>
+    <t>SCRAPIE$AT08A</t>
+  </si>
+  <si>
+    <t>CWD$AT08A</t>
+  </si>
+  <si>
+    <t>BSE$AT12A</t>
+  </si>
+  <si>
+    <t>SCRAPIE$AT12A</t>
+  </si>
+  <si>
+    <t>CWD$AT12A</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|sampAnAsses=RELATION{CasesInformation,sampAnAsses.code}|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)</t>
+  </si>
+  <si>
+    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}$RELATION{SummarizedInformation,animage.code}</t>
+  </si>
+  <si>
+    <t>(%type.code==SCRAPIE)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.RELATION{CasesInformation,sampId.label}</t>
   </si>
 </sst>
 </file>
@@ -3390,13 +3390,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -3405,7 +3405,7 @@
         <v>158</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3417,13 +3417,13 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>151</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>153</v>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>152</v>
@@ -3492,20 +3492,20 @@
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>153</v>
@@ -3548,7 +3548,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3609,13 +3609,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>115</v>
@@ -3624,7 +3624,7 @@
         <v>158</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3632,7 +3632,7 @@
         <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>131</v>
@@ -3668,14 +3668,14 @@
         <v>133</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
         <v>134</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>14</v>
@@ -3696,7 +3696,7 @@
         <v>123</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>161</v>
+        <v>405</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3707,14 +3707,14 @@
         <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
         <v>136</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>14</v>
@@ -3735,7 +3735,7 @@
         <v>123</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>162</v>
+        <v>406</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3746,14 +3746,14 @@
         <v>137</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="7" t="s">
         <v>138</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -3774,7 +3774,7 @@
         <v>123</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>163</v>
+        <v>407</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3785,7 +3785,7 @@
         <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
@@ -3813,7 +3813,7 @@
         <v>123</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>161</v>
+        <v>408</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3824,7 +3824,7 @@
         <v>142</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
@@ -3852,7 +3852,7 @@
         <v>123</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>162</v>
+        <v>409</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3863,7 +3863,7 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="7" t="s">
@@ -3891,7 +3891,7 @@
         <v>123</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>163</v>
+        <v>410</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3899,17 +3899,17 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>14</v>
@@ -3930,7 +3930,7 @@
         <v>123</v>
       </c>
       <c r="L9" s="32" t="s">
-        <v>161</v>
+        <v>411</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -3938,17 +3938,17 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>14</v>
@@ -3969,7 +3969,7 @@
         <v>123</v>
       </c>
       <c r="L10" s="32" t="s">
-        <v>162</v>
+        <v>412</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -3977,17 +3977,17 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="F11" s="34" t="s">
         <v>14</v>
@@ -4008,7 +4008,7 @@
         <v>123</v>
       </c>
       <c r="L11" s="32" t="s">
-        <v>163</v>
+        <v>413</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
@@ -4101,13 +4101,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -4116,28 +4116,28 @@
         <v>158</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>11</v>
@@ -4149,15 +4149,15 @@
         <v>11</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -4172,17 +4172,17 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>14</v>
@@ -4200,15 +4200,15 @@
         <v>11</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -4223,18 +4223,18 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -4251,10 +4251,10 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4271,7 +4271,7 @@
         <v>130</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
@@ -4300,11 +4300,11 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16" t="s">
@@ -4319,10 +4319,10 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>5</v>
@@ -4342,16 +4342,16 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>5</v>
@@ -4372,18 +4372,18 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23" t="s">
@@ -4411,18 +4411,18 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23" t="s">
@@ -4450,18 +4450,18 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23" t="s">
@@ -4504,7 +4504,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4569,13 +4569,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -4584,7 +4584,7 @@
         <v>158</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4619,13 +4619,13 @@
         <v>119</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R2" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S2" s="12" t="s">
         <v>11</v>
@@ -4663,10 +4663,10 @@
         <v>121</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>129</v>
@@ -4675,7 +4675,7 @@
         <v>5</v>
       </c>
       <c r="R3" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S3" s="12" t="s">
         <v>11</v>
@@ -4713,13 +4713,13 @@
         <v>122</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>11</v>
@@ -4757,13 +4757,13 @@
         <v>117</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>11</v>
@@ -4792,7 +4792,7 @@
         <v>44</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>363</v>
+        <v>417</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>3</v>
@@ -4804,13 +4804,13 @@
         <v>118</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="R6" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S6" s="12" t="s">
         <v>11</v>
@@ -4827,10 +4827,10 @@
         <v>98</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>14</v>
@@ -4848,22 +4848,22 @@
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="M7" s="12" t="s">
         <v>100</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R7" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -4877,10 +4877,10 @@
         <v>102</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>14</v>
@@ -4901,19 +4901,19 @@
         <v>123</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R8" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -4930,7 +4930,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>10</v>
@@ -4951,7 +4951,7 @@
         <v>5</v>
       </c>
       <c r="R9" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -4968,7 +4968,7 @@
         <v>31</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>10</v>
@@ -4989,7 +4989,7 @@
         <v>5</v>
       </c>
       <c r="R10" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -5006,7 +5006,7 @@
         <v>34</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>10</v>
@@ -5027,7 +5027,7 @@
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -5044,7 +5044,7 @@
         <v>25</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>10</v>
@@ -5059,13 +5059,13 @@
         <v>3</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -5082,7 +5082,7 @@
         <v>37</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>10</v>
@@ -5103,7 +5103,7 @@
         <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -5123,7 +5123,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>10</v>
@@ -5138,13 +5138,13 @@
         <v>3</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R14" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -5161,7 +5161,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>156</v>
@@ -5176,16 +5176,16 @@
         <v>157</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R15" s="12">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -5199,7 +5199,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>15</v>
@@ -5234,7 +5234,7 @@
         <v>18</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>10</v>
@@ -5249,7 +5249,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>11</v>
@@ -5266,13 +5266,13 @@
         <v>39</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -5281,10 +5281,10 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -5298,7 +5298,7 @@
         <v>46</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>10</v>
@@ -5313,7 +5313,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>11</v>
@@ -5330,7 +5330,7 @@
         <v>48</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>49</v>
@@ -5345,10 +5345,10 @@
         <v>4</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>11</v>
@@ -5365,7 +5365,7 @@
         <v>51</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>49</v>
@@ -5380,10 +5380,10 @@
         <v>4</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="P21" s="12" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>11</v>
@@ -5400,7 +5400,7 @@
         <v>53</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>10</v>
@@ -5415,10 +5415,10 @@
         <v>4</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>11</v>
@@ -5435,7 +5435,7 @@
         <v>55</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>10</v>
@@ -5450,7 +5450,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>11</v>
@@ -5467,7 +5467,7 @@
         <v>58</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>10</v>
@@ -5482,10 +5482,10 @@
         <v>4</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>11</v>
@@ -5502,7 +5502,7 @@
         <v>61</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>62</v>
@@ -5537,7 +5537,7 @@
         <v>65</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>66</v>
@@ -5552,7 +5552,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="12" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>11</v>
@@ -5569,7 +5569,7 @@
         <v>84</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>10</v>
@@ -5584,7 +5584,7 @@
         <v>4</v>
       </c>
       <c r="P27" s="12" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>11</v>
@@ -5601,7 +5601,7 @@
         <v>86</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>10</v>
@@ -5616,7 +5616,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>11</v>
@@ -5633,7 +5633,7 @@
         <v>88</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>89</v>
@@ -5668,7 +5668,7 @@
         <v>92</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>93</v>
@@ -5703,7 +5703,7 @@
         <v>96</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>10</v>
@@ -5718,7 +5718,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="12" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>11</v>
@@ -5735,7 +5735,7 @@
         <v>106</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>10</v>
@@ -5750,7 +5750,7 @@
         <v>4</v>
       </c>
       <c r="O32" s="12" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>11</v>
@@ -5758,10 +5758,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>4</v>
@@ -5775,10 +5775,10 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>4</v>
@@ -5792,10 +5792,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>4</v>
@@ -5809,13 +5809,13 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>4</v>
@@ -5843,10 +5843,10 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD20"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5911,13 +5911,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -5926,27 +5926,27 @@
         <v>158</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>3</v>
@@ -5958,10 +5958,10 @@
         <v>3</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -6002,10 +6002,10 @@
         <v>120</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>127</v>
@@ -6022,25 +6022,25 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="B4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>210</v>
-      </c>
       <c r="F4" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>3</v>
@@ -6066,13 +6066,13 @@
         <v>45</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>10</v>
@@ -6095,25 +6095,25 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="I6" s="29" t="s">
         <v>3</v>
@@ -6122,10 +6122,10 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -6136,25 +6136,25 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>221</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
@@ -6171,19 +6171,19 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>10</v>
@@ -6207,19 +6207,19 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>10</v>
@@ -6242,16 +6242,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>14</v>
@@ -6260,7 +6260,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>3</v>
@@ -6282,22 +6282,22 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>4</v>
@@ -6309,7 +6309,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -6320,25 +6320,25 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>3</v>
@@ -6347,7 +6347,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
@@ -6358,23 +6358,23 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="29" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="I13" s="26" t="s">
         <v>3</v>
@@ -6383,7 +6383,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6394,25 +6394,25 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>232</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="I14" s="23" t="s">
         <v>3</v>
@@ -6421,10 +6421,10 @@
         <v>3</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -6435,16 +6435,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>14</v>
@@ -6459,7 +6459,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
@@ -6470,19 +6470,19 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>10</v>
@@ -6505,19 +6505,19 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>10</v>
@@ -6540,10 +6540,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -6557,10 +6557,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -6574,13 +6574,13 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>4</v>
@@ -6608,11 +6608,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6626,7 +6626,7 @@
     <col min="7" max="7" width="23.85546875" style="12" customWidth="1"/>
     <col min="8" max="8" width="49.42578125" style="12" customWidth="1"/>
     <col min="9" max="9" width="51.28515625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="39.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="55" style="12" customWidth="1"/>
     <col min="11" max="11" width="17" style="12" customWidth="1"/>
     <col min="12" max="12" width="67.140625" style="12" customWidth="1"/>
     <col min="13" max="13" width="19.140625" style="12" customWidth="1"/>
@@ -6677,13 +6677,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -6703,7 +6703,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>10</v>
@@ -6718,7 +6718,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>11</v>
@@ -6735,7 +6735,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>15</v>
@@ -6770,7 +6770,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>10</v>
@@ -6785,7 +6785,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>11</v>
@@ -6802,7 +6802,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>10</v>
@@ -6817,7 +6817,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>335</v>
+        <v>419</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>11</v>
@@ -6825,16 +6825,16 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>10</v>
@@ -6849,7 +6849,7 @@
         <v>4</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>337</v>
+        <v>415</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>11</v>
@@ -6866,7 +6866,7 @@
         <v>108</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>3</v>
@@ -6878,7 +6878,7 @@
         <v>4</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>367</v>
+        <v>418</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>11</v>
@@ -6895,13 +6895,13 @@
         <v>46</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>10</v>
@@ -6916,7 +6916,7 @@
         <v>4</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>11</v>
@@ -6933,7 +6933,7 @@
         <v>48</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>49</v>
@@ -6948,7 +6948,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>11</v>
@@ -6965,7 +6965,7 @@
         <v>51</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>49</v>
@@ -6980,7 +6980,7 @@
         <v>4</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>11</v>
@@ -6988,25 +6988,25 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>232</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>3</v>
@@ -7018,13 +7018,13 @@
         <v>4</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>11</v>
@@ -7041,7 +7041,7 @@
         <v>53</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>10</v>
@@ -7056,7 +7056,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>11</v>
@@ -7073,7 +7073,7 @@
         <v>55</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>10</v>
@@ -7088,7 +7088,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>11</v>
@@ -7105,7 +7105,7 @@
         <v>58</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>10</v>
@@ -7120,7 +7120,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>11</v>
@@ -7128,16 +7128,16 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>10</v>
@@ -7152,7 +7152,7 @@
         <v>4</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>11</v>
@@ -7169,7 +7169,7 @@
         <v>61</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>62</v>
@@ -7204,7 +7204,7 @@
         <v>65</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>66</v>
@@ -7219,7 +7219,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>329</v>
+        <v>416</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>11</v>
@@ -7227,16 +7227,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>4</v>
@@ -7248,7 +7248,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>11</v>
@@ -7265,7 +7265,7 @@
         <v>84</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>10</v>
@@ -7280,7 +7280,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>11</v>
@@ -7297,13 +7297,13 @@
         <v>86</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>10</v>
@@ -7318,19 +7318,19 @@
         <v>3</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R20" s="12">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7344,7 +7344,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>89</v>
@@ -7359,10 +7359,10 @@
         <v>4</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>11</v>
@@ -7370,19 +7370,19 @@
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>406</v>
+        <v>272</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>93</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>3</v>
@@ -7391,24 +7391,27 @@
         <v>3</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="R22" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23" s="12" t="s">
         <v>4</v>
@@ -7431,10 +7434,10 @@
         <v>92</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>10</v>
@@ -7449,7 +7452,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>11</v>
@@ -7457,74 +7460,74 @@
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>91</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>14</v>
       </c>
       <c r="H25" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="K25" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>380</v>
       </c>
       <c r="L25" s="13"/>
       <c r="Q25" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R25" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>91</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="K26" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>380</v>
       </c>
       <c r="L26" s="13"/>
       <c r="Q26" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R26" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7538,13 +7541,13 @@
         <v>96</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>10</v>
@@ -7553,19 +7556,16 @@
         <v>3</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O27" s="12" t="s">
-        <v>336</v>
+        <v>4</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>347</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="R27" s="12">
-        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7579,13 +7579,13 @@
         <v>98</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>99</v>
@@ -7600,22 +7600,16 @@
         <v>3</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>281</v>
+        <v>326</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R28" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7653,19 +7647,13 @@
         <v>123</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="M29" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="O29" s="12" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R29" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7679,13 +7667,13 @@
         <v>106</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>10</v>
@@ -7700,7 +7688,7 @@
         <v>3</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>11</v>
@@ -7711,57 +7699,51 @@
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>373</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="R31" s="12">
-        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>3</v>
@@ -7773,7 +7755,7 @@
         <v>4</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>11</v>
@@ -7781,16 +7763,16 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>3</v>
@@ -7802,7 +7784,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>343</v>
+        <v>414</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>11</v>
@@ -7810,10 +7792,10 @@
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>4</v>
@@ -7827,10 +7809,10 @@
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>4</v>
@@ -7844,10 +7826,10 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>4</v>
@@ -7884,21 +7866,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -7906,10 +7888,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -7917,10 +7899,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -7928,10 +7910,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -7939,10 +7921,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -7950,10 +7932,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -7961,10 +7943,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -7972,10 +7954,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -7983,10 +7965,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -7994,10 +7976,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -8005,10 +7987,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -8037,58 +8019,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B7" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -8103,7 +8085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8174,13 +8156,13 @@
         <v>128</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>114</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>115</v>
@@ -8189,7 +8171,7 @@
         <v>158</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -8203,7 +8185,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -8218,7 +8200,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -8229,16 +8211,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -8253,7 +8235,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -8264,16 +8246,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -8287,7 +8269,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8297,16 +8279,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
@@ -8320,7 +8302,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="16"/>
       <c r="P5" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>3</v>
@@ -8330,13 +8312,13 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>4</v>
@@ -8345,7 +8327,7 @@
         <v>4</v>
       </c>
       <c r="O6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>3</v>
@@ -8353,13 +8335,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>4</v>
@@ -8369,7 +8351,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="12" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -8377,13 +8359,13 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>4</v>
@@ -8393,7 +8375,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8401,13 +8383,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>4</v>
@@ -8417,7 +8399,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="12" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>
@@ -8425,18 +8407,18 @@
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -8452,26 +8434,26 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="4" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -8485,7 +8467,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="P11" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -8495,14 +8477,14 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>4</v>
@@ -8511,21 +8493,21 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>4</v>
@@ -8540,16 +8522,16 @@
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>4</v>
@@ -8564,10 +8546,10 @@
     </row>
     <row r="15" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -8578,10 +8560,10 @@
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
added icons in repo, changed xlsx table schema
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -17,12 +17,15 @@
     <sheet name="Tables" sheetId="10" r:id="rId8"/>
     <sheet name="MessageConfig" sheetId="15" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">SummarizedInformation!$A$2:$E$16</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="422">
   <si>
     <t>Type</t>
   </si>
@@ -1282,6 +1285,12 @@
   </si>
   <si>
     <t>RELATION{SummarizedInformation,progId.label}|.RELATION{CasesInformation,sampId.label}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,source.code}</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1447,6 +1456,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2893,8 +2903,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S36" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S37" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:S37"/>
   <sortState ref="A2:S36">
     <sortCondition ref="R1:R36"/>
   </sortState>
@@ -2926,8 +2936,8 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2512" displayName="Table2512" ref="A1:S20" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A1:S20"/>
-  <sortState ref="A2:S19">
-    <sortCondition ref="R1:R19"/>
+  <sortState ref="A2:S20">
+    <sortCondition ref="R1:R20"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="58"/>
@@ -4498,13 +4508,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,66 +4599,63 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>3</v>
+        <v>156</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>348</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>357</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R2" s="12">
-        <v>2</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>3</v>
@@ -4660,22 +4667,16 @@
         <v>3</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R3" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3" s="12" t="s">
         <v>11</v>
@@ -4683,22 +4684,22 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
@@ -4710,16 +4711,22 @@
         <v>3</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>348</v>
       </c>
+      <c r="M4" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>129</v>
+      </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>11</v>
@@ -4727,22 +4734,22 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>3</v>
@@ -4754,7 +4761,7 @@
         <v>3</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>348</v>
@@ -4763,7 +4770,7 @@
         <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>11</v>
@@ -4771,28 +4778,25 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>417</v>
+        <v>3</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>3</v>
@@ -4801,16 +4805,16 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>348</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>351</v>
+        <v>5</v>
       </c>
       <c r="R6" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S6" s="12" t="s">
         <v>11</v>
@@ -4818,78 +4822,57 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>333</v>
+        <v>108</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>277</v>
+        <v>4</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>421</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="R7" s="12">
-        <v>7</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>336</v>
+        <v>42</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>337</v>
+        <v>43</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>3</v>
+        <v>417</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>3</v>
@@ -4898,42 +4881,42 @@
         <v>3</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="M8" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>343</v>
-      </c>
       <c r="Q8" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="R8" s="12">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>97</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>27</v>
+        <v>334</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>28</v>
+        <v>333</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>254</v>
+        <v>14</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>3</v>
@@ -4944,34 +4927,46 @@
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O9" s="12">
-        <v>0</v>
+      <c r="K9" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>277</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="R9" s="12">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>17</v>
+        <v>101</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>30</v>
+        <v>336</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>31</v>
+        <v>337</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>254</v>
+        <v>14</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>3</v>
@@ -4982,28 +4977,37 @@
       <c r="J10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="12">
-        <v>0</v>
+      <c r="K10" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>343</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="R10" s="12">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>254</v>
@@ -5027,21 +5031,21 @@
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>254</v>
@@ -5053,33 +5057,33 @@
         <v>3</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P12" s="12" t="s">
-        <v>342</v>
+      <c r="O12" s="12">
+        <v>0</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>254</v>
@@ -5103,27 +5107,24 @@
         <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>188</v>
+        <v>254</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>10</v>
@@ -5137,72 +5138,75 @@
       <c r="J14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="12" t="s">
-        <v>365</v>
+      <c r="P14" s="12" t="s">
+        <v>342</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="R14" s="12">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>148</v>
+        <v>35</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="12">
         <v>0</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="O15" s="12" t="s">
-        <v>357</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R15" s="12">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>3</v>
@@ -5211,33 +5215,33 @@
         <v>4</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>16</v>
+        <v>365</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>11</v>
+      </c>
+      <c r="R16" s="12">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>3</v>
@@ -5248,8 +5252,11 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P17" s="12" t="s">
-        <v>341</v>
+      <c r="M17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>11</v>
@@ -5257,13 +5264,13 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>188</v>
@@ -5272,7 +5279,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>350</v>
+        <v>3</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -5281,21 +5288,21 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>350</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>188</v>
@@ -5304,7 +5311,7 @@
         <v>10</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>3</v>
+        <v>350</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -5313,27 +5320,27 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>3</v>
@@ -5344,11 +5351,8 @@
       <c r="J20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="12" t="s">
-        <v>235</v>
-      </c>
       <c r="P20" s="12" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>11</v>
@@ -5356,13 +5360,13 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>188</v>
@@ -5391,19 +5395,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>3</v>
@@ -5415,10 +5419,10 @@
         <v>4</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>317</v>
+        <v>235</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>11</v>
@@ -5426,13 +5430,13 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>254</v>
@@ -5449,8 +5453,11 @@
       <c r="J23" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N23" s="12" t="s">
+        <v>317</v>
+      </c>
       <c r="P23" s="12" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>11</v>
@@ -5458,13 +5465,13 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>254</v>
@@ -5481,11 +5488,8 @@
       <c r="J24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N24" s="12" t="s">
-        <v>318</v>
-      </c>
       <c r="P24" s="12" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>11</v>
@@ -5493,19 +5497,19 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>188</v>
+        <v>254</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>3</v>
@@ -5516,11 +5520,11 @@
       <c r="J25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M25" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="O25" s="12" t="s">
-        <v>63</v>
+      <c r="N25" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="P25" s="12" t="s">
+        <v>321</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>11</v>
@@ -5528,19 +5532,19 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>3</v>
@@ -5551,8 +5555,11 @@
       <c r="J26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P26" s="12" t="s">
-        <v>368</v>
+      <c r="M26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>11</v>
@@ -5560,19 +5567,19 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>3</v>
@@ -5584,7 +5591,7 @@
         <v>4</v>
       </c>
       <c r="P27" s="12" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>11</v>
@@ -5592,16 +5599,16 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>10</v>
@@ -5616,7 +5623,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>11</v>
@@ -5624,19 +5631,19 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>188</v>
+        <v>254</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>3</v>
@@ -5647,11 +5654,8 @@
       <c r="J29" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M29" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="O29" s="12" t="s">
-        <v>90</v>
+      <c r="P29" s="12" t="s">
+        <v>340</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>11</v>
@@ -5659,19 +5663,19 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>3</v>
@@ -5683,10 +5687,10 @@
         <v>4</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>11</v>
@@ -5694,19 +5698,19 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>3</v>
@@ -5717,8 +5721,11 @@
       <c r="J31" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P31" s="12" t="s">
-        <v>347</v>
+      <c r="M31" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>11</v>
@@ -5726,13 +5733,13 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>188</v>
@@ -5749,8 +5756,8 @@
       <c r="J32" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O32" s="12" t="s">
-        <v>352</v>
+      <c r="P32" s="12" t="s">
+        <v>347</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>11</v>
@@ -5758,10 +5765,22 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>186</v>
+        <v>106</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>4</v>
@@ -5769,13 +5788,16 @@
       <c r="J33" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="O33" s="12" t="s">
+        <v>352</v>
+      </c>
       <c r="Q33" s="12" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>187</v>
@@ -5792,7 +5814,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>187</v>
@@ -5809,31 +5831,49 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q36" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E37" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F37" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="I36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="O36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="12" t="s">
+      <c r="I37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="12" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5843,10 +5883,10 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5972,24 +6012,24 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>73</v>
+        <v>214</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="28" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="12" t="s">
@@ -5997,18 +6037,6 @@
       </c>
       <c r="J3" s="12" t="s">
         <v>3</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -6016,37 +6044,46 @@
       <c r="R3" s="12">
         <v>2</v>
       </c>
-      <c r="S3" s="12" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" t="s">
-        <v>205</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>206</v>
+        <v>72</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>207</v>
+        <v>73</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>188</v>
+        <v>14</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>369</v>
-      </c>
-      <c r="I4" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>3</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>127</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -6060,16 +6097,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>45</v>
+        <v>204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>205</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>188</v>
@@ -6077,10 +6114,10 @@
       <c r="G5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="I5" s="29" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
@@ -6092,40 +6129,37 @@
       <c r="R5" s="12">
         <v>4</v>
       </c>
+      <c r="S5" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
+        <v>215</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>216</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>211</v>
+        <v>10</v>
       </c>
       <c r="H6" s="29" t="s">
         <v>369</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>3</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>313</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -6136,16 +6170,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>216</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>188</v>
@@ -6153,8 +6187,8 @@
       <c r="G7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="29" t="s">
-        <v>369</v>
+      <c r="H7" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
@@ -6162,6 +6196,7 @@
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="K7" s="23"/>
       <c r="Q7" s="12" t="s">
         <v>5</v>
       </c>
@@ -6171,16 +6206,16 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>219</v>
+        <v>296</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>216</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>220</v>
+        <v>297</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>221</v>
+        <v>298</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>188</v>
@@ -6207,22 +6242,19 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>216</v>
+        <v>294</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>10</v>
+        <v>309</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>4</v>
@@ -6232,6 +6264,9 @@
       </c>
       <c r="J9" s="12" t="s">
         <v>3</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>327</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -6242,22 +6277,22 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>40</v>
+        <v>230</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>49</v>
+        <v>233</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>369</v>
@@ -6268,11 +6303,12 @@
       <c r="J10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="O10"/>
-      <c r="P10"/>
+      <c r="K10" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>235</v>
+      </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
       </c>
@@ -6282,34 +6318,37 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>40</v>
+        <v>208</v>
+      </c>
+      <c r="B11" t="s">
+        <v>205</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>338</v>
+        <v>209</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>339</v>
+        <v>210</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>300</v>
+      <c r="H11" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>313</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -6320,35 +6359,37 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>301</v>
+        <v>222</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>302</v>
+        <v>223</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="F12" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>304</v>
+      <c r="G12" s="23" t="s">
+        <v>49</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>370</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="23" t="s">
         <v>3</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>172</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="O12"/>
+      <c r="P12"/>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
@@ -6358,32 +6399,34 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="26"/>
+      <c r="G13" s="11" t="s">
+        <v>304</v>
+      </c>
       <c r="H13" s="29" t="s">
         <v>370</v>
       </c>
-      <c r="I13" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>173</v>
+      <c r="I13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>172</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6394,37 +6437,32 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>230</v>
+        <v>40</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="F14" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="23" t="s">
-        <v>233</v>
-      </c>
+      <c r="G14" s="26"/>
       <c r="H14" s="29" t="s">
-        <v>369</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>235</v>
+        <v>370</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>173</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -6435,20 +6473,23 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>294</v>
+        <v>40</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>14</v>
       </c>
+      <c r="G15" s="12" t="s">
+        <v>211</v>
+      </c>
       <c r="H15" s="12" t="s">
         <v>4</v>
       </c>
@@ -6458,8 +6499,8 @@
       <c r="J15" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="12" t="s">
-        <v>327</v>
+      <c r="K15" s="26" t="s">
+        <v>300</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
@@ -6609,10 +6650,10 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7486,7 +7527,9 @@
       <c r="K25" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="L25" s="13"/>
+      <c r="L25" s="13" t="s">
+        <v>420</v>
+      </c>
       <c r="Q25" s="12" t="s">
         <v>5</v>
       </c>
@@ -7522,7 +7565,9 @@
       <c r="K26" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="L26" s="13"/>
+      <c r="L26" s="13" t="s">
+        <v>420</v>
+      </c>
       <c r="Q26" s="12" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Fixed errors in test case of 1.0.7
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -387,9 +387,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Brain</t>
-  </si>
-  <si>
     <t>defaultCode</t>
   </si>
   <si>
@@ -990,9 +987,6 @@
     <t>RELATION{Report,reportDatasetId.label}</t>
   </si>
   <si>
-    <t>tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code}</t>
-  </si>
-  <si>
     <t>dcTable</t>
   </si>
   <si>
@@ -1026,9 +1020,6 @@
     <t>RELATION{SummarizedInformation,progId.label}</t>
   </si>
   <si>
-    <t>F02.A06AM</t>
-  </si>
-  <si>
     <t>F21.A07RV</t>
   </si>
   <si>
@@ -1059,9 +1050,6 @@
     <t>RESEVAL</t>
   </si>
   <si>
-    <t>A04MQ#%source.code$%prod.code$%animage.code</t>
-  </si>
-  <si>
     <t>paramCodeBaseTerm</t>
   </si>
   <si>
@@ -1188,9 +1176,6 @@
     <t>CWD$AT12A</t>
   </si>
   <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|sampAnAsses=RELATION{CasesInformation,sampAnAsses.code}|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
-  </si>
-  <si>
     <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)</t>
   </si>
   <si>
@@ -1245,9 +1230,6 @@
     <t>(%type.code!=RGT)</t>
   </si>
   <si>
-    <t>tseTargetGroup=%tseTargetGroup.code|IF((%type.code!=RGT),$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,)</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation,progId.label}|.IF_NOT_NULL(RELATION{CasesInformation,animalId.label},A.|RELATION{CasesInformation,animalId.label},S.|RELATION{CasesInformation,sampId.label})</t>
   </si>
   <si>
@@ -1264,6 +1246,24 @@
   </si>
   <si>
     <t>((%anMethType.code==AT13A)AND(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
+  </si>
+  <si>
+    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampAnAsses.code},sampAnAsses=RELATION{CasesInformation,sampAnAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),F02.A06AM,F02.A06AL)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),Brain,Blood)</t>
   </si>
 </sst>
 </file>
@@ -1282,6 +1282,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3373,49 +3374,49 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>10</v>
@@ -3440,23 +3441,23 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>10</v>
@@ -3481,23 +3482,23 @@
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H4" s="17" t="s">
         <v>10</v>
@@ -3592,42 +3593,42 @@
         <v>109</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
@@ -3645,7 +3646,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L2" s="9"/>
       <c r="R2">
@@ -3654,17 +3655,17 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -3685,7 +3686,7 @@
         <v>116</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3693,17 +3694,17 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>13</v>
@@ -3724,7 +3725,7 @@
         <v>116</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3732,17 +3733,17 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
@@ -3763,7 +3764,7 @@
         <v>116</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3771,17 +3772,17 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
@@ -3802,7 +3803,7 @@
         <v>116</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3810,17 +3811,17 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>13</v>
@@ -3841,7 +3842,7 @@
         <v>116</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3849,17 +3850,17 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>13</v>
@@ -3880,7 +3881,7 @@
         <v>116</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3888,17 +3889,17 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>13</v>
@@ -3919,7 +3920,7 @@
         <v>116</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -3927,17 +3928,17 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>13</v>
@@ -3958,7 +3959,7 @@
         <v>116</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -3966,17 +3967,17 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>13</v>
@@ -3997,7 +3998,7 @@
         <v>116</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
@@ -4084,49 +4085,49 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>10</v>
@@ -4138,15 +4139,15 @@
         <v>10</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -4161,23 +4162,23 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>10</v>
@@ -4189,15 +4190,15 @@
         <v>10</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -4212,18 +4213,18 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -4240,10 +4241,10 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4257,17 +4258,17 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>124</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>125</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>13</v>
@@ -4285,15 +4286,15 @@
         <v>10</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16" t="s">
@@ -4308,10 +4309,10 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>5</v>
@@ -4331,16 +4332,16 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>5</v>
@@ -4361,18 +4362,18 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23" t="s">
@@ -4400,18 +4401,18 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>256</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>257</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23" t="s">
@@ -4439,18 +4440,18 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>251</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>252</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23" t="s">
@@ -4552,28 +4553,28 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4581,7 +4582,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>0</v>
@@ -4590,25 +4591,25 @@
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>150</v>
-      </c>
       <c r="M2" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4649,7 +4650,7 @@
         <v>112</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4669,7 +4670,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>72</v>
@@ -4693,13 +4694,13 @@
         <v>114</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -4731,10 +4732,10 @@
         <v>77</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>3</v>
@@ -4743,7 +4744,7 @@
         <v>115</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -4775,10 +4776,10 @@
         <v>21</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>3</v>
@@ -4787,7 +4788,7 @@
         <v>110</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -4813,22 +4814,22 @@
         <v>26</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -4848,25 +4849,25 @@
         <v>28</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -4889,22 +4890,22 @@
         <v>31</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -4924,16 +4925,16 @@
         <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>4</v>
@@ -4942,7 +4943,7 @@
         <v>3</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -4965,22 +4966,22 @@
         <v>34</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -5003,7 +5004,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>9</v>
@@ -5018,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>10</v>
@@ -5038,7 +5039,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>14</v>
@@ -5073,7 +5074,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>9</v>
@@ -5088,7 +5089,7 @@
         <v>4</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>10</v>
@@ -5105,7 +5106,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>9</v>
@@ -5120,7 +5121,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>10</v>
@@ -5137,7 +5138,7 @@
         <v>44</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>45</v>
@@ -5152,10 +5153,10 @@
         <v>4</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>10</v>
@@ -5172,7 +5173,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>45</v>
@@ -5187,10 +5188,10 @@
         <v>4</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>10</v>
@@ -5207,7 +5208,7 @@
         <v>49</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>9</v>
@@ -5222,10 +5223,10 @@
         <v>4</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>10</v>
@@ -5242,7 +5243,7 @@
         <v>51</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>9</v>
@@ -5257,7 +5258,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>10</v>
@@ -5274,7 +5275,7 @@
         <v>54</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>9</v>
@@ -5289,10 +5290,10 @@
         <v>4</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>10</v>
@@ -5309,7 +5310,7 @@
         <v>57</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>58</v>
@@ -5344,7 +5345,7 @@
         <v>61</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>62</v>
@@ -5359,7 +5360,7 @@
         <v>4</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>344</v>
+        <v>407</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>10</v>
@@ -5376,7 +5377,7 @@
         <v>79</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>9</v>
@@ -5391,7 +5392,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>10</v>
@@ -5408,7 +5409,7 @@
         <v>81</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>9</v>
@@ -5423,7 +5424,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>10</v>
@@ -5440,7 +5441,7 @@
         <v>83</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>84</v>
@@ -5475,7 +5476,7 @@
         <v>87</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>88</v>
@@ -5510,7 +5511,7 @@
         <v>99</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>9</v>
@@ -5525,7 +5526,7 @@
         <v>4</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>10</v>
@@ -5533,10 +5534,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>180</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>4</v>
@@ -5550,10 +5551,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>4</v>
@@ -5567,10 +5568,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>4</v>
@@ -5584,13 +5585,13 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>4</v>
@@ -5619,10 +5620,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23:A44"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5681,63 +5682,63 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="B2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>219</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>220</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -5754,13 +5755,13 @@
         <v>41</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>207</v>
-      </c>
       <c r="F3" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>9</v>
@@ -5813,13 +5814,13 @@
         <v>113</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>333</v>
+        <v>411</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>120</v>
+        <v>412</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -5833,31 +5834,31 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
         <v>197</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>200</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -5871,25 +5872,25 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>211</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>3</v>
@@ -5906,19 +5907,19 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>214</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>9</v>
@@ -5942,19 +5943,19 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>290</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
@@ -5978,16 +5979,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>286</v>
-      </c>
       <c r="D9" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>300</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>301</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>13</v>
@@ -6002,7 +6003,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -6013,37 +6014,37 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>225</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>403</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>409</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>227</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>228</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -6054,37 +6055,37 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B11" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>202</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>203</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>403</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>409</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>408</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>205</v>
-      </c>
       <c r="L11" s="12" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -6095,16 +6096,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>216</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>217</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>13</v>
@@ -6113,7 +6114,7 @@
         <v>45</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>3</v>
@@ -6122,7 +6123,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O12"/>
       <c r="P12"/>
@@ -6135,25 +6136,25 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>294</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>295</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>3</v>
@@ -6162,7 +6163,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6173,23 +6174,23 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>298</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>299</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="12" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="I14" s="26" t="s">
         <v>3</v>
@@ -6198,7 +6199,7 @@
         <v>3</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -6209,22 +6210,22 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>4</v>
@@ -6236,7 +6237,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
@@ -6247,19 +6248,19 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>304</v>
-      </c>
       <c r="F16" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>9</v>
@@ -6282,19 +6283,19 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>307</v>
-      </c>
       <c r="F17" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>9</v>
@@ -6317,10 +6318,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -6334,10 +6335,10 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>180</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -6351,13 +6352,13 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>4</v>
@@ -6380,7 +6381,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>39</v>
@@ -6392,19 +6393,19 @@
         <v>40</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="K21" s="12" t="s">
         <v>111</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>5</v>
@@ -6430,10 +6431,10 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6492,25 +6493,25 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6524,7 +6525,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>9</v>
@@ -6539,7 +6540,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>10</v>
@@ -6556,7 +6557,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>14</v>
@@ -6591,7 +6592,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>9</v>
@@ -6606,7 +6607,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>321</v>
+        <v>409</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>10</v>
@@ -6623,7 +6624,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>9</v>
@@ -6638,7 +6639,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>10</v>
@@ -6646,16 +6647,16 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>9</v>
@@ -6670,7 +6671,7 @@
         <v>4</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>10</v>
@@ -6687,7 +6688,7 @@
         <v>101</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>3</v>
@@ -6699,7 +6700,7 @@
         <v>4</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>10</v>
@@ -6716,13 +6717,13 @@
         <v>42</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>207</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
@@ -6737,7 +6738,7 @@
         <v>4</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>10</v>
@@ -6754,7 +6755,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>45</v>
@@ -6769,7 +6770,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>10</v>
@@ -6786,7 +6787,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>45</v>
@@ -6801,7 +6802,7 @@
         <v>4</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>10</v>
@@ -6809,43 +6810,43 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>225</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="L11" s="12" t="s">
-        <v>228</v>
-      </c>
       <c r="N11" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>10</v>
@@ -6862,7 +6863,7 @@
         <v>49</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>9</v>
@@ -6877,7 +6878,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>10</v>
@@ -6894,7 +6895,7 @@
         <v>51</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>9</v>
@@ -6909,7 +6910,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>10</v>
@@ -6926,7 +6927,7 @@
         <v>54</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>9</v>
@@ -6941,7 +6942,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>10</v>
@@ -6949,16 +6950,16 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>286</v>
-      </c>
       <c r="C15" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>9</v>
@@ -6973,7 +6974,7 @@
         <v>4</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>10</v>
@@ -6990,7 +6991,7 @@
         <v>57</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>58</v>
@@ -7025,7 +7026,7 @@
         <v>61</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>62</v>
@@ -7040,7 +7041,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>10</v>
@@ -7048,16 +7049,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>283</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>4</v>
@@ -7069,7 +7070,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>10</v>
@@ -7086,7 +7087,7 @@
         <v>79</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>9</v>
@@ -7101,7 +7102,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>10</v>
@@ -7118,13 +7119,13 @@
         <v>99</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>9</v>
@@ -7139,7 +7140,7 @@
         <v>3</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>10</v>
@@ -7159,7 +7160,7 @@
         <v>83</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>84</v>
@@ -7174,10 +7175,10 @@
         <v>4</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>10</v>
@@ -7194,13 +7195,13 @@
         <v>93</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>94</v>
@@ -7215,10 +7216,10 @@
         <v>3</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>10</v>
@@ -7229,10 +7230,10 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>3</v>
@@ -7244,7 +7245,7 @@
         <v>4</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>5</v>
@@ -7261,10 +7262,10 @@
         <v>87</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>9</v>
@@ -7279,7 +7280,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>10</v>
@@ -7296,10 +7297,10 @@
         <v>96</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>13</v>
@@ -7320,7 +7321,7 @@
         <v>116</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>10</v>
@@ -7331,19 +7332,19 @@
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>88</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="I26" s="12" t="s">
         <v>3</v>
@@ -7352,10 +7353,10 @@
         <v>3</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>5</v>
@@ -7375,13 +7376,13 @@
         <v>91</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>9</v>
@@ -7396,7 +7397,7 @@
         <v>4</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>10</v>
@@ -7413,13 +7414,13 @@
         <v>81</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>9</v>
@@ -7434,13 +7435,13 @@
         <v>3</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>10</v>
@@ -7451,34 +7452,34 @@
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>5</v>
@@ -7489,34 +7490,34 @@
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>5</v>
@@ -7527,22 +7528,22 @@
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>267</v>
-      </c>
       <c r="C31" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>3</v>
@@ -7554,7 +7555,7 @@
         <v>4</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>10</v>
@@ -7562,16 +7563,16 @@
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>262</v>
-      </c>
       <c r="C32" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>3</v>
@@ -7583,7 +7584,7 @@
         <v>4</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>10</v>
@@ -7591,16 +7592,16 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>3</v>
@@ -7612,7 +7613,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>387</v>
+        <v>408</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>10</v>
@@ -7620,10 +7621,10 @@
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>4</v>
@@ -7637,10 +7638,10 @@
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>4</v>
@@ -7654,10 +7655,10 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>180</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>4</v>
@@ -7694,21 +7695,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" t="s">
-        <v>176</v>
-      </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -7716,10 +7717,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -7727,10 +7728,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -7738,10 +7739,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -7749,10 +7750,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
         <v>177</v>
-      </c>
-      <c r="B6" t="s">
-        <v>178</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -7760,10 +7761,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -7771,10 +7772,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -7782,10 +7783,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -7793,10 +7794,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -7804,10 +7805,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -7815,10 +7816,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -7847,58 +7848,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -7978,28 +7979,28 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -8013,7 +8014,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -8028,7 +8029,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -8039,16 +8040,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -8063,7 +8064,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -8074,16 +8075,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -8097,7 +8098,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8107,16 +8108,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
@@ -8130,7 +8131,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="16"/>
       <c r="P5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>3</v>
@@ -8140,22 +8141,22 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
         <v>243</v>
-      </c>
-      <c r="C6" t="s">
-        <v>243</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O6" t="s">
-        <v>244</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>3</v>
@@ -8163,13 +8164,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>4</v>
@@ -8179,7 +8180,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -8187,13 +8188,13 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>4</v>
@@ -8203,7 +8204,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8211,13 +8212,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>4</v>
@@ -8227,7 +8228,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>
@@ -8235,18 +8236,18 @@
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -8262,26 +8263,26 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -8295,7 +8296,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="P11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -8305,14 +8306,14 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>4</v>
@@ -8321,21 +8322,21 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>4</v>
@@ -8350,16 +8351,16 @@
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>4</v>
@@ -8374,10 +8375,10 @@
     </row>
     <row r="15" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>180</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -8388,10 +8389,10 @@
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Test result column in analytical results is now hidden for RGT
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -5619,11 +5619,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6430,11 +6430,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7350,7 +7350,7 @@
         <v>3</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>3</v>
+        <v>402</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>360</v>

</xml_diff>

<commit_message>
Added default species (sheep) for RGT
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="412">
   <si>
     <t>Type</t>
   </si>
@@ -390,9 +390,6 @@
     <t>defaultCode</t>
   </si>
   <si>
-    <t>Farmed</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -1023,9 +1020,6 @@
     <t>F21.A07RV</t>
   </si>
   <si>
-    <t>%type.label</t>
-  </si>
-  <si>
     <t>opType</t>
   </si>
   <si>
@@ -1264,6 +1258,9 @@
   </si>
   <si>
     <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),Brain,Blood)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),F01.A057G,)</t>
   </si>
 </sst>
 </file>
@@ -3374,49 +3371,49 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>10</v>
@@ -3441,23 +3438,23 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>10</v>
@@ -3482,23 +3479,23 @@
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H4" s="17" t="s">
         <v>10</v>
@@ -3593,42 +3590,42 @@
         <v>109</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
@@ -3646,7 +3643,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L2" s="9"/>
       <c r="R2">
@@ -3655,17 +3652,17 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -3686,7 +3683,7 @@
         <v>116</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3694,17 +3691,17 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>13</v>
@@ -3725,7 +3722,7 @@
         <v>116</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3733,17 +3730,17 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
@@ -3764,7 +3761,7 @@
         <v>116</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3772,17 +3769,17 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
@@ -3803,7 +3800,7 @@
         <v>116</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3811,17 +3808,17 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>13</v>
@@ -3842,7 +3839,7 @@
         <v>116</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3850,17 +3847,17 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>13</v>
@@ -3881,7 +3878,7 @@
         <v>116</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3889,17 +3886,17 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>13</v>
@@ -3920,7 +3917,7 @@
         <v>116</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -3928,17 +3925,17 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>13</v>
@@ -3959,7 +3956,7 @@
         <v>116</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -3967,17 +3964,17 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>13</v>
@@ -3998,7 +3995,7 @@
         <v>116</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
@@ -4085,49 +4082,49 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>10</v>
@@ -4139,15 +4136,15 @@
         <v>10</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -4162,23 +4159,23 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>10</v>
@@ -4190,15 +4187,15 @@
         <v>10</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -4213,18 +4210,18 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -4241,10 +4238,10 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4258,17 +4255,17 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>123</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>124</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>13</v>
@@ -4286,15 +4283,15 @@
         <v>10</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16" t="s">
@@ -4309,10 +4306,10 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>5</v>
@@ -4332,16 +4329,16 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>5</v>
@@ -4362,18 +4359,18 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23" t="s">
@@ -4401,18 +4398,18 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>255</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>256</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23" t="s">
@@ -4440,18 +4437,18 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>250</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>251</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23" t="s">
@@ -4490,11 +4487,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4553,28 +4550,28 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4582,7 +4579,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>0</v>
@@ -4591,25 +4588,22 @@
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="M2" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4650,7 +4644,10 @@
         <v>112</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>411</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4670,7 +4667,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>72</v>
@@ -4694,13 +4691,10 @@
         <v>114</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>121</v>
+        <v>330</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -4732,10 +4726,10 @@
         <v>77</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>3</v>
@@ -4744,7 +4738,7 @@
         <v>115</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -4776,10 +4770,10 @@
         <v>21</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>3</v>
@@ -4788,7 +4782,7 @@
         <v>110</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -4814,22 +4808,22 @@
         <v>26</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -4849,25 +4843,25 @@
         <v>28</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -4890,22 +4884,22 @@
         <v>31</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -4925,16 +4919,16 @@
         <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>4</v>
@@ -4943,7 +4937,7 @@
         <v>3</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -4966,22 +4960,22 @@
         <v>34</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -5004,7 +4998,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>9</v>
@@ -5019,7 +5013,7 @@
         <v>3</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>10</v>
@@ -5039,7 +5033,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>14</v>
@@ -5074,7 +5068,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>9</v>
@@ -5089,7 +5083,7 @@
         <v>4</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>10</v>
@@ -5106,7 +5100,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>9</v>
@@ -5121,7 +5115,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>10</v>
@@ -5138,7 +5132,7 @@
         <v>44</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>45</v>
@@ -5153,10 +5147,10 @@
         <v>4</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>10</v>
@@ -5173,7 +5167,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>45</v>
@@ -5188,10 +5182,10 @@
         <v>4</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>10</v>
@@ -5208,7 +5202,7 @@
         <v>49</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>9</v>
@@ -5223,10 +5217,10 @@
         <v>4</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>10</v>
@@ -5243,7 +5237,7 @@
         <v>51</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>9</v>
@@ -5258,7 +5252,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>10</v>
@@ -5275,7 +5269,7 @@
         <v>54</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>9</v>
@@ -5290,10 +5284,10 @@
         <v>4</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>10</v>
@@ -5310,7 +5304,7 @@
         <v>57</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>58</v>
@@ -5345,7 +5339,7 @@
         <v>61</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>62</v>
@@ -5360,7 +5354,7 @@
         <v>4</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>10</v>
@@ -5377,7 +5371,7 @@
         <v>79</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>9</v>
@@ -5392,7 +5386,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>10</v>
@@ -5409,7 +5403,7 @@
         <v>81</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>9</v>
@@ -5424,7 +5418,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>10</v>
@@ -5441,7 +5435,7 @@
         <v>83</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>84</v>
@@ -5476,7 +5470,7 @@
         <v>87</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>88</v>
@@ -5511,7 +5505,7 @@
         <v>99</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>9</v>
@@ -5526,7 +5520,7 @@
         <v>4</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>10</v>
@@ -5534,10 +5528,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>178</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>179</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>4</v>
@@ -5551,10 +5545,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>4</v>
@@ -5568,10 +5562,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>4</v>
@@ -5585,13 +5579,13 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>4</v>
@@ -5682,63 +5676,63 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>218</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>219</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -5755,13 +5749,13 @@
         <v>41</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>206</v>
-      </c>
       <c r="F3" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>9</v>
@@ -5814,13 +5808,13 @@
         <v>113</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -5834,31 +5828,31 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" t="s">
         <v>196</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>199</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -5872,25 +5866,25 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>210</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>3</v>
@@ -5907,19 +5901,19 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>213</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>9</v>
@@ -5943,19 +5937,19 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>289</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
@@ -5979,16 +5973,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>285</v>
-      </c>
       <c r="D9" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>299</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>300</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>13</v>
@@ -6003,7 +5997,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -6014,37 +6008,37 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>223</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>224</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>403</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>226</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>227</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -6055,37 +6049,37 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B11" t="s">
-        <v>197</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>201</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>202</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>403</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>402</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>204</v>
-      </c>
       <c r="L11" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -6096,16 +6090,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>215</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>216</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>13</v>
@@ -6114,7 +6108,7 @@
         <v>45</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>3</v>
@@ -6123,7 +6117,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O12"/>
       <c r="P12"/>
@@ -6136,25 +6130,25 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>293</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>294</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>3</v>
@@ -6163,7 +6157,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6174,23 +6168,23 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>297</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>298</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I14" s="26" t="s">
         <v>3</v>
@@ -6199,7 +6193,7 @@
         <v>3</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -6210,22 +6204,22 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>4</v>
@@ -6237,7 +6231,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
@@ -6248,19 +6242,19 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>303</v>
-      </c>
       <c r="F16" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>9</v>
@@ -6283,19 +6277,19 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>306</v>
-      </c>
       <c r="F17" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>9</v>
@@ -6318,10 +6312,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -6335,10 +6329,10 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>178</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>179</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -6352,13 +6346,13 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>4</v>
@@ -6381,7 +6375,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>39</v>
@@ -6393,19 +6387,19 @@
         <v>40</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K21" s="12" t="s">
         <v>111</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>5</v>
@@ -6430,11 +6424,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6493,25 +6487,25 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6525,7 +6519,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>9</v>
@@ -6540,7 +6534,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>10</v>
@@ -6557,7 +6551,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>14</v>
@@ -6592,7 +6586,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>9</v>
@@ -6607,7 +6601,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>10</v>
@@ -6624,7 +6618,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>9</v>
@@ -6639,7 +6633,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>10</v>
@@ -6647,16 +6641,16 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>9</v>
@@ -6671,7 +6665,7 @@
         <v>4</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>10</v>
@@ -6688,7 +6682,7 @@
         <v>101</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>3</v>
@@ -6700,7 +6694,7 @@
         <v>4</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>10</v>
@@ -6717,13 +6711,13 @@
         <v>42</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>206</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
@@ -6738,7 +6732,7 @@
         <v>4</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>10</v>
@@ -6755,7 +6749,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>45</v>
@@ -6770,7 +6764,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>10</v>
@@ -6787,7 +6781,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>45</v>
@@ -6802,7 +6796,7 @@
         <v>4</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>10</v>
@@ -6810,43 +6804,43 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>223</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>224</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="L11" s="12" t="s">
-        <v>227</v>
-      </c>
       <c r="N11" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>10</v>
@@ -6863,7 +6857,7 @@
         <v>49</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>9</v>
@@ -6878,7 +6872,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>10</v>
@@ -6895,7 +6889,7 @@
         <v>51</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>9</v>
@@ -6910,7 +6904,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>10</v>
@@ -6927,7 +6921,7 @@
         <v>54</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>9</v>
@@ -6942,7 +6936,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>10</v>
@@ -6950,16 +6944,16 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>285</v>
-      </c>
       <c r="C15" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>9</v>
@@ -6974,7 +6968,7 @@
         <v>4</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>10</v>
@@ -6991,7 +6985,7 @@
         <v>57</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>58</v>
@@ -7026,7 +7020,7 @@
         <v>61</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>62</v>
@@ -7041,7 +7035,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>10</v>
@@ -7049,16 +7043,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>282</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>4</v>
@@ -7070,7 +7064,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>10</v>
@@ -7087,7 +7081,7 @@
         <v>79</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>9</v>
@@ -7102,7 +7096,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>10</v>
@@ -7119,13 +7113,13 @@
         <v>99</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>9</v>
@@ -7140,7 +7134,7 @@
         <v>3</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>10</v>
@@ -7160,7 +7154,7 @@
         <v>83</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>84</v>
@@ -7175,10 +7169,10 @@
         <v>4</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>10</v>
@@ -7195,13 +7189,13 @@
         <v>93</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>94</v>
@@ -7216,10 +7210,10 @@
         <v>3</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>10</v>
@@ -7230,11 +7224,11 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="E23" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="E23" s="28" t="s">
-        <v>343</v>
-      </c>
       <c r="H23" s="12" t="s">
         <v>3</v>
       </c>
@@ -7245,7 +7239,7 @@
         <v>4</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>5</v>
@@ -7262,10 +7256,10 @@
         <v>87</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>9</v>
@@ -7280,7 +7274,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>10</v>
@@ -7297,10 +7291,10 @@
         <v>96</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>13</v>
@@ -7321,7 +7315,7 @@
         <v>116</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>10</v>
@@ -7332,31 +7326,31 @@
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>88</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I26" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K26" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="L26" s="12" t="s">
         <v>360</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>362</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>5</v>
@@ -7376,13 +7370,13 @@
         <v>91</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>9</v>
@@ -7397,7 +7391,7 @@
         <v>4</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>10</v>
@@ -7414,13 +7408,13 @@
         <v>81</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>9</v>
@@ -7435,13 +7429,13 @@
         <v>3</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>10</v>
@@ -7452,34 +7446,34 @@
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>5</v>
@@ -7490,34 +7484,34 @@
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>5</v>
@@ -7528,22 +7522,22 @@
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>266</v>
-      </c>
       <c r="C31" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>3</v>
@@ -7555,7 +7549,7 @@
         <v>4</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>10</v>
@@ -7563,16 +7557,16 @@
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>261</v>
-      </c>
       <c r="C32" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>3</v>
@@ -7584,7 +7578,7 @@
         <v>4</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>10</v>
@@ -7592,16 +7586,16 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>3</v>
@@ -7613,7 +7607,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>10</v>
@@ -7621,10 +7615,10 @@
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>4</v>
@@ -7638,10 +7632,10 @@
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>4</v>
@@ -7655,10 +7649,10 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>178</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>179</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>4</v>
@@ -7695,21 +7689,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
         <v>174</v>
       </c>
-      <c r="B1" t="s">
-        <v>175</v>
-      </c>
       <c r="C1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -7717,10 +7711,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -7728,10 +7722,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -7739,10 +7733,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -7750,10 +7744,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" t="s">
         <v>176</v>
-      </c>
-      <c r="B6" t="s">
-        <v>177</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -7761,10 +7755,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -7772,10 +7766,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -7783,10 +7777,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -7794,10 +7788,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -7805,10 +7799,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -7816,10 +7810,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -7848,58 +7842,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -7979,28 +7973,28 @@
         <v>109</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -8014,7 +8008,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -8029,7 +8023,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -8040,16 +8034,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -8064,7 +8058,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -8075,16 +8069,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -8098,7 +8092,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8108,16 +8102,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
@@ -8131,7 +8125,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="16"/>
       <c r="P5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>3</v>
@@ -8141,22 +8135,22 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
         <v>242</v>
-      </c>
-      <c r="C6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O6" t="s">
-        <v>243</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>3</v>
@@ -8164,13 +8158,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>4</v>
@@ -8180,7 +8174,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -8188,13 +8182,13 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>4</v>
@@ -8204,7 +8198,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8212,13 +8206,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>4</v>
@@ -8228,7 +8222,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>
@@ -8236,18 +8230,18 @@
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -8263,26 +8257,26 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -8296,7 +8290,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="P11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -8306,14 +8300,14 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>4</v>
@@ -8322,21 +8316,21 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>4</v>
@@ -8351,16 +8345,16 @@
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>4</v>
@@ -8375,10 +8369,10 @@
     </row>
     <row r="15" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>178</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>179</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -8389,10 +8383,10 @@
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Now report year and birth year take values from different pick-lists, in order to avoid reports with year 1995...2000
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="413">
   <si>
     <t>Type</t>
   </si>
@@ -516,9 +516,6 @@
     <t>month</t>
   </si>
   <si>
-    <t>yearsList</t>
-  </si>
-  <si>
     <t>monthsList</t>
   </si>
   <si>
@@ -1261,6 +1258,12 @@
   </si>
   <si>
     <t>IF((%type.code!=RGT),F01.A057G,)</t>
+  </si>
+  <si>
+    <t>reportYearsList</t>
+  </si>
+  <si>
+    <t>animalYearsList</t>
   </si>
 </sst>
 </file>
@@ -3377,13 +3380,13 @@
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
@@ -3392,7 +3395,7 @@
         <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3410,7 +3413,7 @@
         <v>142</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>144</v>
@@ -3479,20 +3482,20 @@
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>144</v>
@@ -3596,13 +3599,13 @@
         <v>120</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>108</v>
@@ -3611,7 +3614,7 @@
         <v>149</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3662,7 +3665,7 @@
         <v>125</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -3683,7 +3686,7 @@
         <v>116</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3701,7 +3704,7 @@
         <v>127</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>13</v>
@@ -3722,7 +3725,7 @@
         <v>116</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3740,7 +3743,7 @@
         <v>129</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
@@ -3761,7 +3764,7 @@
         <v>116</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3800,7 +3803,7 @@
         <v>116</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3839,7 +3842,7 @@
         <v>116</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3878,7 +3881,7 @@
         <v>116</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3886,17 +3889,17 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>13</v>
@@ -3917,7 +3920,7 @@
         <v>116</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -3925,17 +3928,17 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>13</v>
@@ -3956,7 +3959,7 @@
         <v>116</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -3964,17 +3967,17 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>13</v>
@@ -3995,7 +3998,7 @@
         <v>116</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
@@ -4020,10 +4023,10 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,13 +4091,13 @@
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
@@ -4103,12 +4106,12 @@
         <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>161</v>
@@ -4118,13 +4121,13 @@
         <v>52</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>10</v>
@@ -4136,15 +4139,15 @@
         <v>10</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>163</v>
+        <v>411</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -4159,7 +4162,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>162</v>
@@ -4169,7 +4172,7 @@
         <v>55</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>13</v>
@@ -4187,15 +4190,15 @@
         <v>10</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -4210,18 +4213,18 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -4238,10 +4241,10 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4258,7 +4261,7 @@
         <v>121</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
@@ -4287,11 +4290,11 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16" t="s">
@@ -4306,10 +4309,10 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>5</v>
@@ -4329,16 +4332,16 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>335</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>5</v>
@@ -4359,18 +4362,18 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23" t="s">
@@ -4398,18 +4401,18 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>254</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>255</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23" t="s">
@@ -4437,18 +4440,18 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>249</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>250</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23" t="s">
@@ -4487,7 +4490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4556,13 +4559,13 @@
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
@@ -4571,7 +4574,7 @@
         <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4588,7 +4591,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>147</v>
@@ -4603,7 +4606,7 @@
         <v>148</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4644,10 +4647,10 @@
         <v>112</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4667,7 +4670,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>72</v>
@@ -4691,10 +4694,10 @@
         <v>114</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -4726,10 +4729,10 @@
         <v>77</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>3</v>
@@ -4738,7 +4741,7 @@
         <v>115</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -4770,10 +4773,10 @@
         <v>21</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>3</v>
@@ -4782,7 +4785,7 @@
         <v>110</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -4808,22 +4811,22 @@
         <v>26</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -4843,25 +4846,25 @@
         <v>28</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -4884,22 +4887,22 @@
         <v>31</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -4919,16 +4922,16 @@
         <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>4</v>
@@ -4937,7 +4940,7 @@
         <v>3</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -4960,22 +4963,22 @@
         <v>34</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -4998,7 +5001,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>9</v>
@@ -5013,7 +5016,7 @@
         <v>3</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>10</v>
@@ -5033,7 +5036,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>14</v>
@@ -5068,7 +5071,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>9</v>
@@ -5083,7 +5086,7 @@
         <v>4</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>10</v>
@@ -5100,7 +5103,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>9</v>
@@ -5115,7 +5118,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>10</v>
@@ -5132,7 +5135,7 @@
         <v>44</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>45</v>
@@ -5147,10 +5150,10 @@
         <v>4</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>10</v>
@@ -5167,7 +5170,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>45</v>
@@ -5182,10 +5185,10 @@
         <v>4</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>10</v>
@@ -5202,7 +5205,7 @@
         <v>49</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>9</v>
@@ -5217,10 +5220,10 @@
         <v>4</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>10</v>
@@ -5237,7 +5240,7 @@
         <v>51</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>9</v>
@@ -5252,7 +5255,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>10</v>
@@ -5269,7 +5272,7 @@
         <v>54</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>9</v>
@@ -5284,10 +5287,10 @@
         <v>4</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>10</v>
@@ -5304,7 +5307,7 @@
         <v>57</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>58</v>
@@ -5339,7 +5342,7 @@
         <v>61</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>62</v>
@@ -5354,7 +5357,7 @@
         <v>4</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>10</v>
@@ -5371,7 +5374,7 @@
         <v>79</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>9</v>
@@ -5386,7 +5389,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>10</v>
@@ -5403,7 +5406,7 @@
         <v>81</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>9</v>
@@ -5418,7 +5421,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>10</v>
@@ -5435,7 +5438,7 @@
         <v>83</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>84</v>
@@ -5470,7 +5473,7 @@
         <v>87</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>88</v>
@@ -5505,7 +5508,7 @@
         <v>99</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>9</v>
@@ -5520,7 +5523,7 @@
         <v>4</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>10</v>
@@ -5528,10 +5531,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>178</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>4</v>
@@ -5545,10 +5548,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>4</v>
@@ -5562,10 +5565,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>4</v>
@@ -5579,13 +5582,13 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>367</v>
-      </c>
       <c r="F31" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>4</v>
@@ -5617,7 +5620,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5682,13 +5685,13 @@
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
@@ -5697,42 +5700,42 @@
         <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="B2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>218</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -5749,13 +5752,13 @@
         <v>41</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>205</v>
-      </c>
       <c r="F3" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>9</v>
@@ -5808,13 +5811,13 @@
         <v>113</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M4" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>409</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>410</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -5828,31 +5831,31 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
         <v>195</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>198</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -5866,25 +5869,25 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>209</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>3</v>
@@ -5901,19 +5904,19 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>212</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>9</v>
@@ -5937,19 +5940,19 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>288</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
@@ -5973,16 +5976,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>284</v>
-      </c>
       <c r="D9" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>298</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>299</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>13</v>
@@ -5997,7 +6000,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -6008,37 +6011,37 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>222</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>223</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>226</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -6049,37 +6052,37 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>200</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>201</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>400</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>203</v>
-      </c>
       <c r="L11" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -6090,16 +6093,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>214</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>215</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>13</v>
@@ -6108,7 +6111,7 @@
         <v>45</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>3</v>
@@ -6130,25 +6133,25 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>292</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>293</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>3</v>
@@ -6157,7 +6160,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>163</v>
+        <v>412</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6168,23 +6171,23 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>296</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>297</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I14" s="26" t="s">
         <v>3</v>
@@ -6193,7 +6196,7 @@
         <v>3</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -6204,22 +6207,22 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>4</v>
@@ -6231,7 +6234,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
@@ -6242,19 +6245,19 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>302</v>
-      </c>
       <c r="F16" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>9</v>
@@ -6277,19 +6280,19 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>305</v>
-      </c>
       <c r="F17" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>9</v>
@@ -6312,10 +6315,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -6329,10 +6332,10 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>178</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -6346,13 +6349,13 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>367</v>
-      </c>
       <c r="F20" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>4</v>
@@ -6375,7 +6378,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>39</v>
@@ -6387,19 +6390,19 @@
         <v>40</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K21" s="12" t="s">
         <v>111</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>5</v>
@@ -6425,10 +6428,10 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6493,13 +6496,13 @@
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
@@ -6519,7 +6522,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>9</v>
@@ -6534,7 +6537,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>10</v>
@@ -6551,7 +6554,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>14</v>
@@ -6586,7 +6589,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>9</v>
@@ -6601,7 +6604,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>10</v>
@@ -6618,7 +6621,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>9</v>
@@ -6633,7 +6636,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>10</v>
@@ -6641,16 +6644,16 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>9</v>
@@ -6665,7 +6668,7 @@
         <v>4</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>10</v>
@@ -6682,7 +6685,7 @@
         <v>101</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>3</v>
@@ -6694,7 +6697,7 @@
         <v>4</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>10</v>
@@ -6711,13 +6714,13 @@
         <v>42</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>205</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>9</v>
@@ -6732,7 +6735,7 @@
         <v>4</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>10</v>
@@ -6749,7 +6752,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>45</v>
@@ -6764,7 +6767,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>10</v>
@@ -6781,7 +6784,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>45</v>
@@ -6796,7 +6799,7 @@
         <v>4</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>10</v>
@@ -6804,43 +6807,43 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>222</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>223</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="L11" s="12" t="s">
-        <v>226</v>
-      </c>
       <c r="N11" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>10</v>
@@ -6857,7 +6860,7 @@
         <v>49</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>9</v>
@@ -6872,7 +6875,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>10</v>
@@ -6889,7 +6892,7 @@
         <v>51</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>9</v>
@@ -6904,7 +6907,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>10</v>
@@ -6921,7 +6924,7 @@
         <v>54</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>9</v>
@@ -6936,7 +6939,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>10</v>
@@ -6944,16 +6947,16 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>284</v>
-      </c>
       <c r="C15" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>9</v>
@@ -6968,7 +6971,7 @@
         <v>4</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>10</v>
@@ -6985,7 +6988,7 @@
         <v>57</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>58</v>
@@ -7020,7 +7023,7 @@
         <v>61</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>62</v>
@@ -7035,7 +7038,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>10</v>
@@ -7043,16 +7046,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>281</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>4</v>
@@ -7064,7 +7067,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>10</v>
@@ -7081,7 +7084,7 @@
         <v>79</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>9</v>
@@ -7096,7 +7099,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>10</v>
@@ -7113,13 +7116,13 @@
         <v>99</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>9</v>
@@ -7134,7 +7137,7 @@
         <v>3</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>10</v>
@@ -7154,7 +7157,7 @@
         <v>83</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>84</v>
@@ -7169,10 +7172,10 @@
         <v>4</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>10</v>
@@ -7189,13 +7192,13 @@
         <v>93</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>94</v>
@@ -7210,10 +7213,10 @@
         <v>3</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>10</v>
@@ -7224,10 +7227,10 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>3</v>
@@ -7239,7 +7242,7 @@
         <v>4</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>5</v>
@@ -7256,10 +7259,10 @@
         <v>87</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>9</v>
@@ -7274,7 +7277,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>10</v>
@@ -7294,7 +7297,7 @@
         <v>146</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>13</v>
@@ -7315,7 +7318,7 @@
         <v>116</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>10</v>
@@ -7326,31 +7329,31 @@
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>88</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I26" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>5</v>
@@ -7370,13 +7373,13 @@
         <v>91</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>9</v>
@@ -7391,7 +7394,7 @@
         <v>4</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>10</v>
@@ -7408,13 +7411,13 @@
         <v>81</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>9</v>
@@ -7429,13 +7432,13 @@
         <v>3</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>163</v>
+        <v>411</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>10</v>
@@ -7446,34 +7449,34 @@
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>5</v>
@@ -7484,34 +7487,34 @@
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>5</v>
@@ -7522,22 +7525,22 @@
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>265</v>
-      </c>
       <c r="C31" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>3</v>
@@ -7549,7 +7552,7 @@
         <v>4</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>10</v>
@@ -7557,16 +7560,16 @@
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>260</v>
-      </c>
       <c r="C32" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>3</v>
@@ -7578,7 +7581,7 @@
         <v>4</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>10</v>
@@ -7586,16 +7589,16 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>3</v>
@@ -7607,7 +7610,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>10</v>
@@ -7615,10 +7618,10 @@
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>4</v>
@@ -7632,10 +7635,10 @@
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>4</v>
@@ -7649,10 +7652,10 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>178</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>4</v>
@@ -7689,21 +7692,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
         <v>173</v>
       </c>
-      <c r="B1" t="s">
-        <v>174</v>
-      </c>
       <c r="C1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -7711,10 +7714,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -7722,10 +7725,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -7733,10 +7736,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -7744,10 +7747,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
         <v>175</v>
-      </c>
-      <c r="B6" t="s">
-        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -7755,10 +7758,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -7766,10 +7769,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -7777,10 +7780,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -7788,10 +7791,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -7799,10 +7802,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -7810,10 +7813,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -7842,58 +7845,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -7908,7 +7911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7979,13 +7982,13 @@
         <v>120</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>107</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>108</v>
@@ -7994,7 +7997,7 @@
         <v>149</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -8008,7 +8011,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -8023,7 +8026,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -8034,16 +8037,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -8058,7 +8061,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -8069,16 +8072,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -8092,7 +8095,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8102,16 +8105,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
@@ -8125,7 +8128,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="16"/>
       <c r="P5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>3</v>
@@ -8135,22 +8138,22 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
         <v>241</v>
-      </c>
-      <c r="C6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O6" t="s">
-        <v>242</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>3</v>
@@ -8158,13 +8161,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>4</v>
@@ -8174,7 +8177,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -8182,13 +8185,13 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>4</v>
@@ -8198,7 +8201,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8206,13 +8209,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>4</v>
@@ -8222,7 +8225,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>
@@ -8230,18 +8233,18 @@
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -8257,26 +8260,26 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -8290,7 +8293,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="P11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -8300,14 +8303,14 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>4</v>
@@ -8316,21 +8319,21 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>4</v>
@@ -8345,16 +8348,16 @@
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E14" s="35" t="s">
         <v>331</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>332</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>4</v>
@@ -8369,10 +8372,10 @@
     </row>
     <row r="15" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>178</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -8383,10 +8386,10 @@
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Fixed: sheep is default source only for RGT now
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -1257,13 +1257,13 @@
     <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),Brain,Blood)</t>
   </si>
   <si>
-    <t>IF((%type.code!=RGT),F01.A057G,)</t>
-  </si>
-  <si>
     <t>reportYearsList</t>
   </si>
   <si>
     <t>animalYearsList</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)</t>
   </si>
 </sst>
 </file>
@@ -4139,7 +4139,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4490,11 +4490,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4650,7 +4650,7 @@
         <v>326</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -6160,7 +6160,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -7432,7 +7432,7 @@
         <v>3</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M28" s="12" t="s">
         <v>305</v>
@@ -7911,7 +7911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
CWD update, its LegalRef is now N305A
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="13530" windowHeight="5595" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="417">
   <si>
     <t>Type</t>
   </si>
@@ -1273,6 +1273,9 @@
   </si>
   <si>
     <t>DO NOT TOUCH, AUTOMATICALLY FILLED</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),N305A,N123A)</t>
   </si>
 </sst>
 </file>
@@ -4031,7 +4034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6475,11 +6478,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6617,10 +6620,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>15</v>
+        <v>416</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added Bio-Rad TeSeE Western Blot as discriminatory test for BSE/SCRAPIE/CWD
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4542,10 +4542,10 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6479,10 +6479,10 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bug of editEnded listener
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="13530" windowHeight="5535" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="600" windowWidth="13530" windowHeight="5535" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -5709,11 +5709,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6078,7 +6078,7 @@
         <v>335</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>3</v>
+        <v>335</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>392</v>
@@ -6520,7 +6520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
area of sampling now optional for wild cwd
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="13530" windowHeight="5535" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="424">
   <si>
     <t>Type</t>
   </si>
@@ -1098,9 +1098,6 @@
     <t>(%internalOpType.label!=Insert)</t>
   </si>
   <si>
-    <t>IF(((%internalOpType.label==Reject)OR(%internalOpType.label==Submit)),No,Yes)</t>
-  </si>
-  <si>
     <t>IF((%internalOpType.label!=Test),{app.dcCode},{app.dcTestCode})</t>
   </si>
   <si>
@@ -1206,18 +1203,9 @@
     <t>(RELATION{SummarizedInformation,type.code}!=RGT)</t>
   </si>
   <si>
-    <t>((%sampAnAsses.code!=J051A)AND(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>(((%sampAnAsses.code!=J051A)AND(RELATION{SummarizedInformation,prod.code}!=F21.A07RY))AND(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
     <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
   </si>
   <si>
-    <t>((%anMethType.code==AT13A)AND(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
-  </si>
-  <si>
     <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)</t>
   </si>
   <si>
@@ -1294,6 +1282,21 @@
   </si>
   <si>
     <t>IF_NOT_NULL(%progLegalRef.code,.|%progLegalRef.code,)|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}!=F21.A07RY),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
+  </si>
+  <si>
+    <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1467,7 +1470,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2916,8 +2918,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S32" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A1:S32"/>
-  <sortState ref="A2:S31">
-    <sortCondition ref="B1:B31"/>
+  <sortState ref="A2:S32">
+    <sortCondition ref="J1:J32"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="79"/>
@@ -2978,8 +2980,8 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R37" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:R37"/>
-  <sortState ref="A20:R30">
-    <sortCondition ref="R1:R36"/>
+  <sortState ref="A2:R37">
+    <sortCondition ref="B1:B37"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" name="id" dataDxfId="37"/>
@@ -3717,7 +3719,7 @@
         <v>114</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3756,7 +3758,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3795,7 +3797,7 @@
         <v>114</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3834,7 +3836,7 @@
         <v>114</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3873,7 +3875,7 @@
         <v>114</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3912,7 +3914,7 @@
         <v>114</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3951,7 +3953,7 @@
         <v>114</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -3990,7 +3992,7 @@
         <v>114</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -4029,7 +4031,7 @@
         <v>114</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
@@ -4170,7 +4172,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4275,7 +4277,7 @@
         <v>306</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4510,15 +4512,15 @@
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4560,11 +4562,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4649,60 +4651,45 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>2</v>
+        <v>412</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>145</v>
+        <v>8</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>321</v>
+        <v>4</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>414</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="R2" s="12">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>417</v>
+        <v>11</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>3</v>
@@ -4711,21 +4698,24 @@
         <v>4</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>329</v>
+        <v>4</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>406</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="R3" s="12">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>416</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>176</v>
@@ -4743,27 +4733,27 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>418</v>
+        <v>396</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>3</v>
@@ -4774,8 +4764,8 @@
       <c r="J5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="12" t="s">
-        <v>410</v>
+      <c r="P5" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>9</v>
@@ -4783,98 +4773,83 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>18</v>
+        <v>41</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>390</v>
+        <v>3</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>390</v>
+        <v>4</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>321</v>
+        <v>4</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>302</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R6" s="12">
-        <v>5</v>
-      </c>
-      <c r="S6" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>24</v>
+        <v>44</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>390</v>
+        <v>3</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>390</v>
+        <v>4</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>389</v>
+        <v>4</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>302</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R7" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>386</v>
+        <v>46</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>242</v>
@@ -4883,36 +4858,33 @@
         <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>390</v>
+        <v>3</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>390</v>
+        <v>4</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>389</v>
+        <v>4</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>303</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R8" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>242</v>
@@ -4921,36 +4893,30 @@
         <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>390</v>
+        <v>3</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>390</v>
+        <v>4</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>389</v>
+        <v>4</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>317</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R9" s="12">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>387</v>
+        <v>51</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>242</v>
@@ -4959,77 +4925,74 @@
         <v>8</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>390</v>
+        <v>3</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>301</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R10" s="12">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>390</v>
+        <v>3</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>390</v>
+        <v>4</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>389</v>
+        <v>57</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R11" s="12">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>3</v>
@@ -5041,7 +5004,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>9</v>
@@ -5049,13 +5012,13 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>176</v>
@@ -5081,19 +5044,19 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>3</v>
@@ -5104,11 +5067,8 @@
       <c r="J14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N14" s="12" t="s">
-        <v>223</v>
-      </c>
       <c r="P14" s="12" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>9</v>
@@ -5116,19 +5076,19 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>3</v>
@@ -5139,11 +5099,11 @@
       <c r="J15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>302</v>
+      <c r="M15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -5151,19 +5111,19 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>3</v>
@@ -5174,11 +5134,11 @@
       <c r="J16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N16" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>303</v>
+      <c r="M16" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
@@ -5186,16 +5146,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>8</v>
@@ -5209,8 +5169,8 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P17" s="12" t="s">
-        <v>317</v>
+      <c r="O17" s="12" t="s">
+        <v>322</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
@@ -5218,22 +5178,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>3</v>
+        <v>175</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -5241,34 +5189,16 @@
       <c r="J18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N18" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>304</v>
-      </c>
       <c r="Q18" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>55</v>
+        <v>179</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>3</v>
+        <v>175</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -5276,169 +5206,106 @@
       <c r="J19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="O19" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="Q19" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>3</v>
+        <v>175</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>405</v>
+        <v>4</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R20" s="12">
-        <v>2</v>
-      </c>
-      <c r="S20" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>70</v>
+        <v>359</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>3</v>
+        <v>176</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>323</v>
+        <v>4</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="Q21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R21" s="12">
-        <v>3</v>
-      </c>
-      <c r="S21" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>58</v>
+        <v>98</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>390</v>
+        <v>145</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>390</v>
+        <v>4</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>3</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L22" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="M22" s="12" t="s">
         <v>321</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R22" s="12">
-        <v>4</v>
-      </c>
-      <c r="S22" s="12" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>59</v>
+        <v>7</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>413</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>3</v>
@@ -5447,56 +5314,74 @@
         <v>4</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P23" s="12" t="s">
-        <v>397</v>
+        <v>3</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>329</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
+      </c>
+      <c r="R23" s="12">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>3</v>
+        <v>389</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>4</v>
+        <v>389</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P24" s="12" t="s">
-        <v>319</v>
+        <v>3</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>321</v>
       </c>
       <c r="Q24" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R24" s="12">
+        <v>5</v>
+      </c>
+      <c r="S24" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>79</v>
+        <v>14</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>242</v>
@@ -5505,195 +5390,312 @@
         <v>8</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>3</v>
+        <v>389</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>4</v>
+        <v>389</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P25" s="12" t="s">
-        <v>317</v>
+        <v>3</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>388</v>
       </c>
       <c r="Q25" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R25" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>14</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>385</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>3</v>
+        <v>389</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>4</v>
+        <v>389</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M26" s="12" t="s">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>83</v>
+        <v>388</v>
       </c>
       <c r="Q26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R26" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>85</v>
+        <v>14</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>3</v>
+        <v>389</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>4</v>
+        <v>389</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M27" s="12" t="s">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>87</v>
+        <v>388</v>
       </c>
       <c r="Q27" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R27" s="12">
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>97</v>
+        <v>14</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>386</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>3</v>
+        <v>389</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>322</v>
+        <v>3</v>
+      </c>
+      <c r="P28" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="Q28" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R28" s="12">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>174</v>
+        <v>30</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>175</v>
+        <v>242</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>389</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>4</v>
+        <v>389</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>388</v>
       </c>
       <c r="Q29" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="R29" s="12">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>179</v>
+        <v>61</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>175</v>
+        <v>12</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>401</v>
       </c>
       <c r="Q30" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="R30" s="12">
+        <v>2</v>
+      </c>
+      <c r="S30" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>180</v>
+        <v>69</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>175</v>
+        <v>12</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>323</v>
       </c>
       <c r="Q31" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="R31" s="12">
+        <v>3</v>
+      </c>
+      <c r="S31" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>359</v>
+        <v>72</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>360</v>
+        <v>74</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>389</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>4</v>
+        <v>389</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="O32" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>321</v>
       </c>
       <c r="Q32" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="R32" s="12">
+        <v>4</v>
+      </c>
+      <c r="S32" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -5709,11 +5711,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5816,7 +5818,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>394</v>
+        <v>421</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>3</v>
@@ -5905,198 +5907,198 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>210</v>
+        <v>36</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>211</v>
+        <v>378</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="F5" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>43</v>
+      <c r="G5" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="O5"/>
-      <c r="P5"/>
+        <v>335</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>309</v>
+      </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>285</v>
+        <v>210</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>286</v>
+        <v>211</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="F6" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>288</v>
+      <c r="G6" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>404</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="O6"/>
+      <c r="P6"/>
       <c r="Q6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R6" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="11" t="s">
+        <v>288</v>
+      </c>
       <c r="H7" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>161</v>
+        <v>421</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>400</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="12">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>385</v>
+        <v>290</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="F8" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>199</v>
-      </c>
+      <c r="G8" s="26"/>
       <c r="H8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="38" t="s">
-        <v>284</v>
+        <v>421</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>161</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="12">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>36</v>
+        <v>283</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>38</v>
+        <v>199</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>335</v>
+        <v>4</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>335</v>
+        <v>3</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>309</v>
+        <v>3</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>284</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R9" s="12">
-        <v>7</v>
-      </c>
-      <c r="S9" s="12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -6154,7 +6156,7 @@
         <v>221</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="I11" s="23" t="s">
         <v>3</v>
@@ -6191,13 +6193,14 @@
       <c r="F12" s="23" t="s">
         <v>12</v>
       </c>
+      <c r="G12" s="23"/>
       <c r="H12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="12" t="s">
+      <c r="I12" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="23" t="s">
         <v>3</v>
       </c>
       <c r="K12" s="12" t="s">
@@ -6245,10 +6248,10 @@
         <v>309</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6315,13 +6318,13 @@
         <v>331</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>216</v>
@@ -6356,13 +6359,13 @@
         <v>8</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
@@ -6394,19 +6397,19 @@
         <v>199</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="I17" s="23" t="s">
         <v>3</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>200</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>5</v>
@@ -6486,10 +6489,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>359</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>360</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>176</v>
@@ -6524,7 +6527,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6630,7 +6633,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>9</v>
@@ -6638,69 +6641,75 @@
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>420</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>409</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>4</v>
+        <v>411</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>4</v>
+        <v>391</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>422</v>
+        <v>391</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>405</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>411</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>413</v>
+        <v>15</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>415</v>
+        <v>3</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>392</v>
+        <v>4</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>414</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>409</v>
+        <v>4</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>395</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
@@ -6708,13 +6717,13 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>176</v>
@@ -6723,7 +6732,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>4</v>
@@ -6732,7 +6741,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>9</v>
@@ -6740,13 +6749,13 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>33</v>
+        <v>204</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>176</v>
@@ -6755,7 +6764,7 @@
         <v>8</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>4</v>
@@ -6764,7 +6773,7 @@
         <v>4</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>9</v>
@@ -6772,20 +6781,17 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>226</v>
+        <v>99</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>204</v>
+        <v>35</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>226</v>
+        <v>99</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="12" t="s">
         <v>3</v>
       </c>
@@ -6796,7 +6802,7 @@
         <v>4</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>9</v>
@@ -6804,17 +6810,26 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>99</v>
+        <v>40</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>202</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G8" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H8" s="12" t="s">
         <v>3</v>
       </c>
@@ -6825,7 +6840,7 @@
         <v>4</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>378</v>
+        <v>273</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>9</v>
@@ -6833,25 +6848,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>3</v>
@@ -6862,8 +6871,8 @@
       <c r="J9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>273</v>
+      <c r="N9" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>9</v>
@@ -6871,13 +6880,13 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>176</v>
@@ -6903,19 +6912,25 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>45</v>
+        <v>217</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>44</v>
+        <v>218</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>45</v>
+        <v>217</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>220</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>43</v>
+        <v>221</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>3</v>
@@ -6926,8 +6941,14 @@
       <c r="J11" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="K11" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>223</v>
+      </c>
       <c r="N11" s="12" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>9</v>
@@ -6935,25 +6956,19 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>217</v>
+        <v>47</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>218</v>
+        <v>46</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>220</v>
+        <v>47</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>12</v>
+        <v>242</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>221</v>
+        <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>3</v>
@@ -6964,14 +6979,8 @@
       <c r="J12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>223</v>
-      </c>
       <c r="N12" s="12" t="s">
-        <v>279</v>
+        <v>300</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>9</v>
@@ -6979,13 +6988,13 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>242</v>
@@ -7011,13 +7020,13 @@
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>242</v>
@@ -7035,7 +7044,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>9</v>
@@ -7043,13 +7052,13 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>52</v>
+        <v>277</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>51</v>
+        <v>278</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>52</v>
+        <v>277</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>242</v>
@@ -7058,7 +7067,7 @@
         <v>8</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -7067,7 +7076,7 @@
         <v>4</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -7075,22 +7084,22 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>277</v>
+        <v>55</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>278</v>
+        <v>54</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>277</v>
+        <v>55</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>
@@ -7098,8 +7107,11 @@
       <c r="J16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N16" s="12" t="s">
-        <v>276</v>
+      <c r="M16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
@@ -7107,19 +7119,19 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>3</v>
@@ -7130,11 +7142,8 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>57</v>
+      <c r="P17" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
@@ -7142,22 +7151,19 @@
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>59</v>
+        <v>274</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>58</v>
+        <v>275</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>59</v>
+        <v>274</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="H18" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -7166,7 +7172,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>375</v>
+        <v>308</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>9</v>
@@ -7174,19 +7180,22 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>274</v>
+        <v>77</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>275</v>
+        <v>76</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>274</v>
+        <v>77</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G19" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H19" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -7195,7 +7204,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
@@ -7203,16 +7212,22 @@
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>8</v>
@@ -7221,145 +7236,157 @@
         <v>3</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P20" s="12" t="s">
-        <v>273</v>
+        <v>3</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>303</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>9</v>
+      </c>
+      <c r="R20" s="12">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>412</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>261</v>
+        <v>81</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>381</v>
+        <v>228</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="R21" s="12">
-        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>81</v>
+        <v>271</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>269</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>3</v>
+        <v>422</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>4</v>
+        <v>392</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>228</v>
+        <v>392</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>375</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R22" s="12">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>3</v>
+        <v>422</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>3</v>
+        <v>392</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>3</v>
+        <v>392</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>309</v>
+        <v>330</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>375</v>
       </c>
       <c r="Q23" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R23" s="12">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>332</v>
+        <v>85</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>334</v>
       </c>
+      <c r="F24" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H24" s="12" t="s">
         <v>3</v>
       </c>
@@ -7369,25 +7396,28 @@
       <c r="J24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="12" t="s">
-        <v>419</v>
+      <c r="P24" s="12" t="s">
+        <v>333</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>334</v>
+        <v>89</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>264</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>176</v>
@@ -7404,8 +7434,8 @@
       <c r="J25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P25" s="12" t="s">
-        <v>333</v>
+      <c r="N25" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>9</v>
@@ -7413,25 +7443,25 @@
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="36" t="s">
-        <v>388</v>
+        <v>263</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>262</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>3</v>
@@ -7443,68 +7473,77 @@
         <v>3</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>114</v>
+        <v>315</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>377</v>
+        <v>309</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>9</v>
       </c>
       <c r="R26" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>352</v>
+        <v>94</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>258</v>
+        <v>144</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>387</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>354</v>
+        <v>3</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>392</v>
+        <v>3</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>351</v>
+        <v>114</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>353</v>
+        <v>376</v>
       </c>
       <c r="Q27" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R27" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>265</v>
+        <v>408</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>176</v>
@@ -7516,185 +7555,158 @@
         <v>3</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>320</v>
+        <v>3</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>380</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
+      </c>
+      <c r="R28" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>79</v>
+        <v>259</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>78</v>
+        <v>260</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>272</v>
+        <v>259</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>334</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>403</v>
+        <v>4</v>
       </c>
       <c r="M29" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="O29" s="12" t="s">
-        <v>303</v>
+        <v>419</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="R29" s="12">
-        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>269</v>
+        <v>257</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>256</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>396</v>
+        <v>3</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>395</v>
+        <v>4</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>376</v>
+        <v>4</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>255</v>
       </c>
       <c r="Q30" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R30" s="12">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>268</v>
+        <v>229</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>266</v>
+        <v>193</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>229</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>396</v>
+        <v>3</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>395</v>
+        <v>4</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>376</v>
+        <v>4</v>
+      </c>
+      <c r="P31" s="12" t="s">
+        <v>394</v>
       </c>
       <c r="Q31" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R31" s="12">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>334</v>
+        <v>352</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>258</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G32" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="H32" s="12" t="s">
-        <v>3</v>
+        <v>354</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>4</v>
+        <v>391</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>353</v>
       </c>
       <c r="Q32" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R32" s="12">
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>256</v>
+        <v>416</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G33" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H33" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>4</v>
@@ -7702,25 +7714,19 @@
       <c r="J33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="12" t="s">
-        <v>255</v>
+      <c r="P33" s="12" t="s">
+        <v>418</v>
       </c>
       <c r="Q33" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>176</v>
+        <v>332</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>334</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>3</v>
@@ -7731,11 +7737,11 @@
       <c r="J34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P34" s="12" t="s">
-        <v>398</v>
+      <c r="M34" s="12" t="s">
+        <v>415</v>
       </c>
       <c r="Q34" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7978,7 +7984,7 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8010,7 +8016,7 @@
         <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8018,7 +8024,7 @@
         <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -8037,7 +8043,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8217,7 +8223,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8323,7 +8329,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8382,10 +8388,10 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>357</v>
+        <v>423</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>

</xml_diff>

<commit_message>
Negative cannot have national case id check added
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -4562,11 +4562,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5711,11 +5711,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added farmed cervids index case check
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -1170,9 +1170,6 @@
     <t>RELATION{SummarizedInformation,progId.label}|.|ZERO_PADDING({rowId},6)</t>
   </si>
   <si>
-    <t>%statusHerd.code</t>
-  </si>
-  <si>
     <t>%country.code|END_TRIM(%reportYear.code,2)|END_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
   </si>
   <si>
@@ -1297,6 +1294,9 @@
   </si>
   <si>
     <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
+  </si>
+  <si>
+    <t>%statusHerd.code|RELATION{SummarizedInformation,type.code}</t>
   </si>
 </sst>
 </file>
@@ -4172,7 +4172,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4277,7 +4277,7 @@
         <v>306</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4512,15 +4512,15 @@
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
+        <v>401</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>402</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>403</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>176</v>
@@ -4669,7 +4669,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4701,7 +4701,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>9</v>
@@ -4733,7 +4733,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
@@ -5004,7 +5004,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>9</v>
@@ -5299,7 +5299,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
@@ -5346,10 +5346,10 @@
         <v>19</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>3</v>
@@ -5390,16 +5390,16 @@
         <v>8</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>5</v>
@@ -5419,7 +5419,7 @@
         <v>26</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>242</v>
@@ -5428,16 +5428,16 @@
         <v>8</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>5</v>
@@ -5466,16 +5466,16 @@
         <v>8</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>5</v>
@@ -5495,7 +5495,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>242</v>
@@ -5504,7 +5504,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>4</v>
@@ -5542,16 +5542,16 @@
         <v>8</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>5</v>
@@ -5595,7 +5595,7 @@
         <v>321</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>5</v>
@@ -5674,10 +5674,10 @@
         <v>75</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J32" s="12" t="s">
         <v>3</v>
@@ -5712,10 +5712,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5818,7 +5818,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>3</v>
@@ -5931,7 +5931,7 @@
         <v>335</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K5" s="23" t="s">
         <v>109</v>
@@ -5969,7 +5969,7 @@
         <v>43</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I6" s="23" t="s">
         <v>3</v>
@@ -6009,7 +6009,7 @@
         <v>288</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>3</v>
@@ -6018,7 +6018,7 @@
         <v>3</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I8" s="26" t="s">
         <v>3</v>
@@ -6071,7 +6071,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>316</v>
@@ -6156,7 +6156,7 @@
         <v>221</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I11" s="23" t="s">
         <v>3</v>
@@ -6248,10 +6248,10 @@
         <v>309</v>
       </c>
       <c r="M13" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="O13" s="12" t="s">
         <v>397</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>398</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6318,13 +6318,13 @@
         <v>331</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>216</v>
@@ -6359,13 +6359,13 @@
         <v>8</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
@@ -6397,19 +6397,19 @@
         <v>199</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I17" s="23" t="s">
         <v>3</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>200</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>381</v>
+        <v>423</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>5</v>
@@ -6633,7 +6633,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>9</v>
@@ -6650,10 +6650,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>176</v>
@@ -6662,22 +6662,22 @@
         <v>13</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>309</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>9</v>
@@ -6709,7 +6709,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
@@ -6741,7 +6741,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>9</v>
@@ -7242,7 +7242,7 @@
         <v>3</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M20" s="12" t="s">
         <v>300</v>
@@ -7309,13 +7309,13 @@
         <v>12</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>330</v>
@@ -7347,13 +7347,13 @@
         <v>12</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>330</v>
@@ -7499,7 +7499,7 @@
         <v>144</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>12</v>
@@ -7540,7 +7540,7 @@
         <v>97</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>261</v>
@@ -7596,7 +7596,7 @@
         <v>4</v>
       </c>
       <c r="M29" s="12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>9</v>
@@ -7654,7 +7654,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>9</v>
@@ -7680,7 +7680,7 @@
         <v>3</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>351</v>
@@ -7697,7 +7697,7 @@
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
@@ -7715,7 +7715,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>5</v>
@@ -7738,7 +7738,7 @@
         <v>4</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>5</v>
@@ -8388,10 +8388,10 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>

</xml_diff>

<commit_message>
added junit test for checking report correctness
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -6494,11 +6494,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8013,7 +8013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
added new columns and changed schema
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="436">
   <si>
     <t>Type</t>
   </si>
@@ -1143,12 +1143,6 @@
     <t>CWD$AT12A</t>
   </si>
   <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)</t>
-  </si>
-  <si>
-    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}$RELATION{SummarizedInformation,animage.code}</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation,type.code}$%anMethType.code</t>
   </si>
   <si>
@@ -1230,9 +1224,6 @@
     <t>DO NOT TOUCH, AUTOMATICALLY FILLED</t>
   </si>
   <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),N305A,N123A)</t>
-  </si>
-  <si>
     <t>EU legal reference</t>
   </si>
   <si>
@@ -1242,68 +1233,113 @@
     <t>EU legislation related to the reason for sampling</t>
   </si>
   <si>
-    <t>progLegalRefLists</t>
+    <t>contextId</t>
+  </si>
+  <si>
+    <t>Prog ID</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),%paramCodeBaseTerm.code,RF-00004629-PAR)</t>
+  </si>
+  <si>
+    <t>progIdSuffix</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}!=F21.A07RY),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
+  </si>
+  <si>
+    <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
+  </si>
+  <si>
+    <t>%statusHerd.code|RELATION{SummarizedInformation,type.code}</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=BSE),N,)|IF((RELATION{SummarizedInformation,type.code}!=CWD),NULL,)</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,source.code}</t>
+  </si>
+  <si>
+    <t>IF((%internalOpType.label!=Insert),RELATION{Report,reportDatasetId.label},)</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>MTX.gender</t>
+  </si>
+  <si>
+    <t>(%type.code==CWD)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=CWD),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==RGT),SCRAPIE,)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),RELATION{SummarizedInformation,animage.code},)</t>
+  </si>
+  <si>
+    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}$RELATION{CasesInformation,animage.code}$RELATION{CasesInformation,sex.code}</t>
+  </si>
+  <si>
+    <t>HASH(MD5,%tseTargetGroup.code|%sampCountry.code%sampY.code|%sampM.code|%source.code|%prod.code|%animage.code|%sex.code)</t>
+  </si>
+  <si>
+    <t>psuId</t>
+  </si>
+  <si>
+    <t>N123A</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,psuId.label},$PSUId=RELATION{SummarizedInformation,psuId.label},)</t>
+  </si>
+  <si>
+    <t>sexLists</t>
+  </si>
+  <si>
+    <t>FM</t>
   </si>
   <si>
     <t>(RELATION{SummarizedInformation,type.code}==RGT)</t>
   </si>
   <si>
-    <t>contextId</t>
-  </si>
-  <si>
-    <t>Prog ID</t>
-  </si>
-  <si>
-    <t>HASH(MD5,%tseTargetGroup.code|%sampCountry.code%sampY.code|%sampM.code|%source.code|%prod.code|%animage.code)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),%paramCodeBaseTerm.code,RF-00004629-PAR)</t>
-  </si>
-  <si>
-    <t>progIdSuffix</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%progLegalRef.code,.|%progLegalRef.code,)|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}!=F21.A07RY),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
-  </si>
-  <si>
-    <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
-  </si>
-  <si>
-    <t>%statusHerd.code|RELATION{SummarizedInformation,type.code}</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=BSE),N,)|IF((RELATION{SummarizedInformation,type.code}!=CWD),NULL,)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|IF((RELATION{SummarizedInformation,type.code}!=RGT),%progIdSuffix.code,)</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,source.code}</t>
-  </si>
-  <si>
-    <t>IF((%internalOpType.label!=Insert),RELATION{Report,reportDatasetId.label},)</t>
+    <t>(RELATION{SummarizedInformation,type.code}!=CWD)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},)</t>
+  </si>
+  <si>
+    <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|IF((RELATION{SummarizedInformation,type.code}!=RGT),.%progIdSuffix.code,)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=CWD),F32.A0C9B,Mixed females and males)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1317,6 +1353,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1431,7 +1473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1470,6 +1512,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2916,10 +2959,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S31" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S33" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:S33"/>
   <sortState ref="A2:S32">
-    <sortCondition ref="J1:J32"/>
+    <sortCondition ref="R1:R32"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="79"/>
@@ -2947,10 +2990,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2512" displayName="Table2512" ref="A1:S21" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
-  <autoFilter ref="A1:S21"/>
-  <sortState ref="A2:S21">
-    <sortCondition ref="B1:B21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2512" displayName="Table2512" ref="A1:S23" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="A1:S23"/>
+  <sortState ref="A2:S22">
+    <sortCondition ref="R1:R22"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="58"/>
@@ -4172,7 +4215,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4277,7 +4320,7 @@
         <v>306</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4512,15 +4555,15 @@
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4560,13 +4603,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4651,208 +4694,287 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>407</v>
+        <v>98</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>409</v>
+      <c r="K2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="R2" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>15</v>
+        <v>58</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>392</v>
+        <v>3</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>395</v>
       </c>
       <c r="Q3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="12">
+        <v>2</v>
+      </c>
+      <c r="S3" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>40</v>
+        <v>58</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>318</v>
+        <v>3</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>322</v>
       </c>
       <c r="Q4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="12">
+        <v>3</v>
+      </c>
+      <c r="S4" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>42</v>
+        <v>58</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="H5" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>302</v>
+      <c r="K5" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="Q5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="12">
+        <v>4</v>
+      </c>
+      <c r="S5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H6" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="J6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>302</v>
+      <c r="K6" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="Q6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="12">
+        <v>5</v>
+      </c>
+      <c r="S6" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>47</v>
+        <v>416</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>417</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>242</v>
+        <v>12</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>8</v>
+        <v>418</v>
       </c>
       <c r="H7" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>4</v>
+      <c r="K7" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>303</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="P7"/>
       <c r="Q7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" s="12">
+        <v>6</v>
+      </c>
+      <c r="S7" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>49</v>
+        <v>14</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>380</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>242</v>
@@ -4861,30 +4983,39 @@
         <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>316</v>
+      <c r="O8" s="12" t="s">
+        <v>383</v>
       </c>
       <c r="Q8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="12">
+        <v>7</v>
+      </c>
+      <c r="S8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>52</v>
+        <v>14</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>242</v>
@@ -4893,135 +5024,153 @@
         <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>304</v>
+      <c r="O9" s="12" t="s">
+        <v>383</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R9" s="12">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>55</v>
+        <v>14</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="H10" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="O10" s="12" t="s">
-        <v>57</v>
+        <v>383</v>
       </c>
       <c r="Q10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R10" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>59</v>
+        <v>14</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>381</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="H11" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>4</v>
-      </c>
       <c r="P11" s="12" t="s">
-        <v>389</v>
+        <v>317</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R11" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>318</v>
+      <c r="O12" s="12" t="s">
+        <v>383</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R12" s="12">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>79</v>
+        <v>7</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>403</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>8</v>
@@ -5033,33 +5182,30 @@
         <v>4</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>316</v>
+        <v>3</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>328</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>9</v>
+      </c>
+      <c r="R13" s="12">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>81</v>
+        <v>402</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>4</v>
@@ -5067,34 +5213,31 @@
       <c r="J14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M14" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>83</v>
+      <c r="P14" s="12" t="s">
+        <v>424</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -5102,11 +5245,8 @@
       <c r="J15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M15" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="O15" s="12" t="s">
-        <v>87</v>
+      <c r="P15" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -5114,13 +5254,13 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -5129,7 +5269,7 @@
         <v>8</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>
@@ -5137,19 +5277,31 @@
       <c r="J16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="12" t="s">
-        <v>321</v>
+      <c r="P16" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>174</v>
+        <v>42</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="I17" s="12" t="s">
         <v>4</v>
@@ -5157,16 +5309,34 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N17" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>302</v>
+      </c>
       <c r="Q17" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>179</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
@@ -5174,16 +5344,34 @@
       <c r="J18" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N18" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>302</v>
+      </c>
       <c r="Q18" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>180</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>175</v>
+        <v>242</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -5191,19 +5379,34 @@
       <c r="J19" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N19" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>303</v>
+      </c>
       <c r="Q19" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>358</v>
+        <v>49</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>4</v>
@@ -5211,183 +5414,156 @@
       <c r="J20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="12" t="s">
-        <v>4</v>
+      <c r="P20" s="12" t="s">
+        <v>316</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>145</v>
+        <v>8</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>320</v>
+        <v>4</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>304</v>
       </c>
       <c r="Q21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R21" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>408</v>
+        <v>55</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>328</v>
+        <v>57</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="R22" s="12">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>320</v>
+        <v>4</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>387</v>
       </c>
       <c r="Q23" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R23" s="12">
-        <v>5</v>
-      </c>
-      <c r="S23" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>24</v>
+        <v>76</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" s="12" t="s">
-        <v>385</v>
+        <v>4</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R24" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>382</v>
+        <v>78</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>242</v>
@@ -5396,274 +5572,224 @@
         <v>8</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O25" s="12" t="s">
-        <v>385</v>
+        <v>4</v>
+      </c>
+      <c r="P25" s="12" t="s">
+        <v>316</v>
       </c>
       <c r="Q25" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R25" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>29</v>
+        <v>80</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>385</v>
+        <v>83</v>
       </c>
       <c r="Q26" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R26" s="12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>383</v>
+        <v>84</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P27" s="12" t="s">
-        <v>317</v>
+        <v>4</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="Q27" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R27" s="12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>32</v>
+        <v>96</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>386</v>
+        <v>4</v>
       </c>
       <c r="J28" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q28" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="38" t="s">
+        <v>425</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="J33" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O28" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q28" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R28" s="12">
+      <c r="Q33" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="R33" s="12">
         <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="L29" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="M29" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="Q29" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R29" s="12">
-        <v>2</v>
-      </c>
-      <c r="S29" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>377</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R30" s="12">
-        <v>3</v>
-      </c>
-      <c r="S30" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q31" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R31" s="12">
-        <v>4</v>
-      </c>
-      <c r="S31" s="12" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -5677,13 +5803,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5768,96 +5894,101 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>204</v>
+        <v>213</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>8</v>
+        <v>330</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>415</v>
+        <v>386</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>3</v>
+        <v>386</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>3</v>
+        <v>386</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>309</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R2" s="12">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>207</v>
+        <v>40</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>204</v>
+        <v>39</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="F3" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="23" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="23"/>
+      <c r="J3" s="23" t="s">
+        <v>3</v>
+      </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R3" s="12">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>280</v>
+        <v>65</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>204</v>
+        <v>58</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>281</v>
+        <v>66</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>282</v>
+        <v>67</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I4" s="12" t="s">
         <v>3</v>
@@ -5865,56 +5996,61 @@
       <c r="J4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="23"/>
+      <c r="K4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>392</v>
+      </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="12">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>35</v>
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>376</v>
+        <v>194</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>37</v>
+        <v>195</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>334</v>
+        <v>407</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>334</v>
+        <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>419</v>
+        <v>386</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>9</v>
@@ -5922,136 +6058,140 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>43</v>
+        <v>206</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>415</v>
-      </c>
-      <c r="I6" s="23" t="s">
+        <v>408</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="O6"/>
-      <c r="P6"/>
       <c r="Q6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R6" s="12">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>285</v>
+        <v>207</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>286</v>
+        <v>208</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>288</v>
+        <v>209</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>415</v>
-      </c>
-      <c r="I7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>396</v>
-      </c>
+      <c r="K7" s="23"/>
       <c r="Q7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="12">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>289</v>
+        <v>36</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>290</v>
+        <v>374</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="F8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="H8" s="12" t="s">
-        <v>415</v>
-      </c>
-      <c r="I8" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>3</v>
+        <v>334</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>334</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>161</v>
+        <v>109</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>412</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="12">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>381</v>
+        <v>281</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>12</v>
+        <v>282</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>4</v>
@@ -6062,37 +6202,33 @@
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="26" t="s">
-        <v>284</v>
-      </c>
+      <c r="K9" s="23"/>
       <c r="Q9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R9" s="12">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>40</v>
+        <v>277</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>39</v>
+        <v>278</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>201</v>
+        <v>292</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>8</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G10" s="27"/>
       <c r="H10" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>3</v>
@@ -6100,11 +6236,14 @@
       <c r="J10" s="27" t="s">
         <v>3</v>
       </c>
+      <c r="K10" s="12" t="s">
+        <v>310</v>
+      </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R10" s="12">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -6127,7 +6266,7 @@
         <v>221</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="I11" s="23" t="s">
         <v>3</v>
@@ -6150,243 +6289,230 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>278</v>
+        <v>196</v>
+      </c>
+      <c r="B12" t="s">
+        <v>193</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>292</v>
+        <v>197</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>293</v>
+        <v>198</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="23"/>
+      <c r="G12" s="23" t="s">
+        <v>199</v>
+      </c>
       <c r="H12" s="12" t="s">
-        <v>4</v>
+        <v>407</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="23" t="s">
-        <v>3</v>
+      <c r="J12" s="12" t="s">
+        <v>386</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>310</v>
+        <v>200</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>411</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>65</v>
+        <v>210</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>66</v>
+        <v>211</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>68</v>
+      <c r="G13" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="H13" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="I13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="J13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>394</v>
-      </c>
+      <c r="K13" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="O13"/>
+      <c r="P13"/>
       <c r="Q13" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>3</v>
-      </c>
-      <c r="S13" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>275</v>
+        <v>35</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>8</v>
+        <v>287</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="11" t="s">
         <v>3</v>
       </c>
+      <c r="K14" s="11" t="s">
+        <v>394</v>
+      </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R14" s="12">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="B15" t="s">
-        <v>193</v>
+        <v>289</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>214</v>
+        <v>290</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="F15" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>330</v>
-      </c>
+      <c r="G15" s="26"/>
       <c r="H15" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>309</v>
+        <v>408</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>161</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R15" s="12">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B16" t="s">
-        <v>193</v>
+        <v>283</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>194</v>
+        <v>379</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>176</v>
+        <v>315</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>414</v>
+        <v>4</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>388</v>
+        <v>3</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>284</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R16" s="12">
-        <v>4</v>
-      </c>
-      <c r="S16" s="12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B17" t="s">
-        <v>193</v>
+        <v>294</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>275</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>197</v>
+        <v>295</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>199</v>
+        <v>296</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>414</v>
-      </c>
-      <c r="I17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>418</v>
+        <v>3</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R17" s="12">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -6426,24 +6552,51 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>224</v>
+        <v>416</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>417</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>175</v>
+        <v>12</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>4</v>
+        <v>431</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>4</v>
+        <v>431</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>432</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="R19" s="12">
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>175</v>
@@ -6460,25 +6613,86 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="I21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="O21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>4</v>
+      <c r="I22" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R23" s="12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6494,11 +6708,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M34" sqref="M34"/>
+      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6589,7 +6803,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>261</v>
@@ -6610,7 +6824,7 @@
         <v>3</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>9</v>
@@ -6677,7 +6891,7 @@
         <v>144</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>12</v>
@@ -6698,7 +6912,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
@@ -6727,7 +6941,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>350</v>
@@ -6774,7 +6988,7 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M6" s="12" t="s">
         <v>300</v>
@@ -6806,19 +7020,19 @@
         <v>12</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>329</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -6844,19 +7058,19 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>329</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -6882,7 +7096,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>4</v>
@@ -6891,7 +7105,7 @@
         <v>4</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>9</v>
@@ -6908,10 +7122,10 @@
         <v>11</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>176</v>
@@ -6920,28 +7134,19 @@
         <v>13</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>406</v>
+        <v>4</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>388</v>
+        <v>4</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>405</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>309</v>
+        <v>4</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="R10" s="12">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6961,7 +7166,7 @@
         <v>8</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>4</v>
@@ -6970,7 +7175,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>9</v>
@@ -7002,7 +7207,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>9</v>
@@ -7025,7 +7230,7 @@
         <v>8</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>4</v>
@@ -7034,7 +7239,7 @@
         <v>4</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>372</v>
+        <v>427</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>9</v>
@@ -7054,7 +7259,7 @@
         <v>176</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>4</v>
@@ -7063,7 +7268,7 @@
         <v>4</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>9</v>
@@ -7092,7 +7297,7 @@
         <v>8</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>4</v>
@@ -7124,7 +7329,7 @@
         <v>43</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>
@@ -7156,7 +7361,7 @@
         <v>43</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17" s="12" t="s">
         <v>4</v>
@@ -7181,32 +7386,20 @@
       <c r="C18" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>220</v>
-      </c>
       <c r="F18" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>221</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J18" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>223</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>279</v>
@@ -7232,7 +7425,7 @@
         <v>8</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>4</v>
@@ -7264,7 +7457,7 @@
         <v>8</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>4</v>
@@ -7296,7 +7489,7 @@
         <v>8</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>4</v>
@@ -7360,7 +7553,7 @@
         <v>56</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I23" s="12" t="s">
         <v>4</v>
@@ -7395,7 +7588,7 @@
         <v>60</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I24" s="12" t="s">
         <v>4</v>
@@ -7404,7 +7597,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>373</v>
+        <v>423</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -7456,7 +7649,7 @@
         <v>8</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I26" s="12" t="s">
         <v>4</v>
@@ -7488,7 +7681,7 @@
         <v>82</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>4</v>
@@ -7526,7 +7719,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>4</v>
@@ -7564,7 +7757,7 @@
         <v>8</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>4</v>
@@ -7596,7 +7789,7 @@
         <v>176</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>4</v>
@@ -7605,7 +7798,7 @@
         <v>4</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>9</v>
@@ -7625,7 +7818,7 @@
         <v>176</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>4</v>
@@ -7654,7 +7847,7 @@
         <v>176</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I32" s="12" t="s">
         <v>4</v>
@@ -7663,7 +7856,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>9</v>
@@ -7671,7 +7864,7 @@
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
@@ -7689,7 +7882,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>5</v>
@@ -7703,7 +7896,7 @@
         <v>333</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>4</v>
@@ -7712,7 +7905,7 @@
         <v>4</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>5</v>
@@ -8362,10 +8555,10 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -8421,7 +8614,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>355</v>

</xml_diff>

<commit_message>
adapted tests with the new refresh status flow
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="438">
   <si>
     <t>Type</t>
   </si>
@@ -759,9 +759,6 @@
     <t>repVersion</t>
   </si>
   <si>
-    <t>DO NOT TOUCH, used with GetAck</t>
-  </si>
-  <si>
     <t>reportMessageId</t>
   </si>
   <si>
@@ -1330,6 +1327,18 @@
   </si>
   <si>
     <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>reportLastMessageId</t>
+  </si>
+  <si>
+    <t>reportLastModifyingMessageId</t>
+  </si>
+  <si>
+    <t>reportValidationMessageId</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
   </si>
 </sst>
 </file>
@@ -2928,8 +2937,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S11" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
-  <autoFilter ref="A1:S11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S14" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+  <autoFilter ref="A1:S14"/>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="98"/>
     <tableColumn id="2" name="code" dataDxfId="97"/>
@@ -3738,7 +3747,7 @@
         <v>123</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>12</v>
@@ -3759,7 +3768,7 @@
         <v>114</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3777,7 +3786,7 @@
         <v>125</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
@@ -3798,7 +3807,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3816,7 +3825,7 @@
         <v>127</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>12</v>
@@ -3837,7 +3846,7 @@
         <v>114</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3876,7 +3885,7 @@
         <v>114</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3915,7 +3924,7 @@
         <v>114</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3954,7 +3963,7 @@
         <v>114</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3962,17 +3971,17 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>12</v>
@@ -3993,7 +4002,7 @@
         <v>114</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -4001,17 +4010,17 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>12</v>
@@ -4032,7 +4041,7 @@
         <v>114</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -4040,17 +4049,17 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>12</v>
@@ -4071,7 +4080,7 @@
         <v>114</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
@@ -4093,13 +4102,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4200,7 +4209,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>9</v>
@@ -4212,7 +4221,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4314,10 +4323,10 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4363,11 +4372,11 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16" t="s">
@@ -4405,13 +4414,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>243</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>176</v>
@@ -4435,15 +4444,15 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>244</v>
+        <v>437</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>176</v>
@@ -4474,15 +4483,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>252</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>244</v>
+        <v>437</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>176</v>
@@ -4513,15 +4520,13 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>247</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>244</v>
+        <v>437</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>176</v>
@@ -4552,15 +4557,13 @@
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>395</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>396</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="B11" s="23"/>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>397</v>
+        <v>437</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4586,6 +4589,123 @@
       </c>
       <c r="R11" s="23"/>
       <c r="S11" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>394</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="23" t="s">
+        <v>396</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4721,7 +4841,7 @@
         <v>146</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4762,10 +4882,10 @@
         <v>110</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4785,7 +4905,7 @@
         <v>58</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>70</v>
@@ -4809,10 +4929,10 @@
         <v>112</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -4844,10 +4964,10 @@
         <v>75</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>3</v>
@@ -4856,7 +4976,7 @@
         <v>113</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -4888,10 +5008,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>3</v>
@@ -4900,7 +5020,7 @@
         <v>108</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -4914,43 +5034,43 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>416</v>
-      </c>
       <c r="I7" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="12" t="s">
@@ -4974,7 +5094,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>242</v>
@@ -4983,16 +5103,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -5024,16 +5144,16 @@
         <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
@@ -5062,16 +5182,16 @@
         <v>8</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -5091,7 +5211,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>242</v>
@@ -5100,7 +5220,7 @@
         <v>8</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>4</v>
@@ -5109,7 +5229,7 @@
         <v>3</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -5138,16 +5258,16 @@
         <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
@@ -5167,7 +5287,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>176</v>
@@ -5185,7 +5305,7 @@
         <v>3</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>9</v>
@@ -5196,7 +5316,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>176</v>
@@ -5214,7 +5334,7 @@
         <v>4</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -5246,7 +5366,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -5278,7 +5398,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
@@ -5313,7 +5433,7 @@
         <v>223</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
@@ -5348,7 +5468,7 @@
         <v>223</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>9</v>
@@ -5380,10 +5500,10 @@
         <v>4</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
@@ -5415,7 +5535,7 @@
         <v>4</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>9</v>
@@ -5447,10 +5567,10 @@
         <v>4</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P21" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>9</v>
@@ -5517,7 +5637,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
@@ -5549,7 +5669,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -5581,7 +5701,7 @@
         <v>4</v>
       </c>
       <c r="P25" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>9</v>
@@ -5683,7 +5803,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
@@ -5751,10 +5871,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>356</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>357</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>176</v>
@@ -5777,22 +5897,22 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="38" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>204</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>3</v>
@@ -5817,7 +5937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5921,22 +6041,22 @@
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>216</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -6012,13 +6132,13 @@
         <v>111</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M4" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>390</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>391</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -6050,13 +6170,13 @@
         <v>8</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -6088,7 +6208,7 @@
         <v>8</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>3</v>
@@ -6147,7 +6267,7 @@
         <v>35</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>37</v>
@@ -6162,19 +6282,19 @@
         <v>4</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K8" s="27" t="s">
         <v>109</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -6188,16 +6308,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>204</v>
       </c>
       <c r="D9" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>281</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>282</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>176</v>
@@ -6224,16 +6344,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>278</v>
-      </c>
       <c r="D10" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>292</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>293</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>12</v>
@@ -6249,7 +6369,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -6278,7 +6398,7 @@
         <v>221</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I11" s="23" t="s">
         <v>3</v>
@@ -6319,19 +6439,19 @@
         <v>199</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>200</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
@@ -6360,7 +6480,7 @@
         <v>43</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>3</v>
@@ -6382,25 +6502,25 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>286</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>287</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>3</v>
@@ -6409,7 +6529,7 @@
         <v>3</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -6420,23 +6540,23 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>291</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I15" s="26" t="s">
         <v>3</v>
@@ -6456,16 +6576,16 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F16" s="23" t="s">
         <v>12</v>
@@ -6483,7 +6603,7 @@
         <v>3</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
@@ -6494,16 +6614,16 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="12" t="s">
         <v>295</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>296</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>176</v>
@@ -6529,16 +6649,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>193</v>
       </c>
       <c r="D18" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>298</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>299</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
@@ -6564,40 +6684,40 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="M19" s="12" t="s">
         <v>428</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>425</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>429</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>5</v>
@@ -6648,10 +6768,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>356</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>357</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>176</v>
@@ -6692,22 +6812,22 @@
         <v>75</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>113</v>
       </c>
       <c r="L23" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="M23" s="12" t="s">
         <v>418</v>
-      </c>
-      <c r="M23" s="12" t="s">
-        <v>419</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>5</v>
@@ -6815,34 +6935,34 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>84</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I2" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>410</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>410</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>411</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -6853,34 +6973,34 @@
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>84</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I3" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>410</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>410</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>411</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -6903,7 +7023,7 @@
         <v>227</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>242</v>
@@ -6921,13 +7041,13 @@
         <v>3</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
@@ -6950,7 +7070,7 @@
         <v>144</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>12</v>
@@ -6971,7 +7091,7 @@
         <v>114</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>9</v>
@@ -6991,10 +7111,10 @@
         <v>89</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>176</v>
@@ -7012,7 +7132,7 @@
         <v>4</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>9</v>
@@ -7029,10 +7149,10 @@
         <v>91</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>176</v>
@@ -7050,10 +7170,10 @@
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>9</v>
@@ -7105,7 +7225,7 @@
         <v>4</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>9</v>
@@ -7122,7 +7242,7 @@
         <v>85</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>176</v>
@@ -7140,7 +7260,7 @@
         <v>4</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>9</v>
@@ -7148,10 +7268,10 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>4</v>
@@ -7163,7 +7283,7 @@
         <v>4</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -7230,7 +7350,7 @@
         <v>4</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>9</v>
@@ -7238,7 +7358,7 @@
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>176</v>
@@ -7256,7 +7376,7 @@
         <v>4</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -7288,7 +7408,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -7305,10 +7425,10 @@
         <v>11</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -7326,7 +7446,7 @@
         <v>4</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
@@ -7410,7 +7530,7 @@
         <v>4</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
@@ -7427,10 +7547,10 @@
         <v>97</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>176</v>
@@ -7448,7 +7568,7 @@
         <v>3</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>9</v>
@@ -7459,16 +7579,16 @@
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>260</v>
-      </c>
       <c r="C21" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>176</v>
@@ -7483,7 +7603,7 @@
         <v>4</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>9</v>
@@ -7491,13 +7611,13 @@
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>257</v>
-      </c>
       <c r="C22" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>176</v>
@@ -7512,7 +7632,7 @@
         <v>4</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
@@ -7544,7 +7664,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
@@ -7576,7 +7696,7 @@
         <v>4</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -7616,13 +7736,13 @@
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>278</v>
-      </c>
       <c r="C26" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>242</v>
@@ -7640,7 +7760,7 @@
         <v>4</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>9</v>
@@ -7672,7 +7792,7 @@
         <v>4</v>
       </c>
       <c r="P27" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>9</v>
@@ -7701,7 +7821,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
@@ -7739,7 +7859,7 @@
         <v>4</v>
       </c>
       <c r="P29" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>9</v>
@@ -7771,7 +7891,7 @@
         <v>4</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>9</v>
@@ -7803,7 +7923,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>9</v>
@@ -7811,13 +7931,13 @@
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>275</v>
-      </c>
       <c r="C32" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>176</v>
@@ -7832,7 +7952,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>9</v>
@@ -7899,7 +8019,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>9</v>
@@ -7931,7 +8051,7 @@
         <v>4</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q35" s="12" t="s">
         <v>9</v>
@@ -7959,10 +8079,10 @@
     </row>
     <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>176</v>
@@ -7971,19 +8091,19 @@
         <v>86</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q37" s="12" t="s">
         <v>5</v>
@@ -8181,7 +8301,7 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8213,7 +8333,7 @@
         <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8221,7 +8341,7 @@
         <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -8420,7 +8540,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8453,7 +8573,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="16"/>
       <c r="P5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>3</v>
@@ -8486,10 +8606,10 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>176</v>
@@ -8502,7 +8622,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -8510,10 +8630,10 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>176</v>
@@ -8526,7 +8646,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8534,10 +8654,10 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>176</v>
@@ -8550,7 +8670,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>
@@ -8566,7 +8686,7 @@
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>176</v>
@@ -8585,10 +8705,10 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -8618,7 +8738,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="P11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -8628,10 +8748,10 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2" t="s">
@@ -8644,18 +8764,18 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>176</v>
@@ -8673,13 +8793,13 @@
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E14" s="35" t="s">
         <v>323</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>324</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
added checks on positive/inc cases number and changed order of columsn
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -2970,8 +2970,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S34" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A1:S34"/>
-  <sortState ref="A2:S32">
-    <sortCondition ref="R1:R32"/>
+  <sortState ref="A2:S34">
+    <sortCondition ref="R1:R34"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="79"/>
@@ -4688,11 +4688,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5050,58 +5050,46 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>25</v>
+      <c r="A8" s="38" t="s">
+        <v>435</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>378</v>
+        <v>435</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="12" t="s">
-        <v>381</v>
-      </c>
       <c r="Q8" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R8" s="12">
         <v>7</v>
       </c>
-      <c r="S8" s="12" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>24</v>
+        <v>378</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>242</v>
@@ -5125,21 +5113,24 @@
         <v>5</v>
       </c>
       <c r="R9" s="12">
+        <v>8</v>
+      </c>
+      <c r="S9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>242</v>
@@ -5163,21 +5154,21 @@
         <v>5</v>
       </c>
       <c r="R10" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>379</v>
+        <v>29</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>242</v>
@@ -5189,33 +5180,33 @@
         <v>382</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>4</v>
+        <v>382</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P11" s="12" t="s">
-        <v>316</v>
+      <c r="O11" s="12" t="s">
+        <v>381</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>32</v>
+        <v>379</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>242</v>
@@ -5224,65 +5215,74 @@
         <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>382</v>
+        <v>4</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>382</v>
+        <v>4</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="12" t="s">
-        <v>381</v>
+      <c r="P12" s="12" t="s">
+        <v>316</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>400</v>
+        <v>31</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>3</v>
+        <v>382</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>4</v>
+        <v>382</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>327</v>
+        <v>381</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>399</v>
+        <v>7</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>400</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>176</v>
@@ -5291,30 +5291,27 @@
         <v>8</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P14" s="12" t="s">
-        <v>436</v>
+        <v>3</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>327</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="R14" s="12">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>15</v>
+        <v>399</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>176</v>
@@ -5332,21 +5329,21 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>387</v>
+        <v>436</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -5364,7 +5361,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>317</v>
+        <v>387</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
@@ -5372,19 +5369,19 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>4</v>
@@ -5395,11 +5392,8 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N17" s="12" t="s">
-        <v>223</v>
-      </c>
       <c r="P17" s="12" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
@@ -5407,13 +5401,13 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
@@ -5442,19 +5436,19 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>4</v>
@@ -5466,10 +5460,10 @@
         <v>4</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>299</v>
+        <v>223</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
@@ -5477,13 +5471,13 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>242</v>
@@ -5500,8 +5494,11 @@
       <c r="J20" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N20" s="12" t="s">
+        <v>299</v>
+      </c>
       <c r="P20" s="12" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>9</v>
@@ -5509,13 +5506,13 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>242</v>
@@ -5532,11 +5529,8 @@
       <c r="J21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="12" t="s">
-        <v>300</v>
-      </c>
       <c r="P21" s="12" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>9</v>
@@ -5544,19 +5538,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>4</v>
@@ -5567,11 +5561,11 @@
       <c r="J22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>57</v>
+      <c r="N22" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>303</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
@@ -5579,19 +5573,19 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>4</v>
@@ -5602,8 +5596,11 @@
       <c r="J23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P23" s="12" t="s">
-        <v>433</v>
+      <c r="M23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
@@ -5611,19 +5608,19 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>4</v>
@@ -5635,7 +5632,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>317</v>
+        <v>433</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -5643,16 +5640,16 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>8</v>
@@ -5667,7 +5664,7 @@
         <v>4</v>
       </c>
       <c r="P25" s="12" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>9</v>
@@ -5675,19 +5672,19 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>4</v>
@@ -5698,11 +5695,8 @@
       <c r="J26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="O26" s="12" t="s">
-        <v>83</v>
+      <c r="P26" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>9</v>
@@ -5710,19 +5704,19 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>4</v>
@@ -5734,10 +5728,10 @@
         <v>4</v>
       </c>
       <c r="M27" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>9</v>
@@ -5745,19 +5739,19 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>4</v>
@@ -5768,8 +5762,11 @@
       <c r="J28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P28" s="12" t="s">
-        <v>320</v>
+      <c r="M28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
@@ -5777,10 +5774,19 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>174</v>
+        <v>97</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>4</v>
@@ -5791,13 +5797,16 @@
       <c r="J29" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="P29" s="12" t="s">
+        <v>320</v>
+      </c>
       <c r="Q29" s="12" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>175</v>
@@ -5817,7 +5826,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>175</v>
@@ -5837,60 +5846,51 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E33" s="12" t="s">
         <v>356</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="O32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q32" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>435</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>414</v>
+        <v>4</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>414</v>
+        <v>4</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R33" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>226</v>
       </c>
@@ -5929,11 +5929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6837,10 +6837,10 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
converted in maven project and updated SWT library
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="465">
   <si>
     <t>Type</t>
   </si>
@@ -666,9 +666,6 @@
     <t>Country of birth of the animal</t>
   </si>
   <si>
-    <t>sampAnAsses</t>
-  </si>
-  <si>
     <t>Final evaluation of the case after discriminatory testing</t>
   </si>
   <si>
@@ -1179,9 +1176,6 @@
     <t>(RELATION{SummarizedInformation,type.code}!=RGT)</t>
   </si>
   <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampAnAsses.code},sampAnAsses=RELATION{CasesInformation,sampAnAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
-  </si>
-  <si>
     <t>IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
   </si>
   <si>
@@ -1218,9 +1212,6 @@
     <t>EU legislation related to the reason for sampling</t>
   </si>
   <si>
-    <t>contextId</t>
-  </si>
-  <si>
     <t>Prog ID</t>
   </si>
   <si>
@@ -1233,9 +1224,6 @@
     <t>POS</t>
   </si>
   <si>
-    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
     <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
   </si>
   <si>
@@ -1287,9 +1275,6 @@
     <t>(RELATION{SummarizedInformation,prod.code}==F21.A07RV)</t>
   </si>
   <si>
-    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
     <t>reportLastMessageId</t>
   </si>
   <si>
@@ -1329,41 +1314,119 @@
     <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
   </si>
   <si>
-    <t>AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=BSE),(RELATION{SummarizedInformation,type.code}!=CWD))</t>
-  </si>
-  <si>
-    <t>IF(AND((%sampAnAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=SCRAPIE),(RELATION{SummarizedInformation,type.code}!=RGT),(RELATION{SummarizedInformation,type.code}!=BSEOS)),Y,)</t>
-  </si>
-  <si>
-    <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Yes,No)</t>
+    <t>%type.code|IF((%type.code==CWD),$RELATION{Report,isExceptionCountry.label},)</t>
+  </si>
+  <si>
+    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{Report,isExceptionCountry.label}==No))</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(RELATION{Report,isExceptionCountry.label}==No)),Mixed females and males,)</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(RELATION{Report,isExceptionCountry.label}==No)),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>First test type</t>
+  </si>
+  <si>
+    <t>First test</t>
+  </si>
+  <si>
+    <t>Type of the first executed test</t>
+  </si>
+  <si>
+    <t>First executed test</t>
+  </si>
+  <si>
+    <t>sampInfo</t>
+  </si>
+  <si>
+    <t>D.11</t>
+  </si>
+  <si>
+    <t>origSampId</t>
+  </si>
+  <si>
+    <t>origSampId=%origSampId.label</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,sampId.label}</t>
+  </si>
+  <si>
+    <t>sampUnitType</t>
+  </si>
+  <si>
+    <t>C.02</t>
+  </si>
+  <si>
+    <t>G199A</t>
+  </si>
+  <si>
+    <t>H.01</t>
+  </si>
+  <si>
+    <t>anPortSeq</t>
+  </si>
+  <si>
+    <t>%type.code$%anMethType.code</t>
+  </si>
+  <si>
+    <t>Portion</t>
+  </si>
+  <si>
+    <t>Portion of the analyzed sample</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>sampEventAsses</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=BSE),(RELATION{SummarizedInformation,type.code}!=CWD))</t>
+  </si>
+  <si>
+    <t>IF(AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=SCRAPIE),(RELATION{SummarizedInformation,type.code}!=RGT),(RELATION{SummarizedInformation,type.code}!=BSEOS)),Y,)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampEventAsses.code},sampEventAsses=RELATION{CasesInformation,sampEventAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
+  </si>
+  <si>
+    <t>cwdExtCont</t>
+  </si>
+  <si>
+    <t>pref11</t>
+  </si>
+  <si>
+    <t>CWD extended context</t>
+  </si>
+  <si>
+    <t>Flag to include sex and PSU in aggregated data</t>
+  </si>
+  <si>
+    <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),0,1)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AND((%type.code==CWD),RELATION{Preferences,cwdExtCont.label})</t>
   </si>
   <si>
     <t>isExceptionCountry</t>
   </si>
   <si>
-    <t>%type.code|IF((%type.code==CWD),$RELATION{Report,isExceptionCountry.label},)</t>
-  </si>
-  <si>
-    <t>AND((%type.code==CWD),RELATION{Report,isExceptionCountry.label})</t>
-  </si>
-  <si>
-    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{Report,isExceptionCountry.label}==No))</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Report,isExceptionCountry.label}==No)),Mixed females and males,)</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Report,isExceptionCountry.label}==No)),F32.A0C9B,)</t>
-  </si>
-  <si>
-    <t>HASH(MD5,%tseTargetGroup.code|%sampCountry.code|%sampY.code|%sampM.code|%source.code|%prod.code|%animage.code|IF(AND((%type.code==CWD),RELATION{Report,isExceptionCountry.label}),%sex.code,)|IF(AND((%type.code==CWD),RELATION{Report,isExceptionCountry.label}),%PSUId.code,))</t>
+    <t>RELATION{Preferences,cwdExtCont.code}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1384,8 +1447,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1401,12 +1470,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1497,7 +1560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1534,9 +1597,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2927,8 +2993,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:S11" totalsRowShown="0" headerRowDxfId="111">
-  <autoFilter ref="A1:S11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:S12" totalsRowShown="0" headerRowDxfId="111">
+  <autoFilter ref="A1:S12"/>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="110"/>
     <tableColumn id="2" name="code"/>
@@ -2983,10 +3049,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S35" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S35"/>
-  <sortState ref="A2:S34">
-    <sortCondition ref="R1:R34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S37" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:S37">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:S36">
+    <sortCondition ref="R1:R36"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="79"/>
@@ -3045,8 +3117,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R39" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A1:R39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R43" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A1:R43"/>
   <sortState ref="A2:R39">
     <sortCondition ref="R1:R39"/>
   </sortState>
@@ -3415,7 +3487,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
@@ -3632,13 +3704,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,39 +3826,45 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="A3" s="41" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3" t="s">
+        <v>457</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>458</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>459</v>
+      </c>
+      <c r="F3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>360</v>
+      <c r="G3" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="L3" s="40"/>
+      <c r="M3" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>3</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3794,22 +3872,22 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
+        <v>122</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="F4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>95</v>
       </c>
       <c r="H4" s="8" t="s">
@@ -3825,7 +3903,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3833,22 +3911,22 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>155</v>
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="F5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>95</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -3864,7 +3942,7 @@
         <v>114</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3872,26 +3950,26 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" t="s">
-        <v>156</v>
+        <v>126</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>95</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>9</v>
@@ -3903,7 +3981,7 @@
         <v>114</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3911,22 +3989,22 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>157</v>
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>95</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -3942,7 +4020,7 @@
         <v>114</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3950,22 +4028,22 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" t="s">
-        <v>158</v>
+        <v>131</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F8" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
         <v>95</v>
       </c>
       <c r="H8" s="8" t="s">
@@ -3981,7 +4059,7 @@
         <v>114</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3989,38 +4067,38 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="F9" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="4" t="s">
         <v>95</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="L9" s="31" t="s">
-        <v>366</v>
+      <c r="L9" s="10" t="s">
+        <v>364</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -4028,17 +4106,17 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>12</v>
@@ -4059,7 +4137,7 @@
         <v>114</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -4067,48 +4145,87 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="F11" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="F11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="29" t="s">
         <v>95</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="34" t="s">
+      <c r="I11" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="30" t="s">
         <v>114</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>368</v>
-      </c>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
+        <v>366</v>
+      </c>
       <c r="R11">
         <v>10</v>
       </c>
-      <c r="S11" s="32"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="L12" s="31" t="s">
+        <v>367</v>
+      </c>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12">
+        <v>11</v>
+      </c>
+      <c r="S12" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4123,10 +4240,10 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4227,7 +4344,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>9</v>
@@ -4239,7 +4356,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4320,7 +4437,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
@@ -4341,10 +4458,10 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4390,11 +4507,11 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16" t="s">
@@ -4432,13 +4549,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>324</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>325</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>176</v>
@@ -4462,15 +4579,15 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>176</v>
@@ -4501,13 +4618,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>176</v>
@@ -4538,13 +4655,13 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>176</v>
@@ -4575,15 +4692,15 @@
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>249</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>250</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4614,15 +4731,15 @@
     </row>
     <row r="12" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>244</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>245</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="24"/>
       <c r="E12" s="23" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>176</v>
@@ -4653,15 +4770,15 @@
     </row>
     <row r="13" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24"/>
       <c r="E13" s="23" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>176</v>
@@ -4690,40 +4807,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>437</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23" t="s">
-        <v>436</v>
-      </c>
-      <c r="Q14" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23" t="s">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4738,13 +4854,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P21" sqref="P21"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4764,8 +4880,11 @@
     <col min="13" max="13" width="14.85546875" style="12" customWidth="1"/>
     <col min="14" max="14" width="50.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="76.28515625" style="12" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="12"/>
+    <col min="16" max="16" width="119.42578125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="12" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="12"/>
+    <col min="19" max="19" width="16.42578125" style="12" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -4859,7 +4978,7 @@
         <v>146</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4891,7 +5010,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>3</v>
@@ -4900,10 +5019,10 @@
         <v>110</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4923,7 +5042,7 @@
         <v>58</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>70</v>
@@ -4938,7 +5057,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>3</v>
@@ -4947,10 +5066,10 @@
         <v>112</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -4982,10 +5101,10 @@
         <v>75</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>3</v>
@@ -4994,7 +5113,7 @@
         <v>113</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -5026,10 +5145,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>3</v>
@@ -5038,7 +5157,7 @@
         <v>108</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -5052,25 +5171,25 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
@@ -5079,16 +5198,16 @@
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="12" t="s">
@@ -5102,67 +5221,91 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>429</v>
+      <c r="A8" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>204</v>
+        <v>90</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>429</v>
+        <v>433</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>435</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>439</v>
+        <v>3</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>439</v>
+        <v>3</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="K8" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>317</v>
+      </c>
       <c r="Q8" s="12" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="R8" s="12">
         <v>7</v>
       </c>
+      <c r="S8" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>14</v>
+        <v>93</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>26</v>
+        <v>434</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>377</v>
+        <v>436</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>241</v>
+        <v>12</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>381</v>
+        <v>3</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>381</v>
+        <v>3</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O9" s="12" t="s">
-        <v>380</v>
+      <c r="K9" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>447</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R9" s="12">
         <v>8</v>
@@ -5172,73 +5315,67 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>22</v>
+      <c r="A10" s="37" t="s">
+        <v>424</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>24</v>
+        <v>424</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>381</v>
+        <v>462</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>381</v>
+        <v>462</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="12" t="s">
-        <v>380</v>
-      </c>
       <c r="Q10" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R10" s="12">
+        <v>9</v>
+      </c>
+      <c r="S10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>29</v>
+        <v>376</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
@@ -5246,37 +5383,40 @@
       <c r="R11" s="12">
         <v>10</v>
       </c>
+      <c r="S11" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>378</v>
+        <v>24</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>4</v>
+        <v>380</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>4</v>
+        <v>380</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P12" s="12" t="s">
-        <v>315</v>
+      <c r="O12" s="12" t="s">
+        <v>379</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
@@ -5287,34 +5427,34 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -5325,25 +5465,25 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>398</v>
+        <v>21</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>377</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>4</v>
@@ -5351,11 +5491,11 @@
       <c r="J14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="12" t="s">
-        <v>326</v>
+      <c r="P14" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R14" s="12">
         <v>13</v>
@@ -5363,39 +5503,54 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>397</v>
+        <v>30</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>4</v>
+        <v>380</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>4</v>
+        <v>380</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>443</v>
+        <v>3</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>379</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="R15" s="12">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>395</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -5404,33 +5559,36 @@
         <v>8</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>386</v>
+        <v>3</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>325</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>8</v>
@@ -5445,28 +5603,22 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>42</v>
+        <v>353</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>354</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="H18" s="12" t="s">
         <v>4</v>
       </c>
@@ -5476,31 +5628,28 @@
       <c r="J18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N18" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>300</v>
+      <c r="O18" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>4</v>
@@ -5511,31 +5660,31 @@
       <c r="J19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N19" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>300</v>
+      <c r="M19" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>4</v>
@@ -5546,31 +5695,22 @@
       <c r="J20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="P20" s="12" t="s">
-        <v>301</v>
+      <c r="M20" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>4</v>
@@ -5581,28 +5721,22 @@
       <c r="J21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="P21" s="12" t="s">
-        <v>301</v>
-      </c>
       <c r="Q21" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>8</v>
@@ -5616,32 +5750,26 @@
       <c r="J22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N22" s="12" t="s">
-        <v>299</v>
-      </c>
       <c r="P22" s="12" t="s">
-        <v>302</v>
+        <v>384</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G23" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="H23" s="12" t="s">
         <v>4</v>
       </c>
@@ -5652,30 +5780,27 @@
         <v>4</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="O23" s="12" t="s">
-        <v>57</v>
+        <v>409</v>
       </c>
       <c r="Q23" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>4</v>
@@ -5686,28 +5811,22 @@
       <c r="J24" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N24" s="12" t="s">
+        <v>221</v>
+      </c>
       <c r="P24" s="12" t="s">
-        <v>427</v>
+        <v>299</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>77</v>
+        <v>174</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>4</v>
@@ -5718,25 +5837,22 @@
       <c r="J25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P25" s="12" t="s">
-        <v>316</v>
-      </c>
       <c r="Q25" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>8</v>
@@ -5750,28 +5866,31 @@
       <c r="J26" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N26" s="12" t="s">
+        <v>297</v>
+      </c>
       <c r="P26" s="12" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>4</v>
@@ -5782,31 +5901,28 @@
       <c r="J27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M27" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="O27" s="12" t="s">
-        <v>83</v>
+      <c r="P27" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>4</v>
@@ -5817,55 +5933,64 @@
       <c r="J28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M28" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>87</v>
+      <c r="P28" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G29" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="P29" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q29" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q29" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>175</v>
-      </c>
       <c r="H30" s="12" t="s">
         <v>4</v>
       </c>
@@ -5875,16 +6000,28 @@
       <c r="J30" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="P30" s="12" t="s">
+        <v>315</v>
+      </c>
       <c r="Q30" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>179</v>
+        <v>52</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>175</v>
+        <v>240</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>4</v>
@@ -5895,16 +6032,31 @@
       <c r="J31" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N31" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="P31" s="12" t="s">
+        <v>301</v>
+      </c>
       <c r="Q31" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>180</v>
+        <v>59</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>4</v>
@@ -5915,20 +6067,29 @@
       <c r="J32" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="P32" s="12" t="s">
+        <v>422</v>
+      </c>
       <c r="Q32" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>355</v>
+        <v>55</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G33" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="H33" s="12" t="s">
         <v>4</v>
       </c>
@@ -5938,19 +6099,22 @@
       <c r="J33" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="M33" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="O33" s="12" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="Q33" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>176</v>
@@ -5965,39 +6129,97 @@
         <v>4</v>
       </c>
       <c r="P34" s="12" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="F35" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="P35" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q35" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q36" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="H35" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q35" s="12" t="s">
-        <v>3</v>
+      <c r="G37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q37" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6014,10 +6236,10 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6102,37 +6324,37 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>213</v>
+        <v>451</v>
       </c>
       <c r="B2" t="s">
         <v>193</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -6208,13 +6430,13 @@
         <v>111</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -6228,37 +6450,37 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>414</v>
-      </c>
       <c r="L5" s="12" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -6287,19 +6509,19 @@
         <v>75</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>113</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -6328,13 +6550,13 @@
         <v>8</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>402</v>
+        <v>450</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -6366,7 +6588,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>3</v>
@@ -6426,7 +6648,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>37</v>
@@ -6441,16 +6663,16 @@
         <v>4</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>109</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -6464,16 +6686,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>204</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>279</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>280</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>176</v>
@@ -6500,16 +6722,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>276</v>
-      </c>
       <c r="D12" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>291</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>12</v>
@@ -6525,7 +6747,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
@@ -6536,25 +6758,25 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>218</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>219</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>3</v>
@@ -6563,10 +6785,10 @@
         <v>3</v>
       </c>
       <c r="K13" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>221</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>222</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -6595,22 +6817,22 @@
         <v>199</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>402</v>
+        <v>450</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>434</v>
+        <v>453</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>200</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>435</v>
+        <v>454</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
@@ -6639,7 +6861,7 @@
         <v>43</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>3</v>
@@ -6661,25 +6883,25 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>284</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>285</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>3</v>
@@ -6688,7 +6910,7 @@
         <v>3</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
@@ -6699,23 +6921,23 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>289</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="12" t="s">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="I17" s="26" t="s">
         <v>3</v>
@@ -6735,16 +6957,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>12</v>
@@ -6762,7 +6984,7 @@
         <v>3</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>5</v>
@@ -6773,16 +6995,16 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>293</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>294</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>176</v>
@@ -6808,16 +7030,16 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>193</v>
       </c>
       <c r="D20" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>296</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>297</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>176</v>
@@ -6843,7 +7065,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>175</v>
@@ -6883,10 +7105,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>354</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>355</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
@@ -6918,13 +7140,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P37" sqref="P37"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7015,10 +7237,10 @@
         <v>97</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>176</v>
@@ -7036,7 +7258,7 @@
         <v>3</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>9</v>
@@ -7056,13 +7278,13 @@
         <v>91</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>92</v>
@@ -7077,10 +7299,10 @@
         <v>3</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>9</v>
@@ -7102,8 +7324,8 @@
       <c r="D4" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>379</v>
+      <c r="E4" s="12" t="s">
+        <v>378</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>12</v>
@@ -7124,7 +7346,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
@@ -7135,10 +7357,10 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>176</v>
@@ -7147,19 +7369,19 @@
         <v>86</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -7179,13 +7401,13 @@
         <v>79</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>8</v>
@@ -7200,13 +7422,13 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>9</v>
@@ -7217,78 +7439,78 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>84</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>84</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7302,10 +7524,10 @@
         <v>89</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>176</v>
@@ -7323,7 +7545,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>9</v>
@@ -7331,7 +7553,7 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>175</v>
@@ -7351,13 +7573,13 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>193</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>176</v>
@@ -7372,7 +7594,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>384</v>
+        <v>455</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>9</v>
@@ -7389,7 +7611,7 @@
         <v>85</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>176</v>
@@ -7407,7 +7629,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>9</v>
@@ -7415,10 +7637,10 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>4</v>
@@ -7430,7 +7652,7 @@
         <v>4</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -7462,10 +7684,10 @@
         <v>4</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>9</v>
@@ -7497,7 +7719,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -7505,7 +7727,7 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -7523,7 +7745,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
@@ -7555,7 +7777,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
@@ -7572,10 +7794,10 @@
         <v>11</v>
       </c>
       <c r="D18" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>394</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>396</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
@@ -7593,7 +7815,7 @@
         <v>4</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>9</v>
@@ -7625,7 +7847,7 @@
         <v>4</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
@@ -7662,7 +7884,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>8</v>
@@ -7677,7 +7899,7 @@
         <v>4</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>9</v>
@@ -7685,16 +7907,16 @@
     </row>
     <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>258</v>
-      </c>
       <c r="C22" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>176</v>
@@ -7709,7 +7931,7 @@
         <v>4</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
@@ -7717,13 +7939,13 @@
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>255</v>
-      </c>
       <c r="C23" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
@@ -7738,7 +7960,7 @@
         <v>4</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
@@ -7770,7 +7992,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -7778,19 +8000,19 @@
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>217</v>
-      </c>
       <c r="C25" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>4</v>
@@ -7802,7 +8024,7 @@
         <v>4</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>9</v>
@@ -7834,7 +8056,7 @@
         <v>4</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>9</v>
@@ -7842,16 +8064,16 @@
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>276</v>
-      </c>
       <c r="C27" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>8</v>
@@ -7866,7 +8088,7 @@
         <v>4</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>9</v>
@@ -7898,7 +8120,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
@@ -7927,7 +8149,7 @@
         <v>4</v>
       </c>
       <c r="P29" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>9</v>
@@ -7965,7 +8187,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>9</v>
@@ -7982,7 +8204,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>8</v>
@@ -7997,7 +8219,7 @@
         <v>4</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>9</v>
@@ -8029,21 +8251,21 @@
         <v>4</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>273</v>
-      </c>
       <c r="C33" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
@@ -8058,13 +8280,13 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>55</v>
       </c>
@@ -8099,15 +8321,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>204</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>176</v>
@@ -8125,13 +8347,13 @@
         <v>4</v>
       </c>
       <c r="P35" s="12" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="Q35" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>49</v>
       </c>
@@ -8142,7 +8364,7 @@
         <v>49</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>8</v>
@@ -8157,18 +8379,18 @@
         <v>4</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P36" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q36" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>175</v>
@@ -8186,9 +8408,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>58</v>
@@ -8206,13 +8428,13 @@
         <v>4</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="Q38" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>72</v>
       </c>
@@ -8232,10 +8454,132 @@
         <v>4</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="Q39" s="12" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q40" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P41" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q41" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q42" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O43" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="R43" s="12">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -8269,7 +8613,7 @@
         <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8277,7 +8621,7 @@
         <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -8288,7 +8632,7 @@
         <v>173</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -8340,10 +8684,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -8354,7 +8698,7 @@
         <v>172</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -8365,7 +8709,7 @@
         <v>173</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -8376,7 +8720,7 @@
         <v>172</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -8387,7 +8731,7 @@
         <v>177</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -8427,7 +8771,7 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8456,18 +8800,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -8597,7 +8941,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -8608,11 +8952,11 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8632,7 +8976,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -8643,11 +8987,11 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -8666,7 +9010,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8676,11 +9020,11 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -8699,7 +9043,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="16"/>
       <c r="P5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>3</v>
@@ -8709,10 +9053,10 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>176</v>
@@ -8724,7 +9068,7 @@
         <v>4</v>
       </c>
       <c r="O6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>3</v>
@@ -8732,10 +9076,10 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>176</v>
@@ -8748,7 +9092,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -8756,10 +9100,10 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>176</v>
@@ -8772,7 +9116,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8780,10 +9124,10 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>176</v>
@@ -8796,7 +9140,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>
@@ -8804,15 +9148,15 @@
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>176</v>
@@ -8830,11 +9174,11 @@
       <c r="M10" s="16"/>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="37" t="s">
-        <v>375</v>
+      <c r="P10" s="36" t="s">
+        <v>374</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -8864,7 +9208,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="P11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -8874,10 +9218,10 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2" t="s">
@@ -8890,18 +9234,18 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>176</v>
@@ -8919,13 +9263,13 @@
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E14" s="35" t="s">
         <v>321</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>322</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
-Added new pureMandatory function -New check function for editable and pure mandatory fields -Changes to formulas on the tableSchema -Small changes to check conditions when empty cells where analysed
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12405" windowHeight="2760" tabRatio="690" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23280" windowHeight="4785" tabRatio="690" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -21,12 +21,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">SummarizedInformation!$A$2:$E$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="470">
   <si>
     <t>Type</t>
   </si>
@@ -1306,9 +1305,6 @@
     <t>Sample/case assessment</t>
   </si>
   <si>
-    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{Report,isExceptionCountry.label}==No))</t>
-  </si>
-  <si>
     <t>First test type</t>
   </si>
   <si>
@@ -1417,22 +1413,28 @@
     <t>%type.code|$%anMethType.code</t>
   </si>
   <si>
+    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)</t>
+  </si>
+  <si>
+    <t>(%type.code==SCRAPIE)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F01.A056M,)</t>
+  </si>
+  <si>
+    <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.label},)</t>
+  </si>
+  <si>
+    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{Preferences,cwdExtCont.label}==No))</t>
+  </si>
+  <si>
     <t>IF((%type.code==RGT),,AT06A)</t>
   </si>
   <si>
-    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)</t>
-  </si>
-  <si>
-    <t>(%type.code==SCRAPIE)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F01.A056M,)</t>
-  </si>
-  <si>
-    <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.label},)</t>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1469,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1484,6 +1486,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1567,7 +1575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1600,6 +1608,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3123,7 +3132,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S39" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A1:S39"/>
   <sortState ref="A2:S39">
-    <sortCondition ref="R1:R39"/>
+    <sortCondition ref="A1:A39"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="79"/>
@@ -3775,7 +3784,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3789,7 +3798,7 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
     <col min="13" max="14" width="14.140625" customWidth="1"/>
     <col min="15" max="16" width="14.7109375" customWidth="1"/>
     <col min="17" max="17" width="14.140625" customWidth="1"/>
@@ -3892,16 +3901,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>451</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>452</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>12</v>
@@ -3919,16 +3928,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>3</v>
@@ -4307,7 +4316,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4884,11 +4893,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4974,66 +4983,57 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>2</v>
+        <v>79</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>316</v>
+        <v>4</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" s="6">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>3</v>
+        <v>379</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>379</v>
@@ -5042,19 +5042,16 @@
         <v>3</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>467</v>
+        <v>316</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="R3" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>9</v>
@@ -5062,25 +5059,28 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>93</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>370</v>
+        <v>427</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>3</v>
+        <v>379</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>379</v>
@@ -5089,19 +5089,22 @@
         <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>316</v>
+        <v>461</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>318</v>
+        <v>462</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>462</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R4" s="6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>9</v>
@@ -5109,66 +5112,57 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>74</v>
+        <v>88</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>316</v>
+        <v>4</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>315</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R5" s="6">
-        <v>4</v>
-      </c>
-      <c r="S5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>90</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>17</v>
+        <v>426</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>18</v>
+        <v>428</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>379</v>
@@ -5180,16 +5174,22 @@
         <v>3</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>108</v>
+        <v>310</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>316</v>
+        <v>460</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>468</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R6" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>9</v>
@@ -5197,223 +5197,162 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>457</v>
+        <v>352</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>458</v>
+        <v>353</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>405</v>
+        <v>176</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="P7"/>
+        <v>4</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="Q7" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="R7" s="6">
-        <v>6</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>429</v>
+        <v>85</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>461</v>
+        <v>4</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>463</v>
+        <v>87</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="6">
-        <v>7</v>
-      </c>
-      <c r="S8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>430</v>
+        <v>81</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>462</v>
+        <v>4</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>464</v>
+        <v>83</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R9" s="6">
-        <v>8</v>
-      </c>
-      <c r="S9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="J10" s="6" t="s">
+      <c r="G11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R10" s="6">
-        <v>9</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>422</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>459</v>
-      </c>
       <c r="I11" s="6" t="s">
-        <v>459</v>
+        <v>379</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="K11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="Q11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="R11" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="S11" s="6" t="s">
         <v>9</v>
@@ -5421,244 +5360,199 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>375</v>
+        <v>394</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>240</v>
+        <v>176</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>379</v>
+        <v>3</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>378</v>
+        <v>324</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R12" s="6">
-        <v>11</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="G13" s="17" t="s">
+      <c r="C13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>378</v>
+        <v>4</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>383</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R13" s="6">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="J14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R14" s="6">
-        <v>13</v>
-      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>20</v>
+      <c r="A15" s="25" t="s">
+        <v>422</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>376</v>
+        <v>422</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>4</v>
+        <v>458</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>4</v>
+        <v>458</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="R15" s="6">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>240</v>
+        <v>176</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>379</v>
+        <v>4</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>378</v>
+        <v>4</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R16" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>394</v>
+        <v>174</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>324</v>
+        <v>4</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R17" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>240</v>
@@ -5675,23 +5569,32 @@
       <c r="J18" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="N18" s="6" t="s">
+        <v>296</v>
+      </c>
       <c r="P18" s="6" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>353</v>
+        <v>97</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>176</v>
       </c>
+      <c r="G19" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="H19" s="6" t="s">
         <v>4</v>
       </c>
@@ -5701,28 +5604,28 @@
       <c r="J19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="6" t="s">
-        <v>4</v>
+      <c r="P19" s="6" t="s">
+        <v>317</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>176</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>4</v>
@@ -5733,31 +5636,28 @@
       <c r="J20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M20" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>87</v>
+      <c r="P20" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>176</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>4</v>
@@ -5768,22 +5668,28 @@
       <c r="J21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>83</v>
+      <c r="N21" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="Q21" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>179</v>
+        <v>99</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>4</v>
@@ -5794,19 +5700,22 @@
       <c r="J22" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="P22" s="6" t="s">
+        <v>464</v>
+      </c>
       <c r="Q22" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>176</v>
@@ -5824,24 +5733,27 @@
         <v>4</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>383</v>
+        <v>314</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>176</v>
+        <v>240</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>4</v>
@@ -5852,28 +5764,31 @@
       <c r="J24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="6" t="s">
-        <v>407</v>
+      <c r="N24" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>176</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>4</v>
@@ -5884,22 +5799,28 @@
       <c r="J25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N25" s="6" t="s">
-        <v>221</v>
-      </c>
       <c r="P25" s="6" t="s">
-        <v>298</v>
+        <v>420</v>
       </c>
       <c r="Q25" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>174</v>
+        <v>55</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>4</v>
@@ -5910,57 +5831,54 @@
       <c r="J26" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="M26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="Q26" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>46</v>
+        <v>224</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>47</v>
+        <v>224</v>
       </c>
       <c r="F27" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q27" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>8</v>
@@ -5974,249 +5892,310 @@
       <c r="J28" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="N28" s="6" t="s">
+        <v>296</v>
+      </c>
       <c r="P28" s="6" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G29" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="P30"/>
+      <c r="Q30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R30" s="6">
+        <v>6</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R31" s="6">
+        <v>2</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R32" s="6">
+        <v>9</v>
+      </c>
+      <c r="S32" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q29" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="P30" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q30" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G31" s="6" t="s">
+      <c r="H33" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R33" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q31" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="6" t="s">
+      <c r="H34" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R34" s="6">
+        <v>11</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G35" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>176</v>
-      </c>
       <c r="H35" s="6" t="s">
-        <v>4</v>
+        <v>379</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>4</v>
+        <v>379</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>421</v>
+        <v>3</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>378</v>
       </c>
       <c r="Q35" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R35" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>49</v>
+        <v>14</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>376</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>240</v>
@@ -6231,97 +6210,139 @@
         <v>4</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N36" s="6" t="s">
-        <v>296</v>
+        <v>3</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="Q36" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R36" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>180</v>
+        <v>30</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>175</v>
+        <v>240</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>4</v>
+        <v>379</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>4</v>
+        <v>379</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>378</v>
       </c>
       <c r="Q37" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R37" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>89</v>
+        <v>14</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>4</v>
+        <v>379</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>4</v>
+        <v>379</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N38" s="6" t="s">
-        <v>315</v>
+        <v>3</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="Q38" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R38" s="6">
+        <v>5</v>
+      </c>
+      <c r="S38" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>176</v>
       </c>
+      <c r="G39" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="H39" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P39" s="6" t="s">
-        <v>466</v>
+        <v>3</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="Q39" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R39" s="6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6338,10 +6359,10 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6426,7 +6447,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B2" t="s">
         <v>193</v>
@@ -6572,11 +6593,11 @@
       <c r="H5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>426</v>
+      <c r="I5" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>467</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>408</v>
@@ -6652,7 +6673,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
@@ -6690,7 +6711,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -6878,7 +6899,7 @@
         <v>219</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>3</v>
@@ -6919,10 +6940,10 @@
         <v>199</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>381</v>
@@ -6934,7 +6955,7 @@
         <v>305</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -6963,7 +6984,7 @@
         <v>43</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>3</v>
@@ -7003,7 +7024,7 @@
         <v>284</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>3</v>
@@ -7039,7 +7060,7 @@
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>3</v>
@@ -7086,10 +7107,10 @@
         <v>3</v>
       </c>
       <c r="K18" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="L18" s="6" t="s">
         <v>455</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>456</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -7247,11 +7268,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7608,19 +7629,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>439</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>441</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>442</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>176</v>
@@ -7687,7 +7708,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -7695,10 +7716,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>176</v>
@@ -7713,7 +7734,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -8355,13 +8376,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>432</v>
-      </c>
       <c r="C33" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>176</v>
@@ -8376,7 +8397,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8544,13 +8565,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>437</v>
-      </c>
       <c r="C39" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>176</v>
@@ -8565,7 +8586,7 @@
         <v>4</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
New formula for ProgId under Default code
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="470">
   <si>
     <t>Type</t>
   </si>
@@ -4894,10 +4894,10 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5386,6 +5386,12 @@
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="M12" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>324</v>
+      </c>
       <c r="O12" s="6" t="s">
         <v>324</v>
       </c>
@@ -6051,10 +6057,7 @@
       <c r="L32" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="M32" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="N32" s="6" t="s">
+      <c r="O32" s="6" t="s">
         <v>469</v>
       </c>
       <c r="Q32" s="6" t="s">

</xml_diff>

<commit_message>
Auto clean the cwdExtContext when country is changed
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="23280" windowHeight="4785" tabRatio="690" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="6705" tabRatio="690" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="471">
   <si>
     <t>Type</t>
   </si>
@@ -1383,58 +1383,61 @@
     <t>Flag to include sex and PSU in aggregated data</t>
   </si>
   <si>
+    <t>yesNoLists</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Sex of the animals</t>
+  </si>
+  <si>
+    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==Yes))</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>BSE</t>
+  </si>
+  <si>
+    <t>%type.code|$%anMethType.code</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)</t>
+  </si>
+  <si>
+    <t>(%type.code==SCRAPIE)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F01.A056M,)</t>
+  </si>
+  <si>
+    <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.label},)</t>
+  </si>
+  <si>
+    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{Preferences,cwdExtCont.label}==No))</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),,AT06A)</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>(%type.code==CWD)</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
     <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
-  </si>
-  <si>
-    <t>yesNoLists</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Sex of the animals</t>
-  </si>
-  <si>
-    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==Yes))</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F32.A0C9B,)</t>
-  </si>
-  <si>
-    <t>BSE</t>
-  </si>
-  <si>
-    <t>%type.code|$%anMethType.code</t>
-  </si>
-  <si>
-    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)</t>
-  </si>
-  <si>
-    <t>(%type.code==SCRAPIE)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F01.A056M,)</t>
-  </si>
-  <si>
-    <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.label},)</t>
-  </si>
-  <si>
-    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{Preferences,cwdExtCont.label}==No))</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),,AT06A)</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
 </sst>
 </file>
@@ -3560,7 +3563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3780,11 +3783,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,22 +3931,22 @@
         <v>9</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>453</v>
+        <v>470</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>452</v>
+        <v>469</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>452</v>
+        <v>469</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R3" s="2">
         <v>2</v>
@@ -4312,11 +4315,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4893,11 +4896,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12:N12"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5092,13 +5095,13 @@
         <v>114</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>9</v>
@@ -5177,13 +5180,13 @@
         <v>310</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>9</v>
@@ -5334,7 +5337,7 @@
         <v>3</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>379</v>
+        <v>468</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5477,10 +5480,10 @@
         <v>176</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
@@ -5707,7 +5710,7 @@
         <v>4</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>9</v>
@@ -5936,10 +5939,10 @@
         <v>58</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>12</v>
@@ -5960,10 +5963,10 @@
         <v>408</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="P30"/>
       <c r="Q30" s="6" t="s">
@@ -6008,10 +6011,10 @@
         <v>110</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>5</v>
@@ -6046,7 +6049,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>3</v>
@@ -6057,8 +6060,8 @@
       <c r="L32" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="O32" s="6" t="s">
-        <v>469</v>
+      <c r="N32" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>5</v>
@@ -6597,10 +6600,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>408</v>
@@ -7110,10 +7113,10 @@
         <v>3</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -8723,7 +8726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -8878,7 +8881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -8955,7 +8958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
New updated picklists and tableSchema, corrected version number to 1.2.2
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="6705" tabRatio="690" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="20730" windowHeight="6645" tabRatio="690" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="470">
   <si>
     <t>Type</t>
   </si>
@@ -1131,9 +1131,6 @@
     <t>RELATION{SummarizedInformation,type.code}$%anMethType.code</t>
   </si>
   <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{CasesInformation,statusHerd.code},$statusHerd=RELATION{CasesInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
-  </si>
-  <si>
     <t>Herd status</t>
   </si>
   <si>
@@ -1266,9 +1263,6 @@
     <t>RELATION{SummarizedInformation,progId.label}|IF((RELATION{SummarizedInformation,type.code}!=RGT),.%progIdSuffix.code,)</t>
   </si>
   <si>
-    <t>(RELATION{SummarizedInformation,prod.code}==F21.A07RV)</t>
-  </si>
-  <si>
     <t>reportLastMessageId</t>
   </si>
   <si>
@@ -1299,9 +1293,6 @@
     <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
   </si>
   <si>
-    <t>AND((RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
     <t>Sample/case assessment</t>
   </si>
   <si>
@@ -1380,9 +1371,6 @@
     <t>CWD extended context</t>
   </si>
   <si>
-    <t>Flag to include sex and PSU in aggregated data</t>
-  </si>
-  <si>
     <t>yesNoLists</t>
   </si>
   <si>
@@ -1428,16 +1416,25 @@
     <t>IF((%type.code==RGT),,AT06A)</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>(%type.code==CWD)</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),F,)</t>
+  </si>
+  <si>
+    <t>IF(%type.code==SCRAPIE,F,)</t>
+  </si>
+  <si>
+    <t>Flag to include sex and PSU in the context for aggregated data</t>
+  </si>
+  <si>
+    <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
   </si>
 </sst>
 </file>
@@ -3133,7 +3130,13 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S39" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S39"/>
+  <autoFilter ref="A1:S39">
+    <filterColumn colId="17">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:S39">
     <sortCondition ref="A1:A39"/>
   </sortState>
@@ -3163,8 +3166,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2512" displayName="Table2512" ref="A1:S23" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
-  <autoFilter ref="A1:S23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2512" displayName="Table2512" ref="A1:S22" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="A1:S22"/>
   <sortState ref="A2:S23">
     <sortCondition ref="R1:R23"/>
   </sortState>
@@ -3783,11 +3786,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3904,16 +3907,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>450</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>451</v>
+        <v>447</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>467</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>12</v>
@@ -3931,16 +3934,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -4432,7 +4435,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="8" t="s">
@@ -4537,7 +4540,7 @@
         <v>302</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4663,7 +4666,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>176</v>
@@ -4694,13 +4697,13 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>176</v>
@@ -4731,13 +4734,13 @@
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>176</v>
@@ -4776,7 +4779,7 @@
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
       <c r="E11" s="17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>176</v>
@@ -4815,7 +4818,7 @@
       <c r="C12" s="17"/>
       <c r="D12" s="18"/>
       <c r="E12" s="17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>176</v>
@@ -4846,15 +4849,15 @@
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>388</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>389</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>176</v>
@@ -4897,10 +4900,10 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A1:S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4984,7 +4987,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>79</v>
       </c>
@@ -5036,10 +5039,10 @@
         <v>75</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>3</v>
@@ -5071,10 +5074,10 @@
         <v>94</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>12</v>
@@ -5083,10 +5086,10 @@
         <v>95</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>3</v>
@@ -5095,13 +5098,13 @@
         <v>114</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>9</v>
@@ -5113,7 +5116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>89</v>
       </c>
@@ -5156,10 +5159,10 @@
         <v>91</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
@@ -5168,10 +5171,10 @@
         <v>92</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>3</v>
@@ -5180,13 +5183,13 @@
         <v>310</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>9</v>
@@ -5198,7 +5201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>352</v>
       </c>
@@ -5224,7 +5227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -5259,7 +5262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>81</v>
       </c>
@@ -5294,7 +5297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>179</v>
       </c>
@@ -5322,7 +5325,7 @@
         <v>58</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>70</v>
@@ -5372,7 +5375,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>176</v>
@@ -5405,7 +5408,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -5431,13 +5434,13 @@
         <v>4</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -5460,7 +5463,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>3</v>
@@ -5468,22 +5471,22 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>204</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>176</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
@@ -5498,7 +5501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -5533,7 +5536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>174</v>
       </c>
@@ -5553,7 +5556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
@@ -5588,7 +5591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>97</v>
       </c>
@@ -5620,7 +5623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>77</v>
       </c>
@@ -5652,7 +5655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>45</v>
       </c>
@@ -5687,7 +5690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>99</v>
       </c>
@@ -5710,13 +5713,13 @@
         <v>4</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>40</v>
       </c>
@@ -5748,7 +5751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
@@ -5783,7 +5786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>59</v>
       </c>
@@ -5809,13 +5812,13 @@
         <v>4</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="Q25" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>55</v>
       </c>
@@ -5850,7 +5853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>224</v>
       </c>
@@ -5870,13 +5873,13 @@
         <v>4</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>49</v>
       </c>
@@ -5911,7 +5914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>180</v>
       </c>
@@ -5933,22 +5936,22 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>3</v>
@@ -5960,13 +5963,13 @@
         <v>3</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="P30"/>
       <c r="Q30" s="6" t="s">
@@ -6002,7 +6005,7 @@
         <v>3</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>3</v>
@@ -6011,10 +6014,10 @@
         <v>110</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>5</v>
@@ -6034,7 +6037,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>37</v>
@@ -6046,10 +6049,10 @@
         <v>38</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>4</v>
+        <v>457</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>3</v>
@@ -6060,8 +6063,11 @@
       <c r="L32" s="6" t="s">
         <v>316</v>
       </c>
+      <c r="M32" s="6" t="s">
+        <v>465</v>
+      </c>
       <c r="N32" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>5</v>
@@ -6093,16 +6099,16 @@
         <v>8</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>5</v>
@@ -6122,7 +6128,7 @@
         <v>26</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>240</v>
@@ -6131,16 +6137,16 @@
         <v>8</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>5</v>
@@ -6172,16 +6178,16 @@
         <v>8</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>5</v>
@@ -6201,7 +6207,7 @@
         <v>21</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>240</v>
@@ -6248,16 +6254,16 @@
         <v>8</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Q37" s="6" t="s">
         <v>5</v>
@@ -6286,10 +6292,10 @@
         <v>19</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J38" s="6" t="s">
         <v>3</v>
@@ -6362,13 +6368,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5:J5"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6389,7 +6395,9 @@
     <col min="14" max="14" width="21.85546875" style="6" customWidth="1"/>
     <col min="15" max="16" width="22.85546875" style="6" customWidth="1"/>
     <col min="17" max="17" width="20" style="6" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="6"/>
+    <col min="18" max="18" width="9.140625" style="6"/>
+    <col min="19" max="19" width="10.140625" style="6" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -6453,13 +6461,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B2" t="s">
         <v>193</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>213</v>
@@ -6471,13 +6479,13 @@
         <v>326</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>214</v>
@@ -6562,10 +6570,10 @@
         <v>305</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>384</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>385</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>5</v>
@@ -6579,37 +6587,37 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>408</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>409</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -6638,19 +6646,19 @@
         <v>75</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>113</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>5</v>
@@ -6679,13 +6687,13 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>5</v>
@@ -6717,7 +6725,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -6771,77 +6779,69 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>277</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>369</v>
+        <v>278</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>37</v>
+        <v>279</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>38</v>
+        <v>176</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>305</v>
-      </c>
+      <c r="I10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="17"/>
       <c r="Q10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="R10" s="6">
-        <v>9</v>
-      </c>
-      <c r="S10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>204</v>
+        <v>275</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>8</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="17"/>
       <c r="H11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="17"/>
+      <c r="K11" s="6" t="s">
+        <v>306</v>
+      </c>
       <c r="Q11" s="6" t="s">
         <v>5</v>
       </c>
@@ -6851,23 +6851,25 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>275</v>
+        <v>216</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>288</v>
+        <v>217</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>219</v>
+      </c>
       <c r="H12" s="6" t="s">
-        <v>4</v>
+        <v>441</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -6876,7 +6878,10 @@
         <v>3</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>306</v>
+        <v>220</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -6887,37 +6892,40 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>216</v>
+        <v>196</v>
+      </c>
+      <c r="B13" t="s">
+        <v>193</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>3</v>
+        <v>439</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>380</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>221</v>
+        <v>305</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>443</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>5</v>
@@ -6928,41 +6936,37 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B14" t="s">
-        <v>193</v>
+        <v>210</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>199</v>
+        <v>43</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>442</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>446</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14"/>
+      <c r="P14"/>
       <c r="Q14" s="6" t="s">
         <v>5</v>
       </c>
@@ -6972,37 +6976,35 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>210</v>
+        <v>281</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>211</v>
+        <v>282</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="F15" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>43</v>
+      <c r="G15" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="I15" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="5" t="s">
         <v>3</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="O15"/>
-      <c r="P15"/>
+        <v>386</v>
+      </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
       </c>
@@ -7012,34 +7014,32 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>284</v>
-      </c>
+      <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="I16" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>387</v>
+      <c r="K16" s="17" t="s">
+        <v>161</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>5</v>
@@ -7050,32 +7050,37 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>286</v>
+        <v>373</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="F17" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="20"/>
+      <c r="G17" s="6" t="s">
+        <v>199</v>
+      </c>
       <c r="H17" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="I17" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K17" s="17" t="s">
-        <v>161</v>
+      <c r="K17" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>449</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7086,22 +7091,22 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>35</v>
+        <v>272</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>374</v>
+        <v>291</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>12</v>
+        <v>292</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>4</v>
@@ -7112,12 +7117,6 @@
       <c r="J18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="20" t="s">
-        <v>452</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>453</v>
-      </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
       </c>
@@ -7127,16 +7126,16 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>272</v>
+        <v>193</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>176</v>
@@ -7162,42 +7161,27 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="R20" s="6">
-        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>222</v>
+        <v>174</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>175</v>
@@ -7217,10 +7201,13 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>174</v>
+        <v>352</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>353</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>4</v>
@@ -7231,33 +7218,10 @@
       <c r="J22" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="O22" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="Q22" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q23" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7274,11 +7238,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7375,19 +7339,19 @@
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>325</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>5</v>
@@ -7413,19 +7377,19 @@
         <v>12</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>325</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -7466,7 +7430,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>296</v>
@@ -7501,7 +7465,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7521,7 +7485,7 @@
         <v>144</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
@@ -7635,19 +7599,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>438</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>439</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>441</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>176</v>
@@ -7714,7 +7678,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -7722,10 +7686,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>176</v>
@@ -7740,7 +7704,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -7798,7 +7762,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -7865,7 +7829,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>9</v>
@@ -7873,7 +7837,7 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>176</v>
@@ -7891,7 +7855,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7923,7 +7887,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>9</v>
@@ -7940,10 +7904,10 @@
         <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>176</v>
@@ -7961,7 +7925,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>9</v>
@@ -8062,7 +8026,7 @@
         <v>97</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>258</v>
@@ -8083,7 +8047,7 @@
         <v>3</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -8118,7 +8082,7 @@
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>9</v>
@@ -8307,7 +8271,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>9</v>
@@ -8336,7 +8300,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>368</v>
+        <v>469</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8382,13 +8346,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>176</v>
@@ -8403,7 +8367,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8467,7 +8431,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -8563,7 +8527,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -8571,13 +8535,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>176</v>
@@ -8592,7 +8556,7 @@
         <v>4</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8635,7 +8599,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>58</v>
@@ -8653,7 +8617,7 @@
         <v>4</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>5</v>
@@ -8699,7 +8663,7 @@
         <v>348</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>345</v>
@@ -9307,10 +9271,10 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -9366,7 +9330,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>350</v>

</xml_diff>

<commit_message>
- Force creation of new report at first lunch - New pages name - statusHerd taken from summInfo and removed from tableSchema for sample cases - New Beta tester toolbar +Accepted DWH button - Other small changes and bug fixes
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2565" windowWidth="20730" windowHeight="6585" tabRatio="690" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2685" windowWidth="20730" windowHeight="6465" tabRatio="690" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -1086,15 +1086,6 @@
     <t>Automatically FILLED, special field</t>
   </si>
   <si>
-    <t>AggregatedLevel</t>
-  </si>
-  <si>
-    <t>AnalyticalResult</t>
-  </si>
-  <si>
-    <t>CaseLevel</t>
-  </si>
-  <si>
     <t>IF((%internalOpType.label!=Test),RELATION{Report,reportSenderId.code}|-|today.timestamp,TEST_CONNECTION_|RELATION{Settings,username.code}|_version_{app.version})</t>
   </si>
   <si>
@@ -1413,12 +1404,6 @@
     <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
   </si>
   <si>
-    <t>IF((%type.code==SCRAPIE),F,)</t>
-  </si>
-  <si>
-    <t>IF(%type.code==SCRAPIE,F,)</t>
-  </si>
-  <si>
     <t>Flag to include sex and PSU in the context for aggregated data</t>
   </si>
   <si>
@@ -1432,6 +1417,21 @@
   </si>
   <si>
     <t>Husbandry system</t>
+  </si>
+  <si>
+    <t>Aggregated-Data-(Level-1)</t>
+  </si>
+  <si>
+    <t>Sample-Level-Data-(Level-2)</t>
+  </si>
+  <si>
+    <t>Analytical-Test-Results-(Level-3)</t>
+  </si>
+  <si>
+    <t>Report-Management</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
   </si>
 </sst>
 </file>
@@ -3905,16 +3905,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>12</v>
@@ -3932,16 +3932,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -3985,7 +3985,7 @@
         <v>113</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="R4" s="2">
         <v>3</v>
@@ -4023,7 +4023,7 @@
         <v>113</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="R5" s="2">
         <v>4</v>
@@ -4061,7 +4061,7 @@
         <v>113</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="R6" s="2">
         <v>5</v>
@@ -4099,7 +4099,7 @@
         <v>113</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="R7" s="2">
         <v>6</v>
@@ -4137,7 +4137,7 @@
         <v>113</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="R8" s="2">
         <v>7</v>
@@ -4175,7 +4175,7 @@
         <v>113</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="R9" s="2">
         <v>8</v>
@@ -4214,7 +4214,7 @@
         <v>113</v>
       </c>
       <c r="L10" s="30" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="R10" s="2">
         <v>9</v>
@@ -4253,7 +4253,7 @@
         <v>113</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="R11" s="2">
         <v>10</v>
@@ -4292,7 +4292,7 @@
         <v>113</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -4317,10 +4317,10 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4433,7 +4433,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="8" t="s">
@@ -4538,7 +4538,7 @@
         <v>301</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4664,7 +4664,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>175</v>
@@ -4695,13 +4695,13 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>175</v>
@@ -4732,13 +4732,13 @@
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>175</v>
@@ -4777,7 +4777,7 @@
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
       <c r="E11" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>175</v>
@@ -4816,7 +4816,7 @@
       <c r="C12" s="17"/>
       <c r="D12" s="18"/>
       <c r="E12" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>175</v>
@@ -4847,15 +4847,15 @@
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>175</v>
@@ -4897,11 +4897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5081,7 +5081,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>3</v>
@@ -5090,10 +5090,10 @@
         <v>109</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>5</v>
@@ -5145,7 +5145,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>69</v>
@@ -5160,7 +5160,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>3</v>
@@ -5320,10 +5320,10 @@
         <v>74</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5364,10 +5364,10 @@
         <v>18</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
@@ -5414,7 +5414,7 @@
         <v>4</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>9</v>
@@ -5443,7 +5443,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>3</v>
@@ -5451,22 +5451,22 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>3</v>
@@ -5478,13 +5478,13 @@
         <v>3</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="P15"/>
       <c r="Q15" s="6" t="s">
@@ -5709,7 +5709,7 @@
         <v>4</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>9</v>
@@ -5808,7 +5808,7 @@
         <v>4</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q25" s="6" t="s">
         <v>9</v>
@@ -5869,7 +5869,7 @@
         <v>4</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>9</v>
@@ -5941,10 +5941,10 @@
         <v>90</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>12</v>
@@ -5953,10 +5953,10 @@
         <v>91</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>3</v>
@@ -5965,13 +5965,13 @@
         <v>309</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>9</v>
@@ -5994,10 +5994,10 @@
         <v>93</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>12</v>
@@ -6006,10 +6006,10 @@
         <v>94</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>3</v>
@@ -6018,13 +6018,13 @@
         <v>113</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -6044,7 +6044,7 @@
         <v>34</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>36</v>
@@ -6056,10 +6056,10 @@
         <v>37</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>3</v>
@@ -6071,10 +6071,10 @@
         <v>315</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>463</v>
+        <v>468</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>468</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>5</v>
@@ -6088,22 +6088,22 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>203</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>175</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>3</v>
@@ -6129,7 +6129,7 @@
         <v>25</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>239</v>
@@ -6138,16 +6138,16 @@
         <v>8</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>5</v>
@@ -6179,16 +6179,16 @@
         <v>8</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>5</v>
@@ -6217,16 +6217,16 @@
         <v>8</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>5</v>
@@ -6246,7 +6246,7 @@
         <v>20</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>239</v>
@@ -6293,16 +6293,16 @@
         <v>8</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J38" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>5</v>
@@ -6322,7 +6322,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>175</v>
@@ -6369,10 +6369,10 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6459,13 +6459,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B2" t="s">
         <v>192</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>212</v>
@@ -6477,13 +6477,13 @@
         <v>325</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>213</v>
@@ -6568,10 +6568,10 @@
         <v>304</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>5</v>
@@ -6585,37 +6585,37 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>404</v>
-      </c>
       <c r="L5" s="6" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -6644,19 +6644,19 @@
         <v>74</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>112</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>5</v>
@@ -6685,13 +6685,13 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>5</v>
@@ -6723,7 +6723,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -6867,7 +6867,7 @@
         <v>218</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -6908,13 +6908,13 @@
         <v>198</v>
       </c>
       <c r="H13" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>439</v>
-      </c>
       <c r="J13" s="6" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>199</v>
@@ -6923,7 +6923,7 @@
         <v>304</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>5</v>
@@ -6952,7 +6952,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>3</v>
@@ -6992,7 +6992,7 @@
         <v>283</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>3</v>
@@ -7001,7 +7001,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>3</v>
@@ -7054,7 +7054,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>310</v>
@@ -7075,10 +7075,10 @@
         <v>3</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7236,11 +7236,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R9" sqref="R9"/>
+      <selection pane="bottomRight" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7337,19 +7337,19 @@
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>324</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>5</v>
@@ -7375,19 +7375,19 @@
         <v>12</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>324</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -7428,7 +7428,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>295</v>
@@ -7463,7 +7463,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7483,7 +7483,7 @@
         <v>143</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
@@ -7504,7 +7504,7 @@
         <v>113</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>9</v>
@@ -7597,19 +7597,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>432</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>435</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>175</v>
@@ -7673,7 +7673,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -7681,10 +7681,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>175</v>
@@ -7699,7 +7699,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -7757,7 +7757,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -7824,7 +7824,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>9</v>
@@ -7832,7 +7832,7 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>175</v>
@@ -7850,7 +7850,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7882,7 +7882,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>9</v>
@@ -7899,10 +7899,10 @@
         <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>175</v>
@@ -7920,7 +7920,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>9</v>
@@ -8021,7 +8021,7 @@
         <v>96</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>257</v>
@@ -8042,7 +8042,7 @@
         <v>3</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -8077,7 +8077,7 @@
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>9</v>
@@ -8266,7 +8266,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>9</v>
@@ -8295,7 +8295,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8341,13 +8341,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>175</v>
@@ -8362,7 +8362,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8426,7 +8426,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -8522,7 +8522,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -8530,13 +8530,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>175</v>
@@ -8551,7 +8551,7 @@
         <v>4</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8594,7 +8594,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>57</v>
@@ -8612,7 +8612,7 @@
         <v>4</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>5</v>
@@ -8658,7 +8658,7 @@
         <v>347</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>344</v>
@@ -8841,7 +8841,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8862,7 +8862,7 @@
         <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>353</v>
+        <v>464</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8870,7 +8870,7 @@
         <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8894,7 +8894,7 @@
         <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>355</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8902,7 +8902,7 @@
         <v>228</v>
       </c>
       <c r="B7" t="s">
-        <v>354</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -9101,7 +9101,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="6"/>
       <c r="P4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -9266,10 +9266,10 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="24" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -9325,7 +9325,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>349</v>

</xml_diff>

<commit_message>
* Fixed some business rules following the new variables added/removed * Test and align the correctness of the BR with the tool * Using the available functions for retrieving data to pass to sample level (statusHerd) * Consistency page's name of each level * Removed some business rules not used * First implementation of the import report from excel file (converting it in xml) available from next build •	Adding the clone function for each level with single connection to the database
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -3128,13 +3128,7 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S39" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S39">
-    <filterColumn colId="17">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S39"/>
   <sortState ref="A3:S39">
     <sortCondition ref="R1:R39"/>
   </sortState>
@@ -4898,7 +4892,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
@@ -4985,7 +4979,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>78</v>
       </c>
@@ -5105,7 +5099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>88</v>
       </c>
@@ -5184,7 +5178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>351</v>
       </c>
@@ -5210,7 +5204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>84</v>
       </c>
@@ -5245,7 +5239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>80</v>
       </c>
@@ -5280,7 +5274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>178</v>
       </c>
@@ -5388,7 +5382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -5420,7 +5414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -5497,7 +5491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>41</v>
       </c>
@@ -5532,7 +5526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>173</v>
       </c>
@@ -5552,7 +5546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>46</v>
       </c>
@@ -5587,7 +5581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>96</v>
       </c>
@@ -5619,7 +5613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>76</v>
       </c>
@@ -5651,7 +5645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
@@ -5686,7 +5680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>98</v>
       </c>
@@ -5715,7 +5709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>39</v>
       </c>
@@ -5747,7 +5741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>51</v>
       </c>
@@ -5782,7 +5776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>58</v>
       </c>
@@ -5814,7 +5808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
@@ -5849,7 +5843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>223</v>
       </c>
@@ -5875,7 +5869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
@@ -5910,7 +5904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>179</v>
       </c>
@@ -6369,10 +6363,10 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Double click for open report - Added reference to Preferences for SampleCases - Solved import of report with custom resId - finalised BETA funtions - origSampId null for RGT
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20070" windowHeight="3840" tabRatio="690" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20070" windowHeight="3840" tabRatio="690" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="475">
   <si>
     <t>Type</t>
   </si>
@@ -1290,12 +1290,6 @@
     <t>origSampId</t>
   </si>
   <si>
-    <t>origSampId=%origSampId.label</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,sampId.label}</t>
-  </si>
-  <si>
     <t>sampUnitType</t>
   </si>
   <si>
@@ -1356,12 +1350,6 @@
     <t>Sex of the animals</t>
   </si>
   <si>
-    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==Yes))</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F32.A0C9B,)</t>
-  </si>
-  <si>
     <t>BSE</t>
   </si>
   <si>
@@ -1377,12 +1365,6 @@
     <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
   </si>
   <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.label}==No)),F01.A056M,)</t>
-  </si>
-  <si>
-    <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.label},)</t>
-  </si>
-  <si>
     <t>IF((%type.code==RGT),,AT06A)</t>
   </si>
   <si>
@@ -1428,15 +1410,9 @@
     <t>%progId.label</t>
   </si>
   <si>
-    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{Preferences,cwdExtCont.code}==N))</t>
-  </si>
-  <si>
     <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),Not infected,)</t>
   </si>
   <si>
-    <t>origSampId=%sampId.label</t>
-  </si>
-  <si>
     <t>NEXT(,)</t>
   </si>
   <si>
@@ -1444,6 +1420,36 @@
   </si>
   <si>
     <t>Report Status</t>
+  </si>
+  <si>
+    <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.code},)</t>
+  </si>
+  <si>
+    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
+  </si>
+  <si>
+    <t>RELATION{Preferences,cwdExtCont.code}</t>
+  </si>
+  <si>
+    <t>OR((RELATION{SummarizedInformation,type.code}!=CWD),(RELATION{SummarizedInformation,cwdExtCont.code}==N))</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), RELATION{SummarizedInformation,sampId.label}, )</t>
+  </si>
+  <si>
+    <t>IF(%type.code!=RGT, origSampId=%sampId.label, )</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), origSampId=%origSampId.label, )</t>
+  </si>
+  <si>
+    <t>RELATION{Preferences,cwdExtCont.label}</t>
   </si>
 </sst>
 </file>
@@ -3139,10 +3145,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S40" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S40"/>
-  <sortState ref="A2:S40">
-    <sortCondition ref="B1:B40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S41" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:S41"/>
+  <sortState ref="A2:S41">
+    <sortCondition ref="A1:A41"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="79"/>
@@ -3791,10 +3797,10 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3911,16 +3917,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>438</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>12</v>
@@ -3938,16 +3944,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -4322,11 +4328,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4782,7 +4788,7 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>405</v>
@@ -4825,7 +4831,7 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>405</v>
@@ -4909,13 +4915,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5001,124 +5007,142 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>2</v>
+        <v>78</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>144</v>
+        <v>8</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>314</v>
+        <v>4</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>311</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" s="6">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>3</v>
+        <v>369</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>470</v>
+      <c r="K3" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R3" s="6">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
+        <v>93</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>417</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>175</v>
+        <v>12</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>442</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>397</v>
+        <v>443</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>443</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="R4" s="6">
+        <v>8</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>175</v>
@@ -5135,8 +5159,8 @@
       <c r="J5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>373</v>
+      <c r="N5" s="6" t="s">
+        <v>313</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>9</v>
@@ -5144,22 +5168,25 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>89</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>27</v>
+        <v>414</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>28</v>
+        <v>416</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>239</v>
+        <v>12</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>369</v>
@@ -5170,113 +5197,98 @@
       <c r="J6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>368</v>
+      <c r="K6" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>446</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R6" s="6">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>348</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>8</v>
+        <v>349</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>368</v>
+        <v>4</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="R7" s="6">
-        <v>11</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="G8" s="17" t="s">
+        <v>434</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>368</v>
+        <v>4</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>474</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="R8" s="6">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>366</v>
+        <v>83</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>239</v>
+        <v>175</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>4</v>
@@ -5285,128 +5297,115 @@
         <v>4</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>312</v>
+        <v>4</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R9" s="6">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
+        <v>79</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>239</v>
+        <v>175</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>368</v>
+        <v>82</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R10" s="6">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="J11" s="6" t="s">
+      <c r="G12" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R11" s="6">
-        <v>5</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>411</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="6" t="s">
-        <v>443</v>
-      </c>
       <c r="I12" s="6" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="K12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="S12" s="6" t="s">
         <v>9</v>
@@ -5414,102 +5413,87 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>175</v>
       </c>
+      <c r="G13" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="H13" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>449</v>
+        <v>3</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>462</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="R13" s="6">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>458</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>37</v>
+        <v>14</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>448</v>
+        <v>4</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>448</v>
+        <v>4</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>464</v>
+        <v>4</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>468</v>
+        <v>373</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R14" s="6">
-        <v>9</v>
-      </c>
-      <c r="S14" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="H15" s="6" t="s">
         <v>4</v>
       </c>
@@ -5519,57 +5503,55 @@
       <c r="J15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="6" t="s">
+      <c r="M15" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="Q15" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="I16" s="6" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>297</v>
+        <v>3</v>
       </c>
       <c r="Q16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R16" s="6">
+        <v>10</v>
+      </c>
+      <c r="S16" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>175</v>
@@ -5598,19 +5580,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>4</v>
@@ -5621,25 +5594,19 @@
       <c r="J18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N18" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>298</v>
-      </c>
       <c r="Q18" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>239</v>
@@ -5668,16 +5635,16 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>239</v>
+        <v>175</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>8</v>
@@ -5691,11 +5658,8 @@
       <c r="J20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="6" t="s">
-        <v>296</v>
-      </c>
       <c r="P20" s="6" t="s">
-        <v>299</v>
+        <v>459</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>9</v>
@@ -5703,17 +5667,20 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>418</v>
+        <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>419</v>
+        <v>75</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>418</v>
+        <v>76</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>175</v>
       </c>
+      <c r="G21" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="H21" s="6" t="s">
         <v>4</v>
       </c>
@@ -5723,8 +5690,8 @@
       <c r="J21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="6" t="s">
-        <v>469</v>
+      <c r="P21" s="6" t="s">
+        <v>460</v>
       </c>
       <c r="Q21" s="6" t="s">
         <v>9</v>
@@ -5732,19 +5699,19 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>175</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>4</v>
@@ -5755,11 +5722,11 @@
       <c r="J22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>56</v>
+      <c r="N22" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>9</v>
@@ -5767,111 +5734,78 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>73</v>
+        <v>34</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>314</v>
+        <v>4</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>445</v>
       </c>
       <c r="Q23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R23" s="6">
-        <v>4</v>
-      </c>
-      <c r="S23" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>459</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>69</v>
+        <v>38</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>315</v>
+        <v>4</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>460</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R24" s="6">
-        <v>3</v>
-      </c>
-      <c r="S24" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>58</v>
+        <v>418</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>57</v>
+        <v>419</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>58</v>
+        <v>418</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="H25" s="6" t="s">
         <v>4</v>
       </c>
@@ -5881,8 +5815,8 @@
       <c r="J25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P25" s="6" t="s">
-        <v>409</v>
+      <c r="N25" s="6" t="s">
+        <v>472</v>
       </c>
       <c r="Q25" s="6" t="s">
         <v>9</v>
@@ -5890,114 +5824,86 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>393</v>
+        <v>51</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>442</v>
+        <v>50</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>12</v>
+        <v>239</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>395</v>
+        <v>8</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="P26"/>
+        <v>4</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>299</v>
+      </c>
       <c r="Q26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R26" s="6">
-        <v>6</v>
-      </c>
-      <c r="S26" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>62</v>
+      <c r="C27" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>450</v>
+        <v>4</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>409</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R27" s="6">
-        <v>2</v>
-      </c>
-      <c r="S27" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>175</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>4</v>
@@ -6008,8 +5914,11 @@
       <c r="J28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P28" s="6" t="s">
-        <v>466</v>
+      <c r="M28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>9</v>
@@ -6017,19 +5926,13 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>77</v>
+        <v>223</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>78</v>
+        <v>223</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>4</v>
@@ -6041,7 +5944,7 @@
         <v>4</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>311</v>
+        <v>410</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>9</v>
@@ -6049,19 +5952,19 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>4</v>
@@ -6072,11 +5975,11 @@
       <c r="J30" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M30" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>82</v>
+      <c r="N30" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>9</v>
@@ -6084,19 +5987,10 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>4</v>
@@ -6107,72 +6001,79 @@
       <c r="J31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M31" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="Q31" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>88</v>
+        <v>393</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>440</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>8</v>
+        <v>395</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>313</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="P32"/>
       <c r="Q32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R32" s="6">
+        <v>6</v>
+      </c>
+      <c r="S32" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>414</v>
+        <v>61</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>416</v>
+        <v>62</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>369</v>
+        <v>3</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>369</v>
@@ -6181,22 +6082,19 @@
         <v>3</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>309</v>
+        <v>109</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>445</v>
+        <v>465</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>452</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="Q33" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R33" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="S33" s="6" t="s">
         <v>9</v>
@@ -6204,52 +6102,52 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>415</v>
+        <v>452</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="F34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>94</v>
+      <c r="G34" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>369</v>
+        <v>444</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>369</v>
+        <v>444</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K34" s="6" t="s">
-        <v>113</v>
+      <c r="K34" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>446</v>
+        <v>314</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>447</v>
+        <v>458</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>461</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R34" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S34" s="6" t="s">
         <v>9</v>
@@ -6257,88 +6155,139 @@
     </row>
     <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>96</v>
+        <v>14</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>465</v>
+        <v>3</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="Q35" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R35" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>348</v>
+        <v>24</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>175</v>
+        <v>365</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>4</v>
+        <v>368</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>5</v>
+      </c>
+      <c r="R36" s="6">
+        <v>11</v>
+      </c>
+      <c r="S36" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>174</v>
+        <v>21</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="Q37" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="R37" s="6">
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>173</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>366</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>174</v>
+        <v>239</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>4</v>
@@ -6347,56 +6296,139 @@
         <v>4</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="Q38" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="R38" s="6">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>223</v>
+        <v>29</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>175</v>
+        <v>239</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P39" s="6" t="s">
-        <v>410</v>
+        <v>3</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="Q39" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="R39" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>174</v>
+        <v>16</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="Q40" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="R40" s="6">
+        <v>5</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R41" s="6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6412,11 +6444,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A22"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6503,7 +6535,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B2" t="s">
         <v>192</v>
@@ -6650,10 +6682,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>398</v>
@@ -6729,7 +6761,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
@@ -6767,7 +6799,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -6911,7 +6943,7 @@
         <v>218</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -6952,10 +6984,10 @@
         <v>198</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>371</v>
@@ -6967,7 +6999,7 @@
         <v>304</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>5</v>
@@ -6996,7 +7028,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>3</v>
@@ -7036,7 +7068,7 @@
         <v>283</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>3</v>
@@ -7072,7 +7104,7 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>3</v>
@@ -7119,10 +7151,10 @@
         <v>3</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7281,10 +7313,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomRight" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7641,19 +7673,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>427</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>175</v>
@@ -7668,6 +7700,9 @@
         <v>4</v>
       </c>
       <c r="O9" s="6">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
         <v>1</v>
       </c>
       <c r="Q9" s="6" t="s">
@@ -7717,7 +7752,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -7743,7 +7778,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>422</v>
+        <v>471</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -8339,7 +8374,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8406,7 +8441,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>421</v>
+        <v>473</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8574,13 +8609,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>175</v>
@@ -8595,7 +8630,7 @@
         <v>4</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8730,13 +8765,13 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8906,7 +8941,7 @@
         <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8914,7 +8949,7 @@
         <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8938,7 +8973,7 @@
         <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8946,7 +8981,7 @@
         <v>228</v>
       </c>
       <c r="B7" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* solved portSeq not incrementing when adding same record on Analytical result level (required from GDR101) * solved proxyConfig which now is taken from the external config folder
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="7545" tabRatio="690" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="7545" tabRatio="690" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -6950,7 +6950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7821,11 +7821,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M28" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8211,9 +8211,7 @@
       <c r="O9" s="6">
         <v>1</v>
       </c>
-      <c r="P9" s="6">
-        <v>1</v>
-      </c>
+      <c r="P9" s="35"/>
       <c r="Q9" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>